<commit_message>
Update of the game ER diagram
</commit_message>
<xml_diff>
--- a/Technical documentation/AL table analysis.xlsx
+++ b/Technical documentation/AL table analysis.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martema\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martema\Documents\GitHub\AtariLegend\Technical documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -203,7 +203,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="112">
   <si>
     <t>Table name</t>
   </si>
@@ -313,9 +313,6 @@
     <t>game_music</t>
   </si>
   <si>
-    <t>The cross table between the game and the music structure</t>
-  </si>
-  <si>
     <t>game_developer</t>
   </si>
   <si>
@@ -355,15 +352,9 @@
     <t>The language table - this one is derived from the 'lingo' table</t>
   </si>
   <si>
-    <t>release_individual</t>
-  </si>
-  <si>
     <t>This is the cross table between the release and its creators/individuals. This table also contains the link to the author_type table (programmer, graphics artist, Musician ...)</t>
   </si>
   <si>
-    <t>emulator_incompatibility_release</t>
-  </si>
-  <si>
     <t>This is the cross table between the release table, emulator table and the incompatibility table</t>
   </si>
   <si>
@@ -382,9 +373,6 @@
     <t>to do</t>
   </si>
   <si>
-    <t>release_system_enhanced</t>
-  </si>
-  <si>
     <t>Crosstable between the release, the system and the enhancement tables</t>
   </si>
   <si>
@@ -397,15 +385,9 @@
     <t>This table holds all the enhancements in the games we encounter</t>
   </si>
   <si>
-    <t>release_system_compatibility</t>
-  </si>
-  <si>
     <t>Crosstable between the release, the system and the incompatibility tables</t>
   </si>
   <si>
-    <t>release_resolution</t>
-  </si>
-  <si>
     <t>Crosstable between the release and the resolution table</t>
   </si>
   <si>
@@ -433,9 +415,6 @@
     <t>replaced by game_genre_cross</t>
   </si>
   <si>
-    <t>release_location</t>
-  </si>
-  <si>
     <t>Crosstable between the release and the location table</t>
   </si>
   <si>
@@ -445,9 +424,6 @@
     <t>Table holding countries (UK, France, US, ...) + regions (Europe, Asia, ...)</t>
   </si>
   <si>
-    <t>release_memory_enhanced</t>
-  </si>
-  <si>
     <t>Crosstable between the release, the memory and the enhancement tables</t>
   </si>
   <si>
@@ -457,9 +433,6 @@
     <t>Table holding the RAM amounts (512, 1024, 2048, 4096)</t>
   </si>
   <si>
-    <t>tos_version_incompatibility_release</t>
-  </si>
-  <si>
     <t>Crosstable between the release, the tos version and the incompatibility tables</t>
   </si>
   <si>
@@ -521,6 +494,51 @@
   </si>
   <si>
     <t>game_unreleased</t>
+  </si>
+  <si>
+    <t>game_release_distributor</t>
+  </si>
+  <si>
+    <t>Crosstable between the distributor and the game_release table</t>
+  </si>
+  <si>
+    <t>game_release_individual</t>
+  </si>
+  <si>
+    <t>game_release_emulator_incompatibility</t>
+  </si>
+  <si>
+    <t>game_release_system_enhanced</t>
+  </si>
+  <si>
+    <t>game_release_system_compatibility</t>
+  </si>
+  <si>
+    <t>game_release_resolution</t>
+  </si>
+  <si>
+    <t>game_release_location</t>
+  </si>
+  <si>
+    <t>game_release_memory_enhanced</t>
+  </si>
+  <si>
+    <t>game_release_music</t>
+  </si>
+  <si>
+    <t>The cross table between the game_release and the music structure</t>
+  </si>
+  <si>
+    <t>Cross between game and music - replaced by game_release_music</t>
+  </si>
+  <si>
+    <t>game_release_tos_version_incompatibility</t>
+  </si>
+  <si>
+    <t>game_release_tos_region_incompatibility</t>
+  </si>
+  <si>
+    <t>Crosstable between the release, the tos version, location and the incompatibility tables</t>
   </si>
 </sst>
 </file>
@@ -1115,14 +1133,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L52"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="78.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="40.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80.28515625" style="3" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" style="17" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" style="18" customWidth="1"/>
     <col min="5" max="5" width="58.85546875" style="18" customWidth="1"/>
@@ -1229,7 +1249,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="49" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C5" s="48" t="s">
         <v>7</v>
@@ -1249,7 +1269,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="26"/>
       <c r="D6" s="25"/>
@@ -1267,7 +1287,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C7" s="48" t="s">
         <v>7</v>
@@ -1287,7 +1307,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="26"/>
       <c r="D8" s="25"/>
@@ -1305,7 +1325,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="47" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C9" s="48" t="s">
         <v>7</v>
@@ -1325,7 +1345,7 @@
         <v>24</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="26"/>
       <c r="D10" s="25"/>
@@ -1423,25 +1443,31 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="H16" s="36" t="s">
-        <v>12</v>
+      <c r="B16" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="12"/>
+      <c r="H16" s="46" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>7</v>
@@ -1452,10 +1478,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="43" t="s">
         <v>39</v>
-      </c>
-      <c r="B18" s="43" t="s">
-        <v>40</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="10"/>
@@ -1470,10 +1496,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19" s="45" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>7</v>
@@ -1490,10 +1516,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="43" t="s">
         <v>42</v>
-      </c>
-      <c r="B20" s="43" t="s">
-        <v>43</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="10"/>
@@ -1508,10 +1534,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B21" s="45" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>7</v>
@@ -1528,10 +1554,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="43" t="s">
         <v>48</v>
-      </c>
-      <c r="B22" s="43" t="s">
-        <v>49</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="10"/>
@@ -1546,10 +1572,10 @@
     </row>
     <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="43" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="B23" s="37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="10"/>
@@ -1562,12 +1588,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="43" t="s">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="B24" s="43" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="10"/>
@@ -1580,12 +1606,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="43" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B25" s="43" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="10"/>
@@ -1600,10 +1626,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="43" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B26" s="43" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="10"/>
@@ -1613,15 +1639,15 @@
         <v>7</v>
       </c>
       <c r="H26" s="51" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="43" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="B27" s="43" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="10"/>
@@ -1636,10 +1662,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="43" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B28" s="43" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="10"/>
@@ -1654,10 +1680,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="43" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B29" s="43" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="10"/>
@@ -1667,15 +1693,15 @@
         <v>7</v>
       </c>
       <c r="H29" s="51" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="43" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="B30" s="43" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="10"/>
@@ -1690,10 +1716,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="43" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="B31" s="43" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="10"/>
@@ -1708,10 +1734,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="43" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B32" s="43" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="10"/>
@@ -1726,10 +1752,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="43" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="B33" s="43" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="10"/>
@@ -1744,10 +1770,10 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="43" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B34" s="43" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C34" s="9"/>
       <c r="D34" s="10"/>
@@ -1762,10 +1788,10 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="43" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="B35" s="43" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C35" s="9"/>
       <c r="D35" s="10"/>
@@ -1780,10 +1806,10 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="43" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B36" s="43" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="10"/>
@@ -1796,12 +1822,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="43" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="B37" s="43" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C37" s="9"/>
       <c r="D37" s="10"/>
@@ -1814,81 +1840,81 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="G38" s="13"/>
-      <c r="H38" s="36" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B39" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="45" t="s">
-        <v>90</v>
-      </c>
-      <c r="B40" s="45" t="s">
-        <v>91</v>
-      </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G40" s="12"/>
-      <c r="H40" s="12" t="s">
-        <v>13</v>
+    <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="B38" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="H38" s="28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="B39" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="C39" s="9"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="H39" s="28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="B40" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" s="9"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="H40" s="28" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="45" t="s">
-        <v>92</v>
-      </c>
-      <c r="B41" s="45" t="s">
-        <v>93</v>
-      </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12" t="s">
-        <v>13</v>
+      <c r="A41" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" s="13"/>
+      <c r="H41" s="36" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="45" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="B42" s="45" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="C42" s="6"/>
       <c r="D42" s="7"/>
@@ -1903,10 +1929,10 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="45" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="B43" s="45" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="7"/>
@@ -1921,10 +1947,10 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="45" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="B44" s="45" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C44" s="6"/>
       <c r="D44" s="7"/>
@@ -1939,10 +1965,10 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="45" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="B45" s="45" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C45" s="6"/>
       <c r="D45" s="7"/>
@@ -1957,10 +1983,10 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="45" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="B46" s="45" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C46" s="6"/>
       <c r="D46" s="7"/>
@@ -1975,10 +2001,10 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="45" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B47" s="45" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C47" s="6"/>
       <c r="D47" s="7"/>
@@ -1993,10 +2019,10 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="45" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="B48" s="45" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C48" s="6"/>
       <c r="D48" s="7"/>
@@ -2011,10 +2037,10 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="45" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="B49" s="45" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C49" s="6"/>
       <c r="D49" s="7"/>
@@ -2029,10 +2055,10 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="45" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B50" s="45" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C50" s="6"/>
       <c r="D50" s="7"/>
@@ -2047,10 +2073,10 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="45" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="B51" s="45" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C51" s="6"/>
       <c r="D51" s="7"/>
@@ -2065,10 +2091,10 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="45" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="B52" s="45" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C52" s="6"/>
       <c r="D52" s="7"/>
@@ -2078,6 +2104,60 @@
       </c>
       <c r="G52" s="12"/>
       <c r="H52" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="B53" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="C53" s="6"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G53" s="12"/>
+      <c r="H53" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="B54" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="C54" s="6"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="B55" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="C55" s="6"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
I've updated the game and dump ER diagram
</commit_message>
<xml_diff>
--- a/Technical documentation/AL table analysis.xlsx
+++ b/Technical documentation/AL table analysis.xlsx
@@ -203,7 +203,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="146">
   <si>
     <t>Table name</t>
   </si>
@@ -575,6 +575,72 @@
   </si>
   <si>
     <t>From which system is this game ported (C64, Amiga, Arcade)</t>
+  </si>
+  <si>
+    <t>media</t>
+  </si>
+  <si>
+    <t>This table contains the media of a release.  A release can have multiple media, for example games spread across multiple disks, or games with SS and DS disks. A media has a type like Floppy SS, Floppy DS, Cartridge, Digital...</t>
+  </si>
+  <si>
+    <t>dumps.mwb</t>
+  </si>
+  <si>
+    <t>media_scan</t>
+  </si>
+  <si>
+    <t>This table contains the artwork of the game. A media can have multiple scan images (e.g. front of the floppy, back, goodies...)</t>
+  </si>
+  <si>
+    <t>dump</t>
+  </si>
+  <si>
+    <t>Table containing the actual dump/download of a media. A media can have multiple dumps, for example a Pasti one and a MSA one .</t>
+  </si>
+  <si>
+    <t>game_release_trainer_options</t>
+  </si>
+  <si>
+    <t>Cross between release table and trainer options - this one replaces the game_download_trainer table</t>
+  </si>
+  <si>
+    <t>game_download_trainer</t>
+  </si>
+  <si>
+    <t>replaced by game_release_trainer_options</t>
+  </si>
+  <si>
+    <t>downloads_game.mwb</t>
+  </si>
+  <si>
+    <t>trainer_options</t>
+  </si>
+  <si>
+    <t>table containing all types of trainers</t>
+  </si>
+  <si>
+    <t>game_release_cracktro</t>
+  </si>
+  <si>
+    <t>Cross table between the release and the cracktro table - this table replaces the game_download_intro table</t>
+  </si>
+  <si>
+    <t>game_download_intro</t>
+  </si>
+  <si>
+    <t>This table is replaced by the game_release_cracktro table</t>
+  </si>
+  <si>
+    <t>dump_info</t>
+  </si>
+  <si>
+    <t>Contains extra info about the dump. Its size, who downloaded it, how many times it is downloaded...This table replaces game_download_info</t>
+  </si>
+  <si>
+    <t>game_download_info</t>
+  </si>
+  <si>
+    <t>This table is replaced by the dump_info table</t>
   </si>
 </sst>
 </file>
@@ -1169,10 +1235,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L61"/>
+  <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46:H46"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1184,7 +1250,7 @@
     <col min="5" max="5" width="58.85546875" style="18" customWidth="1"/>
     <col min="6" max="6" width="7" style="19" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="5"/>
-    <col min="8" max="8" width="16.42578125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2303,6 +2369,182 @@
       <c r="G61" s="12"/>
       <c r="H61" s="12" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A62" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="B62" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="C62" s="9"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="11"/>
+      <c r="G62" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="H62" s="44" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="B63" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="C63" s="9"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="H63" s="44" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="B64" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="C64" s="9"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="H64" s="44" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="B65" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="C65" s="9"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="H65" s="28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="45" t="s">
+        <v>133</v>
+      </c>
+      <c r="B66" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="C66" s="6"/>
+      <c r="D66" s="7"/>
+      <c r="E66" s="7"/>
+      <c r="F66" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G66" s="12"/>
+      <c r="H66" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C67" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H67" s="36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="43" t="s">
+        <v>138</v>
+      </c>
+      <c r="B68" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="C68" s="9"/>
+      <c r="D68" s="10"/>
+      <c r="E68" s="10"/>
+      <c r="F68" s="11"/>
+      <c r="G68" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="H68" s="28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="B69" s="45" t="s">
+        <v>141</v>
+      </c>
+      <c r="C69" s="6"/>
+      <c r="D69" s="7"/>
+      <c r="E69" s="7"/>
+      <c r="F69" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G69" s="12"/>
+      <c r="H69" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="43" t="s">
+        <v>142</v>
+      </c>
+      <c r="B70" s="43" t="s">
+        <v>143</v>
+      </c>
+      <c r="C70" s="9"/>
+      <c r="D70" s="10"/>
+      <c r="E70" s="10"/>
+      <c r="F70" s="11"/>
+      <c r="G70" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="H70" s="44" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="45" t="s">
+        <v>144</v>
+      </c>
+      <c r="B71" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="C71" s="6"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G71" s="12"/>
+      <c r="H71" s="12" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on analysis excel file
</commit_message>
<xml_diff>
--- a/Technical documentation/AL table analysis.xlsx
+++ b/Technical documentation/AL table analysis.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Table overview" sheetId="1" r:id="rId1"/>
+    <sheet name="Game structure" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -202,8 +203,43 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Martens Maarten</author>
+  </authors>
+  <commentList>
+    <comment ref="C53" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Martens Maarten:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Extra info on some of the fields of the table
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="169">
   <si>
     <t>Table name</t>
   </si>
@@ -641,6 +677,75 @@
   </si>
   <si>
     <t>This table is replaced by the dump_info table</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">game </t>
+  </si>
+  <si>
+    <t>Fields</t>
+  </si>
+  <si>
+    <t>A game is a port from a single origin system (The system the game appeared on first)</t>
+  </si>
+  <si>
+    <t>Explanation</t>
+  </si>
+  <si>
+    <t>Extra</t>
+  </si>
+  <si>
+    <t>Is the game a port (from an Arcade or another system)</t>
+  </si>
+  <si>
+    <t>port_id</t>
+  </si>
+  <si>
+    <t>game_series_id</t>
+  </si>
+  <si>
+    <t>A game is part of a single series</t>
+  </si>
+  <si>
+    <t>eg. Turrican, Ultima, ...</t>
+  </si>
+  <si>
+    <t>This is the main game table which everything will be connected with</t>
+  </si>
+  <si>
+    <t>The table which holds all programming languages. Eg C, STOS, ASM, GFA...A game can be a mix of STOS + ASM</t>
+  </si>
+  <si>
+    <t>Port</t>
+  </si>
+  <si>
+    <t>This is the cross table between the game and its creators/individuals. This table also contains the link to the author_type table (programmer, graphics artist, Musician ...)</t>
+  </si>
+  <si>
+    <t>What engine was the game built with eg. STOS, STAC, SEUCK ... A game can only be build with 1 engine</t>
+  </si>
+  <si>
+    <t>game_similar_cross</t>
+  </si>
+  <si>
+    <t>contains a game_id</t>
+  </si>
+  <si>
+    <t>This is the cross table between the game and its genre, A game can be part of multiple genres,</t>
+  </si>
+  <si>
+    <t>The table which holds all the genres eg. Action, platformer, adventure</t>
+  </si>
+  <si>
+    <t>nr_of_players</t>
+  </si>
+  <si>
+    <t>How many players can play the game together</t>
+  </si>
+  <si>
+    <t>A game has a single count of maximum players</t>
   </si>
 </sst>
 </file>
@@ -683,7 +788,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -708,8 +813,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -798,11 +915,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -953,6 +1090,24 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -970,6 +1125,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2438399</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>71078</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="13477874" cy="9596078"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1237,9 +1441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1251,6 +1453,7 @@
     <col min="6" max="6" width="7" style="19" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="5"/>
     <col min="8" max="8" width="23.85546875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="2.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2552,4 +2755,235 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A53:E69"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="77.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="B53" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="53" t="s">
+        <v>148</v>
+      </c>
+      <c r="D53" s="53" t="s">
+        <v>150</v>
+      </c>
+      <c r="E53" s="53" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="58" t="s">
+        <v>147</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C54" s="58" t="s">
+        <v>153</v>
+      </c>
+      <c r="D54" t="s">
+        <v>152</v>
+      </c>
+      <c r="E54" s="58" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="58"/>
+      <c r="C55" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="D55" t="s">
+        <v>167</v>
+      </c>
+      <c r="E55" s="58" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="59"/>
+      <c r="B56" s="55"/>
+      <c r="C56" s="59" t="s">
+        <v>154</v>
+      </c>
+      <c r="D56" s="52" t="s">
+        <v>155</v>
+      </c>
+      <c r="E56" s="59" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="60" t="s">
+        <v>15</v>
+      </c>
+      <c r="B57" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="C57" s="60"/>
+      <c r="D57" s="56"/>
+      <c r="E57" s="60"/>
+    </row>
+    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="B58" s="57" t="s">
+        <v>158</v>
+      </c>
+      <c r="C58" s="60"/>
+      <c r="D58" s="56"/>
+      <c r="E58" s="60"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="60" t="s">
+        <v>159</v>
+      </c>
+      <c r="B59" s="57" t="s">
+        <v>123</v>
+      </c>
+      <c r="C59" s="60"/>
+      <c r="D59" s="56"/>
+      <c r="E59" s="60"/>
+    </row>
+    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="B60" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="C60" s="60"/>
+      <c r="D60" s="56"/>
+      <c r="E60" s="60"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="61" t="s">
+        <v>118</v>
+      </c>
+      <c r="B61" s="57" t="s">
+        <v>119</v>
+      </c>
+      <c r="C61" s="61"/>
+      <c r="D61" s="57"/>
+      <c r="E61" s="61"/>
+    </row>
+    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="61" t="s">
+        <v>120</v>
+      </c>
+      <c r="B62" s="57" t="s">
+        <v>161</v>
+      </c>
+      <c r="C62" s="61"/>
+      <c r="D62" s="57"/>
+      <c r="E62" s="61"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="B63" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="C63" s="61"/>
+      <c r="D63" s="57"/>
+      <c r="E63" s="61"/>
+    </row>
+    <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="B64" s="57" t="s">
+        <v>32</v>
+      </c>
+      <c r="C64" s="61"/>
+      <c r="D64" s="57"/>
+      <c r="E64" s="61"/>
+    </row>
+    <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="B65" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="C65" s="61"/>
+      <c r="D65" s="57"/>
+      <c r="E65" s="61"/>
+    </row>
+    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="61" t="s">
+        <v>27</v>
+      </c>
+      <c r="B66" s="57" t="s">
+        <v>28</v>
+      </c>
+      <c r="C66" s="61" t="s">
+        <v>162</v>
+      </c>
+      <c r="D66" s="57" t="s">
+        <v>163</v>
+      </c>
+      <c r="E66" s="61"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="61" t="s">
+        <v>25</v>
+      </c>
+      <c r="B67" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="C67" s="61"/>
+      <c r="D67" s="57"/>
+      <c r="E67" s="61"/>
+    </row>
+    <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="B68" s="57" t="s">
+        <v>164</v>
+      </c>
+      <c r="C68" s="61"/>
+      <c r="D68" s="57"/>
+      <c r="E68" s="61"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="B69" s="57" t="s">
+        <v>165</v>
+      </c>
+      <c r="C69" s="61"/>
+      <c r="D69" s="57"/>
+      <c r="E69" s="61"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
More technical analysis updates
</commit_message>
<xml_diff>
--- a/Technical documentation/AL table analysis.xlsx
+++ b/Technical documentation/AL table analysis.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Table overview" sheetId="1" r:id="rId1"/>
     <sheet name="Game structure" sheetId="2" r:id="rId2"/>
+    <sheet name="Dump Structure" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -238,8 +239,43 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Martens Maarten</author>
+  </authors>
+  <commentList>
+    <comment ref="C38" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Martens Maarten:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Extra info on some of the fields of the table
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="218">
   <si>
     <t>Table name</t>
   </si>
@@ -364,9 +400,6 @@
     <t>lingo_game</t>
   </si>
   <si>
-    <t>release_language</t>
-  </si>
-  <si>
     <t xml:space="preserve"> the cross table between a release and the language table</t>
   </si>
   <si>
@@ -670,9 +703,6 @@
     <t>dump_info</t>
   </si>
   <si>
-    <t>Contains extra info about the dump. Its size, who downloaded it, how many times it is downloaded...This table replaces game_download_info</t>
-  </si>
-  <si>
     <t>game_download_info</t>
   </si>
   <si>
@@ -718,9 +748,6 @@
     <t>The table which holds all programming languages. Eg C, STOS, ASM, GFA...A game can be a mix of STOS + ASM</t>
   </si>
   <si>
-    <t>Port</t>
-  </si>
-  <si>
     <t>This is the cross table between the game and its creators/individuals. This table also contains the link to the author_type table (programmer, graphics artist, Musician ...)</t>
   </si>
   <si>
@@ -860,6 +887,50 @@
   </si>
   <si>
     <t>The cross table between the disk_protection table and the game release table. What disk protection system is used?</t>
+  </si>
+  <si>
+    <t>The cross table between a release and the language table</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Field to add  bugs and other info regarding the release</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>A media has a type like Floppy SS, Floppy DS, Cartridge, Digital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- A release can have multiple media, for example games spread across multiple disks, or games with SS and DS disks
+- A media can have multiple scan images (e.g. front of the floppy, back)
+- A media can have multiple dumps, for example a STX (Pasti), MSA (Magic Shadow Archiver) , RAW (Kryoflux), SCP (SuperCard Pro) </t>
+  </si>
+  <si>
+    <t>imgext</t>
+  </si>
+  <si>
+    <t>Front of the floppy, back, goodies...</t>
+  </si>
+  <si>
+    <t>Extension of the image</t>
+  </si>
+  <si>
+    <t>format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STX (Pasti), MSA (Magic Shadow Archiver) , RAW (Kryoflux), SCP (SuperCard Pro) </t>
+  </si>
+  <si>
+    <t>extra info regarding the dump, bugs ...</t>
+  </si>
+  <si>
+    <t>dump_user_info</t>
+  </si>
+  <si>
+    <t>Extra info regarding who downloaded the dump and when</t>
   </si>
 </sst>
 </file>
@@ -1053,7 +1124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1243,6 +1314,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1272,13 +1373,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1714499</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>179585</xdr:rowOff>
+      <xdr:colOff>1078491</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="4" name="Picture 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1298,7 +1399,56 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="13630274" cy="9704585"/>
+          <a:ext cx="13699116" cy="9753600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>885825</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7467600" cy="6886575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1575,8 +1725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1690,7 +1840,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="48" t="s">
         <v>7</v>
@@ -1710,7 +1860,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="26"/>
       <c r="D6" s="25"/>
@@ -1728,7 +1878,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" s="48" t="s">
         <v>7</v>
@@ -1748,7 +1898,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="26"/>
       <c r="D8" s="25"/>
@@ -1766,7 +1916,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="47" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" s="48" t="s">
         <v>7</v>
@@ -1786,7 +1936,7 @@
         <v>24</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="26"/>
       <c r="D10" s="25"/>
@@ -1888,7 +2038,7 @@
         <v>35</v>
       </c>
       <c r="B16" s="45" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>7</v>
@@ -1940,7 +2090,7 @@
         <v>40</v>
       </c>
       <c r="B19" s="45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>7</v>
@@ -1957,10 +2107,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="43" t="s">
+        <v>185</v>
+      </c>
+      <c r="B20" s="43" t="s">
         <v>41</v>
-      </c>
-      <c r="B20" s="43" t="s">
-        <v>42</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="10"/>
@@ -1975,10 +2125,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B21" s="45" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>7</v>
@@ -1995,10 +2145,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="43" t="s">
         <v>47</v>
-      </c>
-      <c r="B22" s="43" t="s">
-        <v>48</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="10"/>
@@ -2013,10 +2163,10 @@
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B23" s="37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="10"/>
@@ -2031,10 +2181,10 @@
     </row>
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B24" s="43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="10"/>
@@ -2049,10 +2199,10 @@
     </row>
     <row r="25" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="43" t="s">
         <v>51</v>
-      </c>
-      <c r="B25" s="43" t="s">
-        <v>52</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="10"/>
@@ -2067,10 +2217,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="43" t="s">
         <v>53</v>
-      </c>
-      <c r="B26" s="43" t="s">
-        <v>54</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="10"/>
@@ -2080,15 +2230,15 @@
         <v>7</v>
       </c>
       <c r="H26" s="51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B27" s="43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="10"/>
@@ -2103,10 +2253,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="43" t="s">
         <v>57</v>
-      </c>
-      <c r="B28" s="43" t="s">
-        <v>58</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="10"/>
@@ -2121,10 +2271,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" s="43" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="10"/>
@@ -2134,15 +2284,15 @@
         <v>7</v>
       </c>
       <c r="H29" s="51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B30" s="43" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="10"/>
@@ -2157,10 +2307,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B31" s="43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="10"/>
@@ -2175,10 +2325,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="43" t="s">
         <v>62</v>
-      </c>
-      <c r="B32" s="43" t="s">
-        <v>63</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="10"/>
@@ -2193,10 +2343,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="43" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B33" s="43" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="10"/>
@@ -2211,10 +2361,10 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" s="43" t="s">
         <v>71</v>
-      </c>
-      <c r="B34" s="43" t="s">
-        <v>72</v>
       </c>
       <c r="C34" s="9"/>
       <c r="D34" s="10"/>
@@ -2229,10 +2379,10 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B35" s="43" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C35" s="9"/>
       <c r="D35" s="10"/>
@@ -2247,10 +2397,10 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="43" t="s">
         <v>74</v>
-      </c>
-      <c r="B36" s="43" t="s">
-        <v>75</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="10"/>
@@ -2265,10 +2415,10 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="43" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B37" s="43" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C37" s="9"/>
       <c r="D37" s="10"/>
@@ -2283,10 +2433,10 @@
     </row>
     <row r="38" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="B38" s="43" t="s">
         <v>97</v>
-      </c>
-      <c r="B38" s="43" t="s">
-        <v>98</v>
       </c>
       <c r="C38" s="9"/>
       <c r="D38" s="10"/>
@@ -2301,10 +2451,10 @@
     </row>
     <row r="39" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="B39" s="43" t="s">
         <v>106</v>
-      </c>
-      <c r="B39" s="43" t="s">
-        <v>107</v>
       </c>
       <c r="C39" s="9"/>
       <c r="D39" s="10"/>
@@ -2319,10 +2469,10 @@
     </row>
     <row r="40" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="B40" s="43" t="s">
         <v>112</v>
-      </c>
-      <c r="B40" s="43" t="s">
-        <v>113</v>
       </c>
       <c r="C40" s="9"/>
       <c r="D40" s="10"/>
@@ -2337,10 +2487,10 @@
     </row>
     <row r="41" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="B41" s="43" t="s">
         <v>110</v>
-      </c>
-      <c r="B41" s="43" t="s">
-        <v>111</v>
       </c>
       <c r="C41" s="9"/>
       <c r="D41" s="10"/>
@@ -2355,10 +2505,10 @@
     </row>
     <row r="42" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="B42" s="43" t="s">
         <v>116</v>
-      </c>
-      <c r="B42" s="43" t="s">
-        <v>117</v>
       </c>
       <c r="C42" s="9"/>
       <c r="D42" s="10"/>
@@ -2373,10 +2523,10 @@
     </row>
     <row r="43" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="43" t="s">
+        <v>113</v>
+      </c>
+      <c r="B43" s="43" t="s">
         <v>114</v>
-      </c>
-      <c r="B43" s="43" t="s">
-        <v>115</v>
       </c>
       <c r="C43" s="9"/>
       <c r="D43" s="10"/>
@@ -2391,10 +2541,10 @@
     </row>
     <row r="44" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="B44" s="43" t="s">
         <v>118</v>
-      </c>
-      <c r="B44" s="43" t="s">
-        <v>119</v>
       </c>
       <c r="C44" s="9"/>
       <c r="D44" s="10"/>
@@ -2409,10 +2559,10 @@
     </row>
     <row r="45" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="B45" s="43" t="s">
         <v>120</v>
-      </c>
-      <c r="B45" s="43" t="s">
-        <v>121</v>
       </c>
       <c r="C45" s="9"/>
       <c r="D45" s="10"/>
@@ -2427,10 +2577,10 @@
     </row>
     <row r="46" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="B46" s="43" t="s">
         <v>122</v>
-      </c>
-      <c r="B46" s="43" t="s">
-        <v>123</v>
       </c>
       <c r="C46" s="9"/>
       <c r="D46" s="10"/>
@@ -2445,10 +2595,10 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="C47" s="17" t="s">
         <v>7</v>
@@ -2460,10 +2610,10 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="B48" s="45" t="s">
         <v>79</v>
-      </c>
-      <c r="B48" s="45" t="s">
-        <v>80</v>
       </c>
       <c r="C48" s="6"/>
       <c r="D48" s="7"/>
@@ -2478,10 +2628,10 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49" s="45" t="s">
         <v>81</v>
-      </c>
-      <c r="B49" s="45" t="s">
-        <v>82</v>
       </c>
       <c r="C49" s="6"/>
       <c r="D49" s="7"/>
@@ -2496,10 +2646,10 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="B50" s="45" t="s">
         <v>83</v>
-      </c>
-      <c r="B50" s="45" t="s">
-        <v>84</v>
       </c>
       <c r="C50" s="6"/>
       <c r="D50" s="7"/>
@@ -2514,10 +2664,10 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="B51" s="45" t="s">
         <v>85</v>
-      </c>
-      <c r="B51" s="45" t="s">
-        <v>86</v>
       </c>
       <c r="C51" s="6"/>
       <c r="D51" s="7"/>
@@ -2532,10 +2682,10 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B52" s="45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C52" s="6"/>
       <c r="D52" s="7"/>
@@ -2550,10 +2700,10 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B53" s="45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C53" s="6"/>
       <c r="D53" s="7"/>
@@ -2568,10 +2718,10 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B54" s="45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C54" s="6"/>
       <c r="D54" s="7"/>
@@ -2586,10 +2736,10 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="45" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B55" s="45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C55" s="6"/>
       <c r="D55" s="7"/>
@@ -2604,10 +2754,10 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B56" s="45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C56" s="6"/>
       <c r="D56" s="7"/>
@@ -2622,10 +2772,10 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="45" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B57" s="45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C57" s="6"/>
       <c r="D57" s="7"/>
@@ -2640,10 +2790,10 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="45" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B58" s="45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C58" s="6"/>
       <c r="D58" s="7"/>
@@ -2658,10 +2808,10 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B59" s="45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C59" s="6"/>
       <c r="D59" s="7"/>
@@ -2676,10 +2826,10 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B60" s="45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C60" s="6"/>
       <c r="D60" s="7"/>
@@ -2694,10 +2844,10 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B61" s="45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C61" s="6"/>
       <c r="D61" s="7"/>
@@ -2712,10 +2862,10 @@
     </row>
     <row r="62" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="B62" s="43" t="s">
         <v>124</v>
-      </c>
-      <c r="B62" s="43" t="s">
-        <v>125</v>
       </c>
       <c r="C62" s="9"/>
       <c r="D62" s="10"/>
@@ -2725,15 +2875,15 @@
         <v>7</v>
       </c>
       <c r="H62" s="44" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="43" t="s">
+        <v>126</v>
+      </c>
+      <c r="B63" s="43" t="s">
         <v>127</v>
-      </c>
-      <c r="B63" s="43" t="s">
-        <v>128</v>
       </c>
       <c r="C63" s="9"/>
       <c r="D63" s="10"/>
@@ -2743,15 +2893,15 @@
         <v>7</v>
       </c>
       <c r="H63" s="44" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="B64" s="43" t="s">
         <v>129</v>
-      </c>
-      <c r="B64" s="43" t="s">
-        <v>130</v>
       </c>
       <c r="C64" s="9"/>
       <c r="D64" s="10"/>
@@ -2761,15 +2911,15 @@
         <v>7</v>
       </c>
       <c r="H64" s="44" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="B65" s="43" t="s">
         <v>131</v>
-      </c>
-      <c r="B65" s="43" t="s">
-        <v>132</v>
       </c>
       <c r="C65" s="9"/>
       <c r="D65" s="10"/>
@@ -2784,10 +2934,10 @@
     </row>
     <row r="66" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="B66" s="45" t="s">
         <v>133</v>
-      </c>
-      <c r="B66" s="45" t="s">
-        <v>134</v>
       </c>
       <c r="C66" s="6"/>
       <c r="D66" s="7"/>
@@ -2797,15 +2947,15 @@
       </c>
       <c r="G66" s="12"/>
       <c r="H66" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B67" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>137</v>
       </c>
       <c r="C67" s="17" t="s">
         <v>7</v>
@@ -2816,10 +2966,10 @@
     </row>
     <row r="68" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="43" t="s">
+        <v>137</v>
+      </c>
+      <c r="B68" s="43" t="s">
         <v>138</v>
-      </c>
-      <c r="B68" s="43" t="s">
-        <v>139</v>
       </c>
       <c r="C68" s="9"/>
       <c r="D68" s="10"/>
@@ -2834,10 +2984,10 @@
     </row>
     <row r="69" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="B69" s="45" t="s">
         <v>140</v>
-      </c>
-      <c r="B69" s="45" t="s">
-        <v>141</v>
       </c>
       <c r="C69" s="6"/>
       <c r="D69" s="7"/>
@@ -2847,15 +2997,15 @@
       </c>
       <c r="G69" s="12"/>
       <c r="H69" s="12" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="43" t="s">
-        <v>142</v>
-      </c>
-      <c r="B70" s="43" t="s">
-        <v>143</v>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="76" t="s">
+        <v>216</v>
+      </c>
+      <c r="B70" s="77" t="s">
+        <v>217</v>
       </c>
       <c r="C70" s="9"/>
       <c r="D70" s="10"/>
@@ -2865,15 +3015,15 @@
         <v>7</v>
       </c>
       <c r="H70" s="44" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="45" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B71" s="45" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C71" s="6"/>
       <c r="D71" s="7"/>
@@ -2883,7 +3033,7 @@
       </c>
       <c r="G71" s="12"/>
       <c r="H71" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2895,78 +3045,78 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A53:E102"/>
+  <dimension ref="A53:E104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A54" sqref="A54:E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" style="67" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.5703125" style="67" customWidth="1"/>
     <col min="2" max="2" width="69.7109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="60.42578125" style="3" customWidth="1"/>
     <col min="5" max="5" width="77.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="63" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B53" s="53" t="s">
         <v>1</v>
       </c>
       <c r="C53" s="52" t="s">
+        <v>146</v>
+      </c>
+      <c r="D53" s="53" t="s">
         <v>148</v>
       </c>
-      <c r="D53" s="53" t="s">
-        <v>150</v>
-      </c>
       <c r="E53" s="52" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="64" t="s">
+        <v>145</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C54" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E54" s="56" t="s">
         <v>147</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C54" s="56" t="s">
-        <v>153</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="E54" s="56" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="64"/>
       <c r="C55" s="56" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E55" s="56" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="65"/>
       <c r="B56" s="54"/>
       <c r="C56" s="57" t="s">
+        <v>152</v>
+      </c>
+      <c r="D56" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="E56" s="57" t="s">
         <v>154</v>
-      </c>
-      <c r="D56" s="54" t="s">
-        <v>155</v>
-      </c>
-      <c r="E56" s="57" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2985,7 +3135,7 @@
         <v>17</v>
       </c>
       <c r="B58" s="55" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C58" s="58"/>
       <c r="D58" s="55"/>
@@ -2993,10 +3143,10 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="66" t="s">
-        <v>159</v>
+        <v>121</v>
       </c>
       <c r="B59" s="55" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C59" s="58"/>
       <c r="D59" s="55"/>
@@ -3007,7 +3157,7 @@
         <v>24</v>
       </c>
       <c r="B60" s="55" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C60" s="58"/>
       <c r="D60" s="55"/>
@@ -3015,10 +3165,10 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="66" t="s">
+        <v>117</v>
+      </c>
+      <c r="B61" s="55" t="s">
         <v>118</v>
-      </c>
-      <c r="B61" s="55" t="s">
-        <v>119</v>
       </c>
       <c r="C61" s="59"/>
       <c r="D61" s="55"/>
@@ -3026,10 +3176,10 @@
     </row>
     <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="66" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B62" s="55" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C62" s="59"/>
       <c r="D62" s="55"/>
@@ -3076,10 +3226,10 @@
         <v>28</v>
       </c>
       <c r="C66" s="59" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D66" s="55" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E66" s="59"/>
     </row>
@@ -3099,7 +3249,7 @@
         <v>20</v>
       </c>
       <c r="B68" s="55" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C68" s="59"/>
       <c r="D68" s="55"/>
@@ -3110,7 +3260,7 @@
         <v>22</v>
       </c>
       <c r="B69" s="55" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C69" s="59"/>
       <c r="D69" s="55"/>
@@ -3124,305 +3274,304 @@
         <v>39</v>
       </c>
       <c r="C70" s="60" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E70" s="56" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="64"/>
       <c r="C71" s="56" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E71" s="56" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="64"/>
       <c r="C72" s="56" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E72" s="56" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="64"/>
       <c r="C73" s="56" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E73" s="56" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="64"/>
       <c r="C74" s="56" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E74" s="56" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="64"/>
       <c r="C75" s="56" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E75" s="56" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="65"/>
-      <c r="B76" s="54"/>
-      <c r="C76" s="57" t="s">
-        <v>173</v>
-      </c>
-      <c r="D76" s="54" t="s">
+      <c r="A76" s="64"/>
+      <c r="C76" s="56" t="s">
+        <v>205</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E76" s="56"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="65"/>
+      <c r="B77" s="54"/>
+      <c r="C77" s="57" t="s">
+        <v>170</v>
+      </c>
+      <c r="D77" s="54" t="s">
+        <v>182</v>
+      </c>
+      <c r="E77" s="57"/>
+    </row>
+    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="65" t="s">
         <v>185</v>
       </c>
-      <c r="E76" s="57"/>
-    </row>
-    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="65" t="s">
+      <c r="B78" s="54" t="s">
+        <v>193</v>
+      </c>
+      <c r="C78" s="57"/>
+      <c r="D78" s="54"/>
+      <c r="E78" s="57"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="64" t="s">
+        <v>46</v>
+      </c>
+      <c r="B79" s="61" t="s">
+        <v>186</v>
+      </c>
+      <c r="C79" s="62" t="s">
+        <v>46</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E79" s="56"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="65"/>
+      <c r="B80" s="54"/>
+      <c r="C80" s="57" t="s">
         <v>188</v>
       </c>
-      <c r="B77" s="54" t="s">
-        <v>196</v>
-      </c>
-      <c r="C77" s="57"/>
-      <c r="D77" s="54"/>
-      <c r="E77" s="57"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="64" t="s">
-        <v>47</v>
-      </c>
-      <c r="B78" s="61" t="s">
+      <c r="D80" s="54" t="s">
         <v>189</v>
       </c>
-      <c r="C78" s="62" t="s">
-        <v>47</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="E78" s="56"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="65"/>
-      <c r="B79" s="54"/>
-      <c r="C79" s="57" t="s">
-        <v>191</v>
-      </c>
-      <c r="D79" s="54" t="s">
+      <c r="E80" s="57"/>
+    </row>
+    <row r="81" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A81" s="65" t="s">
+        <v>96</v>
+      </c>
+      <c r="B81" s="54" t="s">
         <v>192</v>
-      </c>
-      <c r="E79" s="57"/>
-    </row>
-    <row r="80" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A80" s="65" t="s">
-        <v>97</v>
-      </c>
-      <c r="B80" s="54" t="s">
-        <v>195</v>
-      </c>
-      <c r="C80" s="57"/>
-      <c r="D80" s="54"/>
-      <c r="E80" s="57"/>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="65" t="s">
-        <v>138</v>
-      </c>
-      <c r="B81" s="54" t="s">
-        <v>193</v>
       </c>
       <c r="C81" s="57"/>
       <c r="D81" s="54"/>
       <c r="E81" s="57"/>
     </row>
-    <row r="82" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="65" t="s">
-        <v>99</v>
+        <v>137</v>
       </c>
       <c r="B82" s="54" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C82" s="57"/>
       <c r="D82" s="54"/>
       <c r="E82" s="57"/>
     </row>
-    <row r="83" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A83" s="65" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B83" s="54" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="C83" s="57"/>
       <c r="D83" s="54"/>
       <c r="E83" s="57"/>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" s="65" t="s">
-        <v>51</v>
+        <v>99</v>
       </c>
       <c r="B84" s="54" t="s">
-        <v>52</v>
+        <v>194</v>
       </c>
       <c r="C84" s="57"/>
       <c r="D84" s="54"/>
       <c r="E84" s="57"/>
     </row>
-    <row r="85" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="65" t="s">
-        <v>131</v>
+        <v>50</v>
       </c>
       <c r="B85" s="54" t="s">
-        <v>132</v>
+        <v>51</v>
       </c>
       <c r="C85" s="57"/>
       <c r="D85" s="54"/>
       <c r="E85" s="57"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="65" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B86" s="54" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C86" s="57"/>
       <c r="D86" s="54"/>
       <c r="E86" s="57"/>
     </row>
-    <row r="87" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="65" t="s">
-        <v>101</v>
+        <v>135</v>
       </c>
       <c r="B87" s="54" t="s">
-        <v>198</v>
+        <v>136</v>
       </c>
       <c r="C87" s="57"/>
       <c r="D87" s="54"/>
       <c r="E87" s="57"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="65" t="s">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="B88" s="54" t="s">
-        <v>58</v>
+        <v>195</v>
       </c>
       <c r="C88" s="57"/>
       <c r="D88" s="54"/>
       <c r="E88" s="57"/>
     </row>
-    <row r="89" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="65" t="s">
-        <v>102</v>
+        <v>56</v>
       </c>
       <c r="B89" s="54" t="s">
-        <v>199</v>
+        <v>57</v>
       </c>
       <c r="C89" s="57"/>
       <c r="D89" s="54"/>
       <c r="E89" s="57"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" s="65" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B90" s="54" t="s">
-        <v>107</v>
+        <v>196</v>
       </c>
       <c r="C90" s="57"/>
       <c r="D90" s="54"/>
       <c r="E90" s="57"/>
     </row>
-    <row r="91" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="65" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B91" s="54" t="s">
-        <v>200</v>
+        <v>106</v>
       </c>
       <c r="C91" s="57"/>
       <c r="D91" s="54"/>
       <c r="E91" s="57"/>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="65" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="B92" s="54" t="s">
-        <v>63</v>
+        <v>197</v>
       </c>
       <c r="C92" s="57"/>
       <c r="D92" s="54"/>
       <c r="E92" s="57"/>
     </row>
-    <row r="93" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="65" t="s">
-        <v>104</v>
+        <v>61</v>
       </c>
       <c r="B93" s="54" t="s">
-        <v>201</v>
+        <v>62</v>
       </c>
       <c r="C93" s="57"/>
       <c r="D93" s="54"/>
       <c r="E93" s="57"/>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" s="65" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="B94" s="54" t="s">
-        <v>72</v>
+        <v>198</v>
       </c>
       <c r="C94" s="57"/>
       <c r="D94" s="54"/>
       <c r="E94" s="57"/>
     </row>
-    <row r="95" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="65" t="s">
-        <v>105</v>
+        <v>70</v>
       </c>
       <c r="B95" s="54" t="s">
-        <v>202</v>
+        <v>71</v>
       </c>
       <c r="C95" s="57"/>
       <c r="D95" s="54"/>
       <c r="E95" s="57"/>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="65" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="B96" s="54" t="s">
-        <v>75</v>
+        <v>199</v>
       </c>
       <c r="C96" s="57"/>
       <c r="D96" s="54"/>
@@ -3430,21 +3579,21 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="65" t="s">
-        <v>112</v>
+        <v>73</v>
       </c>
       <c r="B97" s="54" t="s">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="C97" s="57"/>
       <c r="D97" s="54"/>
       <c r="E97" s="57"/>
     </row>
-    <row r="98" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="65" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B98" s="54" t="s">
-        <v>203</v>
+        <v>112</v>
       </c>
       <c r="C98" s="57"/>
       <c r="D98" s="54"/>
@@ -3455,44 +3604,186 @@
         <v>109</v>
       </c>
       <c r="B99" s="54" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C99" s="57"/>
       <c r="D99" s="54"/>
       <c r="E99" s="57"/>
     </row>
-    <row r="100" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A100" s="65" t="s">
-        <v>77</v>
+        <v>108</v>
       </c>
       <c r="B100" s="54" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C100" s="57"/>
       <c r="D100" s="54"/>
       <c r="E100" s="57"/>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="65" t="s">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="B101" s="54" t="s">
-        <v>117</v>
+        <v>202</v>
       </c>
       <c r="C101" s="57"/>
       <c r="D101" s="54"/>
       <c r="E101" s="57"/>
     </row>
-    <row r="102" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="65" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B102" s="54" t="s">
-        <v>206</v>
+        <v>116</v>
       </c>
       <c r="C102" s="57"/>
       <c r="D102" s="54"/>
       <c r="E102" s="57"/>
+    </row>
+    <row r="103" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A103" s="65" t="s">
+        <v>113</v>
+      </c>
+      <c r="B103" s="54" t="s">
+        <v>203</v>
+      </c>
+      <c r="C103" s="57"/>
+      <c r="D103" s="54"/>
+      <c r="E103" s="57"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="65" t="s">
+        <v>185</v>
+      </c>
+      <c r="B104" s="54" t="s">
+        <v>204</v>
+      </c>
+      <c r="C104" s="57"/>
+      <c r="D104" s="54"/>
+      <c r="E104" s="57"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A38:E44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:B44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.42578125" style="70" customWidth="1"/>
+    <col min="2" max="2" width="68.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" style="70" customWidth="1"/>
+    <col min="4" max="4" width="73.85546875" style="70" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="75.5703125" style="67" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="63" t="s">
+        <v>144</v>
+      </c>
+      <c r="B38" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="71" t="s">
+        <v>146</v>
+      </c>
+      <c r="D38" s="63" t="s">
+        <v>148</v>
+      </c>
+      <c r="E38" s="63" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A39" s="66" t="s">
+        <v>123</v>
+      </c>
+      <c r="B39" s="75" t="s">
+        <v>209</v>
+      </c>
+      <c r="C39" s="72" t="s">
+        <v>207</v>
+      </c>
+      <c r="D39" s="73" t="s">
+        <v>208</v>
+      </c>
+      <c r="E39" s="72"/>
+    </row>
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="68" t="s">
+        <v>126</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C40" s="68" t="s">
+        <v>207</v>
+      </c>
+      <c r="D40" s="70" t="s">
+        <v>211</v>
+      </c>
+      <c r="E40" s="64"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="69"/>
+      <c r="B41" s="54"/>
+      <c r="C41" s="69" t="s">
+        <v>210</v>
+      </c>
+      <c r="D41" s="74" t="s">
+        <v>212</v>
+      </c>
+      <c r="E41" s="65"/>
+    </row>
+    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="68" t="s">
+        <v>128</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C42" s="68" t="s">
+        <v>213</v>
+      </c>
+      <c r="D42" s="70" t="s">
+        <v>214</v>
+      </c>
+      <c r="E42" s="64"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="69"/>
+      <c r="B43" s="54"/>
+      <c r="C43" s="69" t="s">
+        <v>141</v>
+      </c>
+      <c r="D43" s="74" t="s">
+        <v>215</v>
+      </c>
+      <c r="E43" s="65"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="69" t="s">
+        <v>216</v>
+      </c>
+      <c r="B44" s="54" t="s">
+        <v>217</v>
+      </c>
+      <c r="C44" s="69"/>
+      <c r="D44" s="74"/>
+      <c r="E44" s="65"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Creating new tables and deleting old ones
STOS, STAC and SEUCK have been merged into game_programming_language
</commit_message>
<xml_diff>
--- a/Technical documentation/AL table analysis.xlsx
+++ b/Technical documentation/AL table analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Table overview" sheetId="1" r:id="rId1"/>
@@ -1143,7 +1143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1811" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1821" uniqueCount="588">
   <si>
     <t>Table name</t>
   </si>
@@ -2895,6 +2895,21 @@
   </si>
   <si>
     <t>Deleted using script nr 162</t>
+  </si>
+  <si>
+    <t>Created using DB script nr 176</t>
+  </si>
+  <si>
+    <t>Created using DB script nr 177</t>
+  </si>
+  <si>
+    <t>Deleted using script nr 180</t>
+  </si>
+  <si>
+    <t>Deleted using script nr 181</t>
+  </si>
+  <si>
+    <t>Deleted using script nr 182</t>
   </si>
 </sst>
 </file>
@@ -4129,6 +4144,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFC2E49C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFDB69"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5757"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="0"/>
         </patternFill>
       </fill>
@@ -4157,6 +4193,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFC2E49C"/>
         </patternFill>
       </fill>
@@ -4185,6 +4228,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFC2E49C"/>
         </patternFill>
       </fill>
@@ -4200,41 +4250,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF5757"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC2E49C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDB69"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5757"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6861,7 +6876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F304"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12208,18 +12223,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="containsText" dxfId="7" priority="2" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="115" priority="2" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="114" priority="3" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="113" priority="4" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="112" priority="1" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C24)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12241,8 +12256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P221"/>
   <sheetViews>
-    <sheetView topLeftCell="A192" workbookViewId="0">
-      <selection activeCell="D143" sqref="D143"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="52.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13289,8 +13304,12 @@
       <c r="B96" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C96" s="69"/>
-      <c r="D96" s="69"/>
+      <c r="C96" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D96" s="69" t="s">
+        <v>584</v>
+      </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="35" t="s">
@@ -13512,8 +13531,12 @@
       <c r="B116" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C116" s="69"/>
-      <c r="D116" s="69"/>
+      <c r="C116" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D116" s="69" t="s">
+        <v>587</v>
+      </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="35" t="s">
@@ -13532,8 +13555,12 @@
       <c r="B118" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C118" s="69"/>
-      <c r="D118" s="69"/>
+      <c r="C118" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D118" s="69" t="s">
+        <v>586</v>
+      </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="35" t="s">
@@ -13570,8 +13597,12 @@
       <c r="B121" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C121" s="69"/>
-      <c r="D121" s="69"/>
+      <c r="C121" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D121" s="69" t="s">
+        <v>585</v>
+      </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="35" t="s">
@@ -14210,8 +14241,12 @@
       <c r="B183" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C183" s="69"/>
-      <c r="D183" s="69"/>
+      <c r="C183" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D183" s="69" t="s">
+        <v>583</v>
+      </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="35" t="s">
@@ -14610,434 +14645,434 @@
     <mergeCell ref="A1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="B95">
-    <cfRule type="containsText" dxfId="115" priority="294" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="111" priority="294" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B95)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="295" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="110" priority="295" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B95)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="113" priority="296" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="109" priority="296" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B95)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B95">
-    <cfRule type="containsText" dxfId="112" priority="293" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="108" priority="293" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B95)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B13 B15:B39 B42:B44 B54:B60 B76:B90 B62:B73">
-    <cfRule type="containsText" dxfId="111" priority="310" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="107" priority="310" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="110" priority="311" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="106" priority="311" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="312" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="105" priority="312" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B13 B15:B39 B42:B44 B54:B60 B76:B90 B62:B73">
-    <cfRule type="containsText" dxfId="108" priority="309" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="104" priority="309" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B92">
-    <cfRule type="containsText" dxfId="107" priority="306" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="103" priority="306" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B92)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="307" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="102" priority="307" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B92)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="308" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="101" priority="308" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B92)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B92">
-    <cfRule type="containsText" dxfId="104" priority="305" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="100" priority="305" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B92)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B94">
-    <cfRule type="containsText" dxfId="103" priority="297" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="99" priority="297" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B94)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B93">
-    <cfRule type="containsText" dxfId="102" priority="302" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="98" priority="302" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="101" priority="303" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="97" priority="303" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="304" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="96" priority="304" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B93)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B93">
-    <cfRule type="containsText" dxfId="99" priority="301" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="95" priority="301" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B93)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B94">
-    <cfRule type="containsText" dxfId="98" priority="298" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="94" priority="298" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B94)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="299" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="93" priority="299" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B94)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="300" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="92" priority="300" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B94)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B207">
-    <cfRule type="containsText" dxfId="95" priority="281" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="91" priority="281" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B207)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B207">
-    <cfRule type="containsText" dxfId="94" priority="282" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="90" priority="282" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B207)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="283" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="89" priority="283" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B207)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="284" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="88" priority="284" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B207)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B208">
-    <cfRule type="containsText" dxfId="91" priority="278" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="87" priority="278" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B208)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="279" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="86" priority="279" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B208)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="280" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="85" priority="280" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B208)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B208">
-    <cfRule type="containsText" dxfId="88" priority="277" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="84" priority="277" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B208)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B209">
-    <cfRule type="containsText" dxfId="87" priority="274" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="83" priority="274" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B209)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="275" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="82" priority="275" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B209)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="276" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="81" priority="276" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B209)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B209">
-    <cfRule type="containsText" dxfId="84" priority="273" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="80" priority="273" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B209)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B210">
-    <cfRule type="containsText" dxfId="83" priority="270" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="79" priority="270" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B210)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="271" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="78" priority="271" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B210)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="272" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="77" priority="272" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B210)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B210">
-    <cfRule type="containsText" dxfId="80" priority="269" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="76" priority="269" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B210)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B211">
-    <cfRule type="containsText" dxfId="79" priority="266" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="75" priority="266" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B211)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="267" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="74" priority="267" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B211)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="268" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="73" priority="268" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B211)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B211">
-    <cfRule type="containsText" dxfId="76" priority="265" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="72" priority="265" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B211)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B213">
-    <cfRule type="containsText" dxfId="75" priority="178" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="71" priority="178" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B213)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="179" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="70" priority="179" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B213)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="180" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="69" priority="180" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B213)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B213">
-    <cfRule type="containsText" dxfId="72" priority="177" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="68" priority="177" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B213)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45:B46">
-    <cfRule type="containsText" dxfId="71" priority="170" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="67" priority="170" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="171" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="66" priority="171" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="172" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="65" priority="172" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45:B46">
-    <cfRule type="containsText" dxfId="68" priority="169" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="64" priority="169" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75">
-    <cfRule type="containsText" dxfId="67" priority="158" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="63" priority="158" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="159" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="62" priority="159" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="160" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="61" priority="160" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75">
-    <cfRule type="containsText" dxfId="64" priority="157" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="60" priority="157" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B74">
-    <cfRule type="containsText" dxfId="63" priority="162" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="59" priority="162" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B74)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="163" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="58" priority="163" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B74)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="164" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="57" priority="164" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B74">
-    <cfRule type="containsText" dxfId="60" priority="161" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="56" priority="161" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51:B53">
-    <cfRule type="containsText" dxfId="59" priority="166" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="55" priority="166" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="167" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="54" priority="167" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="168" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="53" priority="168" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51:B53">
-    <cfRule type="containsText" dxfId="56" priority="165" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="52" priority="165" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="containsText" dxfId="55" priority="150" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="51" priority="150" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="151" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="50" priority="151" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="152" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="49" priority="152" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="containsText" dxfId="52" priority="149" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="48" priority="149" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="containsText" dxfId="51" priority="146" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="47" priority="146" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="147" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="46" priority="147" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="148" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="45" priority="148" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="containsText" dxfId="48" priority="145" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="44" priority="145" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48:B49">
-    <cfRule type="containsText" dxfId="47" priority="142" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="43" priority="142" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="143" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="42" priority="143" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="144" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="41" priority="144" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48:B49">
-    <cfRule type="containsText" dxfId="44" priority="141" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="40" priority="141" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="containsText" dxfId="43" priority="138" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="39" priority="138" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="139" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="38" priority="139" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="140" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="37" priority="140" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="containsText" dxfId="40" priority="137" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="36" priority="137" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41">
-    <cfRule type="containsText" dxfId="39" priority="134" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="35" priority="134" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="135" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="34" priority="135" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="136" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="33" priority="136" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41">
-    <cfRule type="containsText" dxfId="36" priority="133" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="32" priority="133" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50">
-    <cfRule type="containsText" dxfId="35" priority="130" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="31" priority="130" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="131" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="30" priority="131" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="132" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="29" priority="132" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50">
-    <cfRule type="containsText" dxfId="32" priority="129" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="28" priority="129" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B215">
-    <cfRule type="containsText" dxfId="31" priority="66" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="27" priority="66" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B215)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="67" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="26" priority="67" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B215)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="68" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="25" priority="68" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B215)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B215">
-    <cfRule type="containsText" dxfId="28" priority="65" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="24" priority="65" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B215)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B219">
-    <cfRule type="containsText" dxfId="27" priority="58" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="23" priority="58" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B219)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="59" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="22" priority="59" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B219)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="60" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="21" priority="60" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B219)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B219">
-    <cfRule type="containsText" dxfId="24" priority="57" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="20" priority="57" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B219)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B216:B218">
-    <cfRule type="containsText" dxfId="23" priority="62" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="19" priority="62" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B216)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="63" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="18" priority="63" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B216)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="64" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="17" priority="64" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B216)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B216:B218">
-    <cfRule type="containsText" dxfId="20" priority="61" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="16" priority="61" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B216)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91">
-    <cfRule type="containsText" dxfId="19" priority="42" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="15" priority="42" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B91)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="43" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="14" priority="43" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B91)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="44" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="13" priority="44" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B91)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91">
-    <cfRule type="containsText" dxfId="16" priority="41" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="12" priority="41" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B91)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B96:B141 B143:B206">
-    <cfRule type="containsText" dxfId="15" priority="10" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="11" priority="10" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="11" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="12" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B96)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B96:B141 B143:B206">
-    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B96)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B142">
-    <cfRule type="containsText" dxfId="11" priority="6" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="7" priority="6" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B142)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B142)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="5" priority="8" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B142)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B142">
-    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B142)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15071,8 +15106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A53:E104"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Remove publishers relinking page
This one needs some good testing!
</commit_message>
<xml_diff>
--- a/Technical documentation/AL table analysis.xlsx
+++ b/Technical documentation/AL table analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Table overview" sheetId="1" r:id="rId1"/>
@@ -1143,7 +1143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1866" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1870" uniqueCount="609">
   <si>
     <t>Table name</t>
   </si>
@@ -2876,9 +2876,6 @@
     <t>Add language_id field</t>
   </si>
   <si>
-    <t>Will be removed when publisher relinking is done</t>
-  </si>
-  <si>
     <t>Changed using DB script nr 165</t>
   </si>
   <si>
@@ -2967,6 +2964,15 @@
   </si>
   <si>
     <t>Created using DB script 208</t>
+  </si>
+  <si>
+    <t>Deleted using DB script nr 210</t>
+  </si>
+  <si>
+    <t>Deleted using DB script nr 211</t>
+  </si>
+  <si>
+    <t>Deleted using DB script nr 212</t>
   </si>
 </sst>
 </file>
@@ -6961,7 +6967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F306"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
@@ -7330,10 +7336,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="35" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B24" s="39" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C24" s="42" t="s">
         <v>16</v>
@@ -7344,10 +7350,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="35" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B25" s="39" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C25" s="42" t="s">
         <v>16</v>
@@ -10999,7 +11005,7 @@
         <v>2</v>
       </c>
       <c r="D292" s="39" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="E292" s="43" t="s">
         <v>8</v>
@@ -12374,8 +12380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P223"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="52.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12545,8 +12551,12 @@
       <c r="B12" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
+      <c r="C12" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D12" s="69" t="s">
+        <v>608</v>
+      </c>
     </row>
     <row r="13" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
@@ -12559,7 +12569,7 @@
         <v>550</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -12592,7 +12602,7 @@
       <c r="C16" s="69"/>
       <c r="D16" s="69"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="35" t="s">
         <v>237</v>
       </c>
@@ -12602,22 +12612,23 @@
       <c r="C17" s="69"/>
       <c r="D17" s="69"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="35" t="s">
         <v>239</v>
       </c>
       <c r="B18" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="69"/>
-      <c r="D18" s="69"/>
-      <c r="E18" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D18" s="69" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="35" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B19" s="42" t="s">
         <v>16</v>
@@ -12626,10 +12637,10 @@
         <v>550</v>
       </c>
       <c r="D19" s="69" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="35" t="s">
         <v>102</v>
       </c>
@@ -12639,7 +12650,7 @@
       <c r="C20" s="69"/>
       <c r="D20" s="69"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="35" t="s">
         <v>241</v>
       </c>
@@ -12649,7 +12660,7 @@
       <c r="C21" s="69"/>
       <c r="D21" s="69"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="35" t="s">
         <v>255</v>
       </c>
@@ -12659,7 +12670,7 @@
       <c r="C22" s="69"/>
       <c r="D22" s="69"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="35" t="s">
         <v>252</v>
       </c>
@@ -12669,7 +12680,7 @@
       <c r="C23" s="69"/>
       <c r="D23" s="69"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="35" t="s">
         <v>254</v>
       </c>
@@ -12679,7 +12690,7 @@
       <c r="C24" s="69"/>
       <c r="D24" s="69"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="35" t="s">
         <v>265</v>
       </c>
@@ -12689,7 +12700,7 @@
       <c r="C25" s="69"/>
       <c r="D25" s="69"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="35" t="s">
         <v>268</v>
       </c>
@@ -12699,7 +12710,7 @@
       <c r="C26" s="69"/>
       <c r="D26" s="69"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="35" t="s">
         <v>270</v>
       </c>
@@ -12709,7 +12720,7 @@
       <c r="C27" s="69"/>
       <c r="D27" s="69"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="35" t="s">
         <v>271</v>
       </c>
@@ -12719,7 +12730,7 @@
       <c r="C28" s="69"/>
       <c r="D28" s="69"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="35" t="s">
         <v>272</v>
       </c>
@@ -12729,7 +12740,7 @@
       <c r="C29" s="69"/>
       <c r="D29" s="69"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="35" t="s">
         <v>273</v>
       </c>
@@ -12739,7 +12750,7 @@
       <c r="C30" s="69"/>
       <c r="D30" s="69"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="35" t="s">
         <v>274</v>
       </c>
@@ -12749,7 +12760,7 @@
       <c r="C31" s="69"/>
       <c r="D31" s="69"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="35" t="s">
         <v>275</v>
       </c>
@@ -13020,7 +13031,7 @@
         <v>550</v>
       </c>
       <c r="D58" s="69" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -13062,7 +13073,7 @@
       </c>
       <c r="C62" s="69"/>
       <c r="D62" s="38" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -13076,7 +13087,7 @@
         <v>550</v>
       </c>
       <c r="D63" s="69" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -13090,7 +13101,7 @@
         <v>550</v>
       </c>
       <c r="D64" s="38" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -13124,7 +13135,7 @@
         <v>550</v>
       </c>
       <c r="D67" s="38" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13138,21 +13149,21 @@
         <v>550</v>
       </c>
       <c r="D68" s="38" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="35" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B69" s="42" t="s">
         <v>16</v>
       </c>
       <c r="C69" s="69" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D69" s="69" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -13320,7 +13331,7 @@
         <v>550</v>
       </c>
       <c r="D85" s="69" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -13438,7 +13449,7 @@
         <v>550</v>
       </c>
       <c r="D94" s="38" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -13452,7 +13463,7 @@
         <v>550</v>
       </c>
       <c r="D95" s="38" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -13466,10 +13477,10 @@
         <v>550</v>
       </c>
       <c r="D96" s="38" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="35" t="s">
         <v>81</v>
       </c>
@@ -13483,7 +13494,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="35" t="s">
         <v>30</v>
       </c>
@@ -13493,7 +13504,7 @@
       <c r="C98" s="69"/>
       <c r="D98" s="69"/>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="41" t="s">
         <v>10</v>
       </c>
@@ -13504,23 +13515,24 @@
         <v>550</v>
       </c>
       <c r="D99" s="69" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="35" t="s">
         <v>346</v>
       </c>
       <c r="B100" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C100" s="69"/>
-      <c r="D100" s="69"/>
-      <c r="E100" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C100" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D100" s="69" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="35" t="s">
         <v>33</v>
       </c>
@@ -13534,7 +13546,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="35" t="s">
         <v>100</v>
       </c>
@@ -13544,7 +13556,7 @@
       <c r="C102" s="69"/>
       <c r="D102" s="69"/>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="35" t="s">
         <v>125</v>
       </c>
@@ -13554,7 +13566,7 @@
       <c r="C103" s="69"/>
       <c r="D103" s="69"/>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="35" t="s">
         <v>104</v>
       </c>
@@ -13564,7 +13576,7 @@
       <c r="C104" s="69"/>
       <c r="D104" s="69"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="35" t="s">
         <v>87</v>
       </c>
@@ -13574,7 +13586,7 @@
       <c r="C105" s="69"/>
       <c r="D105" s="69"/>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="35" t="s">
         <v>90</v>
       </c>
@@ -13584,7 +13596,7 @@
       <c r="C106" s="69"/>
       <c r="D106" s="69"/>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="35" t="s">
         <v>89</v>
       </c>
@@ -13594,7 +13606,7 @@
       <c r="C107" s="69"/>
       <c r="D107" s="69"/>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="35" t="s">
         <v>172</v>
       </c>
@@ -13604,7 +13616,7 @@
       <c r="C108" s="69"/>
       <c r="D108" s="69"/>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="35" t="s">
         <v>94</v>
       </c>
@@ -13615,10 +13627,10 @@
         <v>550</v>
       </c>
       <c r="D109" s="69" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="35" t="s">
         <v>95</v>
       </c>
@@ -13628,7 +13640,7 @@
       <c r="C110" s="69"/>
       <c r="D110" s="69"/>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="35" t="s">
         <v>96</v>
       </c>
@@ -13638,7 +13650,7 @@
       <c r="C111" s="69"/>
       <c r="D111" s="69"/>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="35" t="s">
         <v>93</v>
       </c>
@@ -13721,7 +13733,7 @@
         <v>550</v>
       </c>
       <c r="D118" s="69" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -13735,7 +13747,7 @@
         <v>550</v>
       </c>
       <c r="D119" s="69" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -13759,7 +13771,7 @@
         <v>550</v>
       </c>
       <c r="D121" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -13801,7 +13813,7 @@
         <v>550</v>
       </c>
       <c r="D124" s="69" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -13999,7 +14011,7 @@
         <v>550</v>
       </c>
       <c r="D143" s="66" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -14013,7 +14025,7 @@
         <v>550</v>
       </c>
       <c r="D144" s="66" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -14027,7 +14039,7 @@
         <v>550</v>
       </c>
       <c r="D145" s="69" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -14041,7 +14053,7 @@
         <v>550</v>
       </c>
       <c r="D146" s="69" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -14422,10 +14434,10 @@
         <v>16</v>
       </c>
       <c r="C184" s="69" t="s">
+        <v>589</v>
+      </c>
+      <c r="D184" s="69" t="s">
         <v>590</v>
-      </c>
-      <c r="D184" s="69" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -14439,7 +14451,7 @@
         <v>550</v>
       </c>
       <c r="D185" s="69" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -15316,7 +15328,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A53:E106"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
@@ -15456,10 +15468,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="16" t="s">
+        <v>598</v>
+      </c>
+      <c r="B63" s="5" t="s">
         <v>599</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>600</v>
       </c>
       <c r="C63" s="9"/>
       <c r="D63" s="5"/>
@@ -15467,10 +15479,10 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="16" t="s">
+        <v>600</v>
+      </c>
+      <c r="B64" s="5" t="s">
         <v>601</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>602</v>
       </c>
       <c r="C64" s="9"/>
       <c r="D64" s="5"/>

</xml_diff>

<commit_message>
Final correction to the analysis
</commit_message>
<xml_diff>
--- a/Technical documentation/AL table analysis.xlsx
+++ b/Technical documentation/AL table analysis.xlsx
@@ -1143,7 +1143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1872" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1878" uniqueCount="612">
   <si>
     <t>Table name</t>
   </si>
@@ -2876,9 +2876,6 @@
     <t>Add language_id field</t>
   </si>
   <si>
-    <t>Will be removed when publisher relinking is done</t>
-  </si>
-  <si>
     <t>Changed using DB script nr 165</t>
   </si>
   <si>
@@ -2973,6 +2970,18 @@
   </si>
   <si>
     <t>When a release has another title, this title is stored in here, Eg. No seperate release but language selection in game.</t>
+  </si>
+  <si>
+    <t>Created using DB script nr 213</t>
+  </si>
+  <si>
+    <t>Deleted using DB script nr 211</t>
+  </si>
+  <si>
+    <t>Deleted using DB script nr 212</t>
+  </si>
+  <si>
+    <t>Deleted using DB script nr 210</t>
   </si>
 </sst>
 </file>
@@ -3587,7 +3596,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="420">
+  <dxfs count="404">
     <dxf>
       <fill>
         <patternFill>
@@ -4235,6 +4244,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFC2E49C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFDB69"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5757"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="0"/>
         </patternFill>
       </fill>
@@ -4263,6 +4293,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFC2E49C"/>
         </patternFill>
       </fill>
@@ -4291,6 +4328,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFC2E49C"/>
         </patternFill>
       </fill>
@@ -4347,6 +4391,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFC2E49C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFDB69"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5757"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="0"/>
         </patternFill>
       </fill>
@@ -6027,6 +6092,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFC2E49C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFDB69"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5757"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="0"/>
         </patternFill>
       </fill>
@@ -6139,6 +6225,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFC2E49C"/>
         </patternFill>
       </fill>
@@ -6160,6 +6253,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFC2E49C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFDB69"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5757"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="0"/>
         </patternFill>
       </fill>
@@ -6195,6 +6309,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFC2E49C"/>
         </patternFill>
       </fill>
@@ -6245,230 +6366,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC2E49C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDB69"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5757"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC2E49C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDB69"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5757"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC2E49C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDB69"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5757"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC2E49C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDB69"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5757"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC2E49C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDB69"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5757"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC2E49C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDB69"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5757"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC2E49C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDB69"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5757"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC2E49C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDB69"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5757"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7474,10 +7371,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="35" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B24" s="39" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C24" s="42" t="s">
         <v>16</v>
@@ -7488,10 +7385,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="35" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B25" s="39" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C25" s="42" t="s">
         <v>16</v>
@@ -7955,10 +7852,10 @@
     </row>
     <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="35" t="s">
+        <v>606</v>
+      </c>
+      <c r="B53" s="39" t="s">
         <v>607</v>
-      </c>
-      <c r="B53" s="39" t="s">
-        <v>608</v>
       </c>
       <c r="C53" s="42" t="s">
         <v>16</v>
@@ -11158,7 +11055,7 @@
         <v>2</v>
       </c>
       <c r="D293" s="39" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="E293" s="43" t="s">
         <v>8</v>
@@ -11380,1154 +11277,1154 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C82:C85 C281 C289:C291 C98:C99 C76:C78 C54:C73 C4:C11 C87:C94 C42:C44 C181 C114:C115 C249:C250 C118:C119 C96 C283:C287 C27:C39 C13:C25">
-    <cfRule type="containsText" dxfId="411" priority="358" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="403" priority="358" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="410" priority="359" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="402" priority="359" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="409" priority="360" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="401" priority="360" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C85 C281 C289:C291 C98:C99 C76:C78 C54:C73 C4:C11 C87:C94 C42:C44 C181 C114:C115 C249:C250 C118:C119 C96 C283:C287 C27:C39 C13:C25">
-    <cfRule type="containsText" dxfId="408" priority="357" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="400" priority="357" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C103">
-    <cfRule type="containsText" dxfId="407" priority="354" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="399" priority="354" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C103)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="406" priority="355" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="398" priority="355" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C103)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="405" priority="356" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="397" priority="356" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C103)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C103">
-    <cfRule type="containsText" dxfId="404" priority="353" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="396" priority="353" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C103)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C105">
-    <cfRule type="containsText" dxfId="403" priority="345" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="395" priority="345" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C105)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C104">
-    <cfRule type="containsText" dxfId="402" priority="350" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="394" priority="350" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C104)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="401" priority="351" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="393" priority="351" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C104)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="400" priority="352" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="392" priority="352" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C104)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C104">
-    <cfRule type="containsText" dxfId="399" priority="349" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="391" priority="349" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C104)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C105">
-    <cfRule type="containsText" dxfId="398" priority="346" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="390" priority="346" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C105)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="397" priority="347" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="389" priority="347" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C105)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="396" priority="348" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="388" priority="348" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C105)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C107:C109">
-    <cfRule type="containsText" dxfId="395" priority="337" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="387" priority="337" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C107)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C106">
-    <cfRule type="containsText" dxfId="394" priority="341" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="386" priority="341" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C106)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C106">
-    <cfRule type="containsText" dxfId="393" priority="342" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="385" priority="342" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C106)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="392" priority="343" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="384" priority="343" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C106)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="391" priority="344" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="383" priority="344" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C106)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C288">
-    <cfRule type="containsText" dxfId="390" priority="309" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="382" priority="309" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C288)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C107:C109">
-    <cfRule type="containsText" dxfId="389" priority="338" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="381" priority="338" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="388" priority="339" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="380" priority="339" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="387" priority="340" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="379" priority="340" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C107)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C292">
-    <cfRule type="containsText" dxfId="386" priority="334" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="378" priority="334" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C292)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="385" priority="335" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="377" priority="335" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C292)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="384" priority="336" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="376" priority="336" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C292)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C292">
-    <cfRule type="containsText" dxfId="383" priority="333" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="375" priority="333" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C292)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C294">
-    <cfRule type="containsText" dxfId="382" priority="326" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="374" priority="326" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C294)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="381" priority="327" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="373" priority="327" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C294)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="380" priority="328" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="372" priority="328" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C294)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C294">
-    <cfRule type="containsText" dxfId="379" priority="325" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="371" priority="325" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C294)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C295">
-    <cfRule type="containsText" dxfId="378" priority="322" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="370" priority="322" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C295)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="377" priority="323" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="369" priority="323" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C295)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="376" priority="324" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="368" priority="324" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C295)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C295">
-    <cfRule type="containsText" dxfId="375" priority="321" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="367" priority="321" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C295)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C296">
-    <cfRule type="containsText" dxfId="374" priority="318" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="366" priority="318" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C296)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="373" priority="319" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="365" priority="319" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C296)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="372" priority="320" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="364" priority="320" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C296)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C296">
-    <cfRule type="containsText" dxfId="371" priority="317" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="363" priority="317" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C296)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C297">
-    <cfRule type="containsText" dxfId="370" priority="314" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="362" priority="314" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C297)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="369" priority="315" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="361" priority="315" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C297)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="368" priority="316" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="360" priority="316" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C297)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C297">
-    <cfRule type="containsText" dxfId="367" priority="313" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="359" priority="313" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C297)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C288">
-    <cfRule type="containsText" dxfId="366" priority="310" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="358" priority="310" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C288)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="365" priority="311" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="357" priority="311" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C288)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="364" priority="312" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="356" priority="312" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C288)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C113">
-    <cfRule type="containsText" dxfId="363" priority="306" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="355" priority="306" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C113)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="362" priority="307" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="354" priority="307" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C113)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="361" priority="308" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="353" priority="308" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C113)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C113">
-    <cfRule type="containsText" dxfId="360" priority="305" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="352" priority="305" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C113)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C150">
-    <cfRule type="containsText" dxfId="359" priority="298" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="351" priority="298" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C150)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="358" priority="299" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="350" priority="299" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C150)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="357" priority="300" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="349" priority="300" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C150)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C150">
-    <cfRule type="containsText" dxfId="356" priority="297" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="348" priority="297" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C150)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C151">
-    <cfRule type="containsText" dxfId="355" priority="294" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="347" priority="294" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C151)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="354" priority="295" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="346" priority="295" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C151)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="353" priority="296" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="345" priority="296" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C151)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C151">
-    <cfRule type="containsText" dxfId="352" priority="293" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="344" priority="293" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C151)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C152">
-    <cfRule type="containsText" dxfId="351" priority="290" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="343" priority="290" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C152)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="350" priority="291" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="342" priority="291" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C152)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="349" priority="292" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="341" priority="292" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C152)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C152">
-    <cfRule type="containsText" dxfId="348" priority="289" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="340" priority="289" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C152)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C153">
-    <cfRule type="containsText" dxfId="347" priority="286" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="339" priority="286" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C153)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="346" priority="287" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="338" priority="287" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C153)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="345" priority="288" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="337" priority="288" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C153)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C153">
-    <cfRule type="containsText" dxfId="344" priority="285" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="336" priority="285" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C153)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C154">
-    <cfRule type="containsText" dxfId="343" priority="282" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="335" priority="282" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C154)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="342" priority="283" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="334" priority="283" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C154)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="341" priority="284" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="333" priority="284" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C154)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C154">
-    <cfRule type="containsText" dxfId="340" priority="281" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="332" priority="281" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C154)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C155">
-    <cfRule type="containsText" dxfId="339" priority="278" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="331" priority="278" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C155)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="338" priority="279" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="330" priority="279" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C155)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="337" priority="280" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="329" priority="280" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C155)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C155">
-    <cfRule type="containsText" dxfId="336" priority="277" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="328" priority="277" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C155)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C156">
-    <cfRule type="containsText" dxfId="335" priority="274" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="327" priority="274" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C156)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="334" priority="275" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="326" priority="275" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C156)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="333" priority="276" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="325" priority="276" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C156)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C156">
-    <cfRule type="containsText" dxfId="332" priority="273" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="324" priority="273" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C156)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C157">
-    <cfRule type="containsText" dxfId="331" priority="270" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="323" priority="270" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C157)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="330" priority="271" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="322" priority="271" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C157)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="329" priority="272" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="321" priority="272" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C157)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C157">
-    <cfRule type="containsText" dxfId="328" priority="269" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="320" priority="269" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C157)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C158">
-    <cfRule type="containsText" dxfId="327" priority="266" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="319" priority="266" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C158)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="326" priority="267" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="318" priority="267" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C158)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="325" priority="268" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="317" priority="268" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C158)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C158">
-    <cfRule type="containsText" dxfId="324" priority="265" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="316" priority="265" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C158)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C159">
-    <cfRule type="containsText" dxfId="323" priority="262" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="315" priority="262" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C159)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="322" priority="263" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="314" priority="263" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C159)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="321" priority="264" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="313" priority="264" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C159)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C159">
-    <cfRule type="containsText" dxfId="320" priority="261" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="312" priority="261" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C159)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C160">
-    <cfRule type="containsText" dxfId="319" priority="258" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="311" priority="258" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C160)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="318" priority="259" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="310" priority="259" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C160)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="317" priority="260" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="309" priority="260" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C160)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C160">
-    <cfRule type="containsText" dxfId="316" priority="257" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="308" priority="257" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C160)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C161">
-    <cfRule type="containsText" dxfId="315" priority="254" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="307" priority="254" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C161)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="314" priority="255" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="306" priority="255" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C161)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="313" priority="256" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="305" priority="256" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C161)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C161">
-    <cfRule type="containsText" dxfId="312" priority="253" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="304" priority="253" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C161)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C162">
-    <cfRule type="containsText" dxfId="311" priority="250" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="303" priority="250" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C162)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="310" priority="251" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="302" priority="251" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C162)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="309" priority="252" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="301" priority="252" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C162)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C162">
-    <cfRule type="containsText" dxfId="308" priority="249" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="300" priority="249" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C162)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C163">
-    <cfRule type="containsText" dxfId="307" priority="246" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="299" priority="246" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C163)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="306" priority="247" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="298" priority="247" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C163)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="305" priority="248" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="297" priority="248" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C163)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C163">
-    <cfRule type="containsText" dxfId="304" priority="245" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="296" priority="245" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C163)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C164">
-    <cfRule type="containsText" dxfId="303" priority="242" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="295" priority="242" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C164)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="302" priority="243" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="294" priority="243" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C164)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="301" priority="244" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="293" priority="244" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C164)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C164">
-    <cfRule type="containsText" dxfId="300" priority="241" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="292" priority="241" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C164)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C165">
-    <cfRule type="containsText" dxfId="299" priority="238" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="291" priority="238" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C165)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="298" priority="239" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="290" priority="239" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C165)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="297" priority="240" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="289" priority="240" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C165)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C165">
-    <cfRule type="containsText" dxfId="296" priority="237" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="288" priority="237" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C165)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C166">
-    <cfRule type="containsText" dxfId="295" priority="234" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="287" priority="234" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C166)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="294" priority="235" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="286" priority="235" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C166)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="293" priority="236" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="285" priority="236" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C166)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C166">
-    <cfRule type="containsText" dxfId="292" priority="233" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="284" priority="233" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C166)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C167">
-    <cfRule type="containsText" dxfId="291" priority="230" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="283" priority="230" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C167)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="290" priority="231" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="282" priority="231" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C167)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="289" priority="232" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="281" priority="232" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C167)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C167">
-    <cfRule type="containsText" dxfId="288" priority="229" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="280" priority="229" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C167)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C168:C170">
-    <cfRule type="containsText" dxfId="287" priority="226" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="279" priority="226" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C168)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="286" priority="227" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="278" priority="227" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C168)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="285" priority="228" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="277" priority="228" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C168)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C168:C170">
-    <cfRule type="containsText" dxfId="284" priority="225" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="276" priority="225" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C168)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C299">
-    <cfRule type="containsText" dxfId="283" priority="218" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="275" priority="218" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C299)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="282" priority="219" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="274" priority="219" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C299)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="281" priority="220" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="273" priority="220" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C299)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C299">
-    <cfRule type="containsText" dxfId="280" priority="217" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="272" priority="217" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C299)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C86">
-    <cfRule type="containsText" dxfId="279" priority="206" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="271" priority="206" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="278" priority="207" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="270" priority="207" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="277" priority="208" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="269" priority="208" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C86)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C86">
-    <cfRule type="containsText" dxfId="276" priority="205" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="268" priority="205" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C86)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="275" priority="194" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="267" priority="194" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="274" priority="195" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="266" priority="195" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="273" priority="196" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="265" priority="196" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="272" priority="193" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="264" priority="193" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C75">
-    <cfRule type="containsText" dxfId="271" priority="182" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="263" priority="182" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="270" priority="183" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="262" priority="183" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="269" priority="184" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="261" priority="184" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C75">
-    <cfRule type="containsText" dxfId="268" priority="181" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="260" priority="181" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74">
-    <cfRule type="containsText" dxfId="267" priority="186" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="259" priority="186" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C74)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="266" priority="187" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="258" priority="187" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C74)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="265" priority="188" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="257" priority="188" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74">
-    <cfRule type="containsText" dxfId="264" priority="185" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="256" priority="185" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51:C52">
-    <cfRule type="containsText" dxfId="263" priority="190" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="255" priority="190" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="262" priority="191" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="254" priority="191" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="261" priority="192" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="253" priority="192" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51:C52">
-    <cfRule type="containsText" dxfId="260" priority="189" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="252" priority="189" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C97">
-    <cfRule type="containsText" dxfId="259" priority="174" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="251" priority="174" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C97)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="258" priority="175" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="250" priority="175" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C97)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="257" priority="176" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="249" priority="176" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C97)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C97">
-    <cfRule type="containsText" dxfId="256" priority="173" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="248" priority="173" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C97)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="255" priority="170" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="247" priority="170" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="254" priority="171" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="246" priority="171" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="253" priority="172" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="245" priority="172" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="252" priority="169" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="244" priority="169" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="containsText" dxfId="251" priority="166" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="243" priority="166" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="250" priority="167" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="242" priority="167" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="249" priority="168" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="241" priority="168" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="containsText" dxfId="248" priority="165" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="240" priority="165" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C49">
-    <cfRule type="containsText" dxfId="247" priority="162" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="239" priority="162" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="246" priority="163" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="238" priority="163" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="245" priority="164" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="237" priority="164" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C49">
-    <cfRule type="containsText" dxfId="244" priority="161" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="236" priority="161" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="243" priority="158" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="235" priority="158" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="242" priority="159" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="234" priority="159" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="241" priority="160" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="233" priority="160" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="240" priority="157" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="232" priority="157" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="239" priority="154" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="231" priority="154" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="238" priority="155" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="230" priority="155" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="237" priority="156" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="229" priority="156" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="236" priority="153" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="228" priority="153" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="containsText" dxfId="235" priority="150" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="227" priority="150" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="234" priority="151" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="226" priority="151" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="233" priority="152" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="225" priority="152" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="containsText" dxfId="232" priority="149" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="224" priority="149" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C230">
-    <cfRule type="containsText" dxfId="231" priority="146" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="223" priority="146" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C230)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="230" priority="147" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="222" priority="147" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C230)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="229" priority="148" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="221" priority="148" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C230)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C230">
-    <cfRule type="containsText" dxfId="228" priority="145" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="220" priority="145" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C230)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C231">
-    <cfRule type="containsText" dxfId="227" priority="142" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="219" priority="142" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C231)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="226" priority="143" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="218" priority="143" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C231)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="225" priority="144" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="217" priority="144" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C231)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C231">
-    <cfRule type="containsText" dxfId="224" priority="141" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="216" priority="141" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C231)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C232">
-    <cfRule type="containsText" dxfId="223" priority="138" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="215" priority="138" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C232)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="222" priority="139" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="214" priority="139" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C232)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="221" priority="140" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="213" priority="140" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C232)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C232">
-    <cfRule type="containsText" dxfId="220" priority="137" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="212" priority="137" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C232)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C145:C146">
-    <cfRule type="containsText" dxfId="219" priority="134" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="211" priority="134" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C145)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="218" priority="135" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="210" priority="135" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C145)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="217" priority="136" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="209" priority="136" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C145)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C145:C146">
-    <cfRule type="containsText" dxfId="216" priority="133" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="208" priority="133" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C145)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C143">
-    <cfRule type="containsText" dxfId="215" priority="122" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="207" priority="122" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C143)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="214" priority="123" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="206" priority="123" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C143)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="213" priority="124" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="205" priority="124" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C143)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C143">
-    <cfRule type="containsText" dxfId="212" priority="121" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="204" priority="121" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C143)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C138">
-    <cfRule type="containsText" dxfId="211" priority="118" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="203" priority="118" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C138)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="210" priority="119" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="202" priority="119" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C138)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="209" priority="120" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="201" priority="120" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C138)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C138">
-    <cfRule type="containsText" dxfId="208" priority="117" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="200" priority="117" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C138)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C239">
-    <cfRule type="containsText" dxfId="207" priority="110" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="199" priority="110" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C239)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="206" priority="111" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="198" priority="111" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C239)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="205" priority="112" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="197" priority="112" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C239)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C239">
-    <cfRule type="containsText" dxfId="204" priority="109" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="196" priority="109" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C239)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C241:C243">
-    <cfRule type="containsText" dxfId="203" priority="106" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="195" priority="106" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C241)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="202" priority="107" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="194" priority="107" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C241)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="201" priority="108" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="193" priority="108" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C241)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C241:C243">
-    <cfRule type="containsText" dxfId="200" priority="105" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="192" priority="105" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C241)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C238">
-    <cfRule type="containsText" dxfId="199" priority="102" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="191" priority="102" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C238)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="198" priority="103" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="190" priority="103" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C238)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="197" priority="104" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="189" priority="104" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C238)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C238">
-    <cfRule type="containsText" dxfId="196" priority="101" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="188" priority="101" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C238)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C255">
-    <cfRule type="containsText" dxfId="195" priority="98" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="187" priority="98" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C255)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="194" priority="99" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="186" priority="99" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C255)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="193" priority="100" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="185" priority="100" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C255)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C255">
-    <cfRule type="containsText" dxfId="192" priority="97" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="184" priority="97" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C255)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C256:C260">
-    <cfRule type="containsText" dxfId="191" priority="94" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="183" priority="94" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C256)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="190" priority="95" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="182" priority="95" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C256)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="189" priority="96" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="181" priority="96" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C256)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C256:C260">
-    <cfRule type="containsText" dxfId="188" priority="93" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="180" priority="93" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C256)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A254:E258">
-    <cfRule type="containsText" dxfId="187" priority="90" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="179" priority="90" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",A254)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="186" priority="91" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="178" priority="91" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",A254)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="185" priority="92" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="177" priority="92" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",A254)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A254:E258">
-    <cfRule type="containsText" dxfId="184" priority="89" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="176" priority="89" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",A254)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C248">
-    <cfRule type="containsText" dxfId="183" priority="86" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="175" priority="86" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C248)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="182" priority="87" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="174" priority="87" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C248)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="181" priority="88" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="173" priority="88" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C248)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C248">
-    <cfRule type="containsText" dxfId="180" priority="85" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="172" priority="85" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C248)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C247">
-    <cfRule type="containsText" dxfId="179" priority="78" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="171" priority="78" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C247)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="178" priority="79" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="170" priority="79" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C247)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="177" priority="80" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="169" priority="80" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C247)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C247">
-    <cfRule type="containsText" dxfId="176" priority="77" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="168" priority="77" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C247)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C205">
-    <cfRule type="containsText" dxfId="175" priority="74" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="167" priority="74" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C205)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="174" priority="75" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="166" priority="75" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C205)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="173" priority="76" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="165" priority="76" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C205)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C205">
-    <cfRule type="containsText" dxfId="172" priority="73" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="164" priority="73" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C205)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C301">
-    <cfRule type="containsText" dxfId="171" priority="62" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="163" priority="62" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C301)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="170" priority="63" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="162" priority="63" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C301)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="169" priority="64" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="161" priority="64" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C301)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C301">
-    <cfRule type="containsText" dxfId="168" priority="61" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="160" priority="61" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C301)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C305">
-    <cfRule type="containsText" dxfId="167" priority="54" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="159" priority="54" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C305)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="166" priority="55" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="158" priority="55" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C305)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="165" priority="56" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="157" priority="56" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C305)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C305">
-    <cfRule type="containsText" dxfId="164" priority="53" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="156" priority="53" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C305)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C302:C304">
-    <cfRule type="containsText" dxfId="163" priority="58" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="155" priority="58" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C302)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="162" priority="59" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="154" priority="59" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C302)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="161" priority="60" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="153" priority="60" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C302:C304">
-    <cfRule type="containsText" dxfId="160" priority="57" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="152" priority="57" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C267:C268">
-    <cfRule type="containsText" dxfId="159" priority="50" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="151" priority="50" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C267)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="158" priority="51" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="150" priority="51" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C267)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="157" priority="52" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="149" priority="52" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C267)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C267:C268">
-    <cfRule type="containsText" dxfId="156" priority="49" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="148" priority="49" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C267)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A264:E266">
-    <cfRule type="containsText" dxfId="155" priority="34" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="147" priority="34" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",A264)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="154" priority="35" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="146" priority="35" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",A264)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="153" priority="36" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="145" priority="36" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",A264)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A264:E266">
-    <cfRule type="containsText" dxfId="152" priority="33" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="144" priority="33" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",A264)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A272:E277">
-    <cfRule type="containsText" dxfId="151" priority="30" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="143" priority="30" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",A272)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="150" priority="31" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="142" priority="31" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",A272)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="149" priority="32" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="141" priority="32" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",A272)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A272:E277">
-    <cfRule type="containsText" dxfId="148" priority="29" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="140" priority="29" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",A272)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C95">
-    <cfRule type="containsText" dxfId="147" priority="26" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="139" priority="26" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C95)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="146" priority="27" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="138" priority="27" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C95)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="145" priority="28" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="137" priority="28" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C95)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C95">
-    <cfRule type="containsText" dxfId="144" priority="25" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="136" priority="25" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C95)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C240">
-    <cfRule type="containsText" dxfId="143" priority="22" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="135" priority="22" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C240)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="142" priority="23" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="134" priority="23" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C240)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="141" priority="24" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="133" priority="24" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C240)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C240">
-    <cfRule type="containsText" dxfId="140" priority="21" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="132" priority="21" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C240)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C282">
-    <cfRule type="containsText" dxfId="139" priority="18" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="131" priority="18" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C282)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="138" priority="19" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="130" priority="19" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C282)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="137" priority="20" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="129" priority="20" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C282)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C282">
-    <cfRule type="containsText" dxfId="136" priority="17" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="128" priority="17" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C282)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="containsText" dxfId="135" priority="14" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="127" priority="14" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="134" priority="15" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="126" priority="15" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="133" priority="16" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="125" priority="16" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="containsText" dxfId="132" priority="13" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="124" priority="13" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C293">
-    <cfRule type="containsText" dxfId="131" priority="10" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="123" priority="10" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C293)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="11" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="122" priority="11" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C293)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="12" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="121" priority="12" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C293)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C293">
-    <cfRule type="containsText" dxfId="128" priority="9" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="120" priority="9" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C293)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="containsText" dxfId="127" priority="2" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="119" priority="2" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C53)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="3" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="118" priority="3" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C53)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="125" priority="4" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="117" priority="4" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="containsText" dxfId="124" priority="1" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="116" priority="1" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C53)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12550,7 +12447,7 @@
   <dimension ref="A1:P224"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="52.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12720,8 +12617,12 @@
       <c r="B12" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
+      <c r="C12" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D12" s="69" t="s">
+        <v>610</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
@@ -12734,7 +12635,7 @@
         <v>550</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -12767,7 +12668,7 @@
       <c r="C16" s="69"/>
       <c r="D16" s="69"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="35" t="s">
         <v>237</v>
       </c>
@@ -12777,22 +12678,23 @@
       <c r="C17" s="69"/>
       <c r="D17" s="69"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="35" t="s">
         <v>239</v>
       </c>
       <c r="B18" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="69"/>
-      <c r="D18" s="69"/>
-      <c r="E18" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D18" s="69" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="35" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B19" s="42" t="s">
         <v>16</v>
@@ -12801,10 +12703,10 @@
         <v>550</v>
       </c>
       <c r="D19" s="69" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="35" t="s">
         <v>102</v>
       </c>
@@ -12814,7 +12716,7 @@
       <c r="C20" s="69"/>
       <c r="D20" s="69"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="35" t="s">
         <v>241</v>
       </c>
@@ -12824,7 +12726,7 @@
       <c r="C21" s="69"/>
       <c r="D21" s="69"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="35" t="s">
         <v>255</v>
       </c>
@@ -12834,7 +12736,7 @@
       <c r="C22" s="69"/>
       <c r="D22" s="69"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="35" t="s">
         <v>252</v>
       </c>
@@ -12844,7 +12746,7 @@
       <c r="C23" s="69"/>
       <c r="D23" s="69"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="35" t="s">
         <v>254</v>
       </c>
@@ -12854,7 +12756,7 @@
       <c r="C24" s="69"/>
       <c r="D24" s="69"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="35" t="s">
         <v>265</v>
       </c>
@@ -12864,7 +12766,7 @@
       <c r="C25" s="69"/>
       <c r="D25" s="69"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="35" t="s">
         <v>268</v>
       </c>
@@ -12874,7 +12776,7 @@
       <c r="C26" s="69"/>
       <c r="D26" s="69"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="35" t="s">
         <v>270</v>
       </c>
@@ -12884,7 +12786,7 @@
       <c r="C27" s="69"/>
       <c r="D27" s="69"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="35" t="s">
         <v>271</v>
       </c>
@@ -12894,7 +12796,7 @@
       <c r="C28" s="69"/>
       <c r="D28" s="69"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="35" t="s">
         <v>272</v>
       </c>
@@ -12904,7 +12806,7 @@
       <c r="C29" s="69"/>
       <c r="D29" s="69"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="35" t="s">
         <v>273</v>
       </c>
@@ -12914,7 +12816,7 @@
       <c r="C30" s="69"/>
       <c r="D30" s="69"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="35" t="s">
         <v>274</v>
       </c>
@@ -12924,7 +12826,7 @@
       <c r="C31" s="69"/>
       <c r="D31" s="69"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="35" t="s">
         <v>275</v>
       </c>
@@ -13195,7 +13097,7 @@
         <v>550</v>
       </c>
       <c r="D58" s="69" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -13237,10 +13139,10 @@
       </c>
       <c r="C62" s="69"/>
       <c r="D62" s="38" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="35" t="s">
         <v>313</v>
       </c>
@@ -13251,10 +13153,10 @@
         <v>550</v>
       </c>
       <c r="D63" s="69" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="41" t="s">
         <v>5</v>
       </c>
@@ -13265,10 +13167,10 @@
         <v>550</v>
       </c>
       <c r="D64" s="38" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="35" t="s">
         <v>318</v>
       </c>
@@ -13288,7 +13190,7 @@
       <c r="C66" s="69"/>
       <c r="D66" s="69"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="41" t="s">
         <v>18</v>
       </c>
@@ -13299,7 +13201,7 @@
         <v>550</v>
       </c>
       <c r="D67" s="38" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -13313,24 +13215,24 @@
         <v>550</v>
       </c>
       <c r="D68" s="38" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="35" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B69" s="42" t="s">
         <v>16</v>
       </c>
       <c r="C69" s="69" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D69" s="69" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="35" t="s">
         <v>31</v>
       </c>
@@ -13344,7 +13246,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="35" t="s">
         <v>321</v>
       </c>
@@ -13495,10 +13397,10 @@
         <v>550</v>
       </c>
       <c r="D85" s="69" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="35" t="s">
         <v>342</v>
       </c>
@@ -13512,7 +13414,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="41" t="s">
         <v>20</v>
       </c>
@@ -13602,7 +13504,7 @@
       <c r="C93" s="69"/>
       <c r="D93" s="69"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="41" t="s">
         <v>17</v>
       </c>
@@ -13613,7 +13515,7 @@
         <v>550</v>
       </c>
       <c r="D94" s="38" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -13627,7 +13529,7 @@
         <v>550</v>
       </c>
       <c r="D95" s="38" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -13641,10 +13543,10 @@
         <v>550</v>
       </c>
       <c r="D96" s="38" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="35" t="s">
         <v>81</v>
       </c>
@@ -13658,7 +13560,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="35" t="s">
         <v>30</v>
       </c>
@@ -13668,7 +13570,7 @@
       <c r="C98" s="69"/>
       <c r="D98" s="69"/>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="41" t="s">
         <v>10</v>
       </c>
@@ -13679,23 +13581,24 @@
         <v>550</v>
       </c>
       <c r="D99" s="69" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="35" t="s">
         <v>346</v>
       </c>
       <c r="B100" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C100" s="69"/>
-      <c r="D100" s="69"/>
-      <c r="E100" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C100" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D100" s="69" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="35" t="s">
         <v>33</v>
       </c>
@@ -13709,17 +13612,21 @@
         <v>573</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="35" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B102" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C102" s="69"/>
-      <c r="D102" s="69"/>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C102" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D102" s="69" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="35" t="s">
         <v>100</v>
       </c>
@@ -13729,7 +13636,7 @@
       <c r="C103" s="69"/>
       <c r="D103" s="69"/>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="35" t="s">
         <v>125</v>
       </c>
@@ -13739,7 +13646,7 @@
       <c r="C104" s="69"/>
       <c r="D104" s="69"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="35" t="s">
         <v>104</v>
       </c>
@@ -13749,7 +13656,7 @@
       <c r="C105" s="69"/>
       <c r="D105" s="69"/>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="35" t="s">
         <v>87</v>
       </c>
@@ -13759,7 +13666,7 @@
       <c r="C106" s="69"/>
       <c r="D106" s="69"/>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="35" t="s">
         <v>90</v>
       </c>
@@ -13769,7 +13676,7 @@
       <c r="C107" s="69"/>
       <c r="D107" s="69"/>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="35" t="s">
         <v>89</v>
       </c>
@@ -13779,7 +13686,7 @@
       <c r="C108" s="69"/>
       <c r="D108" s="69"/>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="35" t="s">
         <v>172</v>
       </c>
@@ -13789,7 +13696,7 @@
       <c r="C109" s="69"/>
       <c r="D109" s="69"/>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="35" t="s">
         <v>94</v>
       </c>
@@ -13800,10 +13707,10 @@
         <v>550</v>
       </c>
       <c r="D110" s="69" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="35" t="s">
         <v>95</v>
       </c>
@@ -13813,7 +13720,7 @@
       <c r="C111" s="69"/>
       <c r="D111" s="69"/>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="35" t="s">
         <v>96</v>
       </c>
@@ -13906,7 +13813,7 @@
         <v>550</v>
       </c>
       <c r="D119" s="69" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -13920,7 +13827,7 @@
         <v>550</v>
       </c>
       <c r="D120" s="69" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -13944,7 +13851,7 @@
         <v>550</v>
       </c>
       <c r="D122" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -13986,7 +13893,7 @@
         <v>550</v>
       </c>
       <c r="D125" s="69" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -14184,7 +14091,7 @@
         <v>550</v>
       </c>
       <c r="D144" s="66" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -14198,7 +14105,7 @@
         <v>550</v>
       </c>
       <c r="D145" s="66" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -14212,7 +14119,7 @@
         <v>550</v>
       </c>
       <c r="D146" s="69" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -14226,7 +14133,7 @@
         <v>550</v>
       </c>
       <c r="D147" s="69" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -14607,10 +14514,10 @@
         <v>16</v>
       </c>
       <c r="C185" s="69" t="s">
+        <v>589</v>
+      </c>
+      <c r="D185" s="69" t="s">
         <v>590</v>
-      </c>
-      <c r="D185" s="69" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -14624,7 +14531,7 @@
         <v>550</v>
       </c>
       <c r="D186" s="69" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -15024,466 +14931,466 @@
     <mergeCell ref="A1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="B96">
-    <cfRule type="containsText" dxfId="119" priority="298" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="115" priority="298" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="299" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="114" priority="299" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="300" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="113" priority="300" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B96)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B96">
-    <cfRule type="containsText" dxfId="116" priority="297" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="112" priority="297" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B96)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B40 B43:B45 B55:B61 B77:B91 B63:B74 B6:B14">
-    <cfRule type="containsText" dxfId="115" priority="314" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="111" priority="314" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="315" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="110" priority="315" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="113" priority="316" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="109" priority="316" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B40 B43:B45 B55:B61 B77:B91 B63:B74 B6:B14">
-    <cfRule type="containsText" dxfId="112" priority="313" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="108" priority="313" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B93">
-    <cfRule type="containsText" dxfId="111" priority="310" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="107" priority="310" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="110" priority="311" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="106" priority="311" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="312" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="105" priority="312" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B93)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B93">
-    <cfRule type="containsText" dxfId="108" priority="309" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="104" priority="309" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B93)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B95">
-    <cfRule type="containsText" dxfId="107" priority="301" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="103" priority="301" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B95)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B94">
-    <cfRule type="containsText" dxfId="106" priority="306" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="102" priority="306" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B94)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="307" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="101" priority="307" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B94)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="308" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="100" priority="308" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B94)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B94">
-    <cfRule type="containsText" dxfId="103" priority="305" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="99" priority="305" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B94)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B95">
-    <cfRule type="containsText" dxfId="102" priority="302" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="98" priority="302" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B95)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="101" priority="303" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="97" priority="303" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B95)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="304" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="96" priority="304" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B95)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B208">
-    <cfRule type="containsText" dxfId="99" priority="285" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="95" priority="285" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B208)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B208">
-    <cfRule type="containsText" dxfId="98" priority="286" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="94" priority="286" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B208)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="287" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="93" priority="287" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B208)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="288" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="92" priority="288" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B208)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B209">
-    <cfRule type="containsText" dxfId="95" priority="282" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="91" priority="282" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B209)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="283" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="90" priority="283" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B209)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="284" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="89" priority="284" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B209)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B209">
-    <cfRule type="containsText" dxfId="92" priority="281" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="88" priority="281" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B209)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B210">
-    <cfRule type="containsText" dxfId="91" priority="278" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="87" priority="278" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B210)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="279" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="86" priority="279" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B210)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="280" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="85" priority="280" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B210)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B210">
-    <cfRule type="containsText" dxfId="88" priority="277" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="84" priority="277" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B210)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B211">
-    <cfRule type="containsText" dxfId="87" priority="274" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="83" priority="274" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B211)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="275" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="82" priority="275" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B211)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="276" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="81" priority="276" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B211)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B211">
-    <cfRule type="containsText" dxfId="84" priority="273" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="80" priority="273" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B211)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B212">
-    <cfRule type="containsText" dxfId="83" priority="270" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="79" priority="270" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B212)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="271" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="78" priority="271" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B212)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="272" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="77" priority="272" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B212)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B212">
-    <cfRule type="containsText" dxfId="80" priority="269" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="76" priority="269" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B212)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B214">
-    <cfRule type="containsText" dxfId="79" priority="182" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="75" priority="182" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B214)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="183" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="74" priority="183" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B214)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="184" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="73" priority="184" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B214)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B214">
-    <cfRule type="containsText" dxfId="76" priority="181" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="72" priority="181" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B214)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46:B47">
-    <cfRule type="containsText" dxfId="75" priority="174" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="71" priority="174" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="175" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="70" priority="175" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="176" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="69" priority="176" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46:B47">
-    <cfRule type="containsText" dxfId="72" priority="173" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="68" priority="173" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76">
-    <cfRule type="containsText" dxfId="71" priority="162" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="67" priority="162" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B76)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="163" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="66" priority="163" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B76)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="164" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="65" priority="164" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76">
-    <cfRule type="containsText" dxfId="68" priority="161" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="64" priority="161" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75">
-    <cfRule type="containsText" dxfId="67" priority="166" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="63" priority="166" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="167" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="62" priority="167" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="168" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="61" priority="168" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75">
-    <cfRule type="containsText" dxfId="64" priority="165" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="60" priority="165" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52:B54">
-    <cfRule type="containsText" dxfId="63" priority="170" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="59" priority="170" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="171" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="58" priority="171" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="172" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="57" priority="172" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52:B54">
-    <cfRule type="containsText" dxfId="60" priority="169" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="56" priority="169" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="containsText" dxfId="59" priority="154" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="55" priority="154" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="155" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="54" priority="155" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="156" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="53" priority="156" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="containsText" dxfId="56" priority="153" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="52" priority="153" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="containsText" dxfId="55" priority="150" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="51" priority="150" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="151" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="50" priority="151" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="152" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="49" priority="152" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="containsText" dxfId="52" priority="149" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="48" priority="149" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49:B50">
-    <cfRule type="containsText" dxfId="51" priority="146" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="47" priority="146" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="147" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="46" priority="147" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="148" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="45" priority="148" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49:B50">
-    <cfRule type="containsText" dxfId="48" priority="145" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="44" priority="145" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41">
-    <cfRule type="containsText" dxfId="47" priority="142" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="43" priority="142" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="143" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="42" priority="143" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="144" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="41" priority="144" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41">
-    <cfRule type="containsText" dxfId="44" priority="141" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="40" priority="141" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="containsText" dxfId="43" priority="138" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="39" priority="138" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B42)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="139" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="38" priority="139" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B42)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="140" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="37" priority="140" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="containsText" dxfId="40" priority="137" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="36" priority="137" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51">
-    <cfRule type="containsText" dxfId="39" priority="134" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="35" priority="134" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="135" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="34" priority="135" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="136" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="33" priority="136" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51">
-    <cfRule type="containsText" dxfId="36" priority="133" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="32" priority="133" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B216">
-    <cfRule type="containsText" dxfId="35" priority="70" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="31" priority="70" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B216)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="71" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="30" priority="71" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B216)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="72" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="29" priority="72" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B216)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B216">
-    <cfRule type="containsText" dxfId="32" priority="69" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="28" priority="69" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B216)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B222">
-    <cfRule type="containsText" dxfId="31" priority="62" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="27" priority="62" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B222)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="63" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="26" priority="63" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B222)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="64" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="25" priority="64" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B222)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B222">
-    <cfRule type="containsText" dxfId="28" priority="61" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="24" priority="61" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B222)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B217:B218 B221">
-    <cfRule type="containsText" dxfId="27" priority="66" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="23" priority="66" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B217)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="67" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="22" priority="67" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B217)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="68" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="21" priority="68" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B217)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B217:B218 B221">
-    <cfRule type="containsText" dxfId="24" priority="65" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="20" priority="65" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B217)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B92">
-    <cfRule type="containsText" dxfId="23" priority="46" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="19" priority="46" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B92)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="47" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="18" priority="47" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B92)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="48" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="17" priority="48" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B92)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B92">
-    <cfRule type="containsText" dxfId="20" priority="45" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="16" priority="45" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B92)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B97:B142 B144:B207">
-    <cfRule type="containsText" dxfId="19" priority="14" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="15" priority="14" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B97)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="15" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B97)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="13" priority="16" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B97)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B97:B142 B144:B207">
-    <cfRule type="containsText" dxfId="16" priority="13" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B97)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B143">
-    <cfRule type="containsText" dxfId="15" priority="10" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="11" priority="10" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B143)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="11" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B143)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="12" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B143)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B143">
-    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B143)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62">
-    <cfRule type="containsText" dxfId="11" priority="6" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="7" priority="6" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B62)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B62)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="5" priority="8" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62">
-    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B219:B220">
-    <cfRule type="containsText" dxfId="7" priority="2" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="3" priority="2" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B219)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B219)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B219)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B219:B220">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B219)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15501,8 +15408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A53:E106"/>
   <sheetViews>
-    <sheetView topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15641,10 +15548,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="16" t="s">
+        <v>598</v>
+      </c>
+      <c r="B63" s="5" t="s">
         <v>599</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>600</v>
       </c>
       <c r="C63" s="9"/>
       <c r="D63" s="5"/>
@@ -15652,10 +15559,10 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="16" t="s">
+        <v>600</v>
+      </c>
+      <c r="B64" s="5" t="s">
         <v>601</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>602</v>
       </c>
       <c r="C64" s="9"/>
       <c r="D64" s="5"/>

</xml_diff>

<commit_message>
Game Release Trainer Options
</commit_message>
<xml_diff>
--- a/Technical documentation/AL table analysis.xlsx
+++ b/Technical documentation/AL table analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Table overview" sheetId="1" r:id="rId1"/>
@@ -1143,7 +1143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1885" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1886" uniqueCount="616">
   <si>
     <t>Table name</t>
   </si>
@@ -2991,6 +2991,9 @@
   </si>
   <si>
     <t>Created using DB script nr 219</t>
+  </si>
+  <si>
+    <t>Created using DB script nr 222</t>
   </si>
 </sst>
 </file>
@@ -7013,7 +7016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F307"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12455,8 +12458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P224"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D107" sqref="D107"/>
+    <sheetView topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="52.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13813,7 +13816,9 @@
         <v>16</v>
       </c>
       <c r="C117" s="69"/>
-      <c r="D117" s="69"/>
+      <c r="D117" s="69" t="s">
+        <v>615</v>
+      </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="41" t="s">

</xml_diff>

<commit_message>
Memory enhancements & minimum memory
</commit_message>
<xml_diff>
--- a/Technical documentation/AL table analysis.xlsx
+++ b/Technical documentation/AL table analysis.xlsx
@@ -1143,7 +1143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1886" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="618">
   <si>
     <t>Table name</t>
   </si>
@@ -2994,6 +2994,12 @@
   </si>
   <si>
     <t>Created using DB script nr 222</t>
+  </si>
+  <si>
+    <t>Created using DB script nr 225</t>
+  </si>
+  <si>
+    <t>Created using DB script nr 223</t>
   </si>
 </sst>
 </file>
@@ -12458,8 +12464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P224"/>
   <sheetViews>
-    <sheetView topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="D118" sqref="D118"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="52.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13743,8 +13749,12 @@
       <c r="B111" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C111" s="69"/>
-      <c r="D111" s="69"/>
+      <c r="C111" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D111" s="69" t="s">
+        <v>616</v>
+      </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="35" t="s">
@@ -14221,8 +14231,12 @@
       <c r="B153" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C153" s="69"/>
-      <c r="D153" s="69"/>
+      <c r="C153" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D153" s="69" t="s">
+        <v>617</v>
+      </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="35" t="s">

</xml_diff>

<commit_message>
Game release TOS incompatibility
</commit_message>
<xml_diff>
--- a/Technical documentation/AL table analysis.xlsx
+++ b/Technical documentation/AL table analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Table overview" sheetId="1" r:id="rId1"/>
@@ -1143,7 +1143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="618">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1893" uniqueCount="619">
   <si>
     <t>Table name</t>
   </si>
@@ -3000,6 +3000,9 @@
   </si>
   <si>
     <t>Created using DB script nr 223</t>
+  </si>
+  <si>
+    <t>Created using DB script nr 229</t>
   </si>
 </sst>
 </file>
@@ -7022,7 +7025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F307"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12464,8 +12467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P224"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:P1"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="52.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13815,8 +13818,12 @@
       <c r="B116" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C116" s="69"/>
-      <c r="D116" s="69"/>
+      <c r="C116" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D116" s="69" t="s">
+        <v>618</v>
+      </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="35" t="s">
@@ -13825,7 +13832,9 @@
       <c r="B117" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C117" s="69"/>
+      <c r="C117" s="69" t="s">
+        <v>550</v>
+      </c>
       <c r="D117" s="69" t="s">
         <v>615</v>
       </c>
@@ -15450,7 +15459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A53:E106"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Final bits of Revamp 3
Game Release Status merge, game release notes and game release disk protections
</commit_message>
<xml_diff>
--- a/Technical documentation/AL table analysis.xlsx
+++ b/Technical documentation/AL table analysis.xlsx
@@ -1143,7 +1143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1899" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1909" uniqueCount="626">
   <si>
     <t>Table name</t>
   </si>
@@ -3012,6 +3012,18 @@
   </si>
   <si>
     <t>Created using DB script nr 233</t>
+  </si>
+  <si>
+    <t>Deleted using DB script 236</t>
+  </si>
+  <si>
+    <t>Deleted using script nr 236</t>
+  </si>
+  <si>
+    <t>Created using DB script 237</t>
+  </si>
+  <si>
+    <t>Created using DB script nr 238</t>
   </si>
 </sst>
 </file>
@@ -12476,8 +12488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="D110" sqref="D110"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="52.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12997,8 +13009,12 @@
       <c r="B45" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C45" s="69"/>
-      <c r="D45" s="69"/>
+      <c r="C45" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D45" s="69" t="s">
+        <v>624</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="35" t="s">
@@ -13293,8 +13309,12 @@
       <c r="B71" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C71" s="69"/>
-      <c r="D71" s="69"/>
+      <c r="C71" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D71" s="69" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="35" t="s">
@@ -13697,8 +13717,12 @@
       <c r="B105" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C105" s="69"/>
-      <c r="D105" s="69"/>
+      <c r="C105" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D105" s="69" t="s">
+        <v>625</v>
+      </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="35" t="s">
@@ -13981,8 +14005,12 @@
       <c r="B127" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C127" s="69"/>
-      <c r="D127" s="69"/>
+      <c r="C127" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D127" s="69" t="s">
+        <v>623</v>
+      </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="35" t="s">
@@ -13991,8 +14019,12 @@
       <c r="B128" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C128" s="69"/>
-      <c r="D128" s="69"/>
+      <c r="C128" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D128" s="69" t="s">
+        <v>623</v>
+      </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="35" t="s">
@@ -15481,7 +15513,7 @@
   <dimension ref="A53:E106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Memory enhancements and system enhancements
</commit_message>
<xml_diff>
--- a/Technical documentation/AL table analysis.xlsx
+++ b/Technical documentation/AL table analysis.xlsx
@@ -1143,7 +1143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1913" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1915" uniqueCount="629">
   <si>
     <t>Table name</t>
   </si>
@@ -3030,6 +3030,9 @@
   </si>
   <si>
     <t>Created using DB script nr 239</t>
+  </si>
+  <si>
+    <t>Created using DB script 242</t>
   </si>
 </sst>
 </file>
@@ -3644,39 +3647,11 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="412">
+  <dxfs count="408">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC2E49C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDB69"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5757"/>
         </patternFill>
       </fill>
     </dxf>
@@ -11381,1154 +11356,1154 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C82:C85 C281 C289:C291 C98:C99 C76:C78 C54:C73 C4:C11 C87:C94 C42:C44 C181 C114:C115 C249:C250 C118:C119 C96 C283:C287 C27:C39 C13:C25">
-    <cfRule type="containsText" dxfId="411" priority="358" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="407" priority="358" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="410" priority="359" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="406" priority="359" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="409" priority="360" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="405" priority="360" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C85 C281 C289:C291 C98:C99 C76:C78 C54:C73 C4:C11 C87:C94 C42:C44 C181 C114:C115 C249:C250 C118:C119 C96 C283:C287 C27:C39 C13:C25">
-    <cfRule type="containsText" dxfId="408" priority="357" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="404" priority="357" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C103">
-    <cfRule type="containsText" dxfId="407" priority="354" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="403" priority="354" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C103)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="406" priority="355" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="402" priority="355" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C103)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="405" priority="356" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="401" priority="356" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C103)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C103">
-    <cfRule type="containsText" dxfId="404" priority="353" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="400" priority="353" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C103)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C105">
-    <cfRule type="containsText" dxfId="403" priority="345" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="399" priority="345" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C105)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C104">
-    <cfRule type="containsText" dxfId="402" priority="350" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="398" priority="350" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C104)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="401" priority="351" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="397" priority="351" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C104)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="400" priority="352" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="396" priority="352" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C104)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C104">
-    <cfRule type="containsText" dxfId="399" priority="349" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="395" priority="349" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C104)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C105">
-    <cfRule type="containsText" dxfId="398" priority="346" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="394" priority="346" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C105)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="397" priority="347" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="393" priority="347" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C105)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="396" priority="348" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="392" priority="348" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C105)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C107:C109">
-    <cfRule type="containsText" dxfId="395" priority="337" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="391" priority="337" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C107)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C106">
-    <cfRule type="containsText" dxfId="394" priority="341" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="390" priority="341" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C106)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C106">
-    <cfRule type="containsText" dxfId="393" priority="342" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="389" priority="342" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C106)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="392" priority="343" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="388" priority="343" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C106)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="391" priority="344" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="387" priority="344" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C106)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C288">
-    <cfRule type="containsText" dxfId="390" priority="309" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="386" priority="309" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C288)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C107:C109">
-    <cfRule type="containsText" dxfId="389" priority="338" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="385" priority="338" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="388" priority="339" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="384" priority="339" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="387" priority="340" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="383" priority="340" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C107)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C292">
-    <cfRule type="containsText" dxfId="386" priority="334" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="382" priority="334" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C292)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="385" priority="335" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="381" priority="335" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C292)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="384" priority="336" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="380" priority="336" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C292)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C292">
-    <cfRule type="containsText" dxfId="383" priority="333" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="379" priority="333" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C292)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C294">
-    <cfRule type="containsText" dxfId="382" priority="326" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="378" priority="326" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C294)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="381" priority="327" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="377" priority="327" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C294)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="380" priority="328" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="376" priority="328" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C294)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C294">
-    <cfRule type="containsText" dxfId="379" priority="325" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="375" priority="325" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C294)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C295">
-    <cfRule type="containsText" dxfId="378" priority="322" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="374" priority="322" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C295)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="377" priority="323" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="373" priority="323" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C295)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="376" priority="324" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="372" priority="324" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C295)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C295">
-    <cfRule type="containsText" dxfId="375" priority="321" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="371" priority="321" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C295)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C296">
-    <cfRule type="containsText" dxfId="374" priority="318" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="370" priority="318" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C296)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="373" priority="319" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="369" priority="319" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C296)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="372" priority="320" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="368" priority="320" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C296)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C296">
-    <cfRule type="containsText" dxfId="371" priority="317" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="367" priority="317" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C296)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C297">
-    <cfRule type="containsText" dxfId="370" priority="314" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="366" priority="314" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C297)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="369" priority="315" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="365" priority="315" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C297)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="368" priority="316" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="364" priority="316" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C297)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C297">
-    <cfRule type="containsText" dxfId="367" priority="313" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="363" priority="313" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C297)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C288">
-    <cfRule type="containsText" dxfId="366" priority="310" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="362" priority="310" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C288)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="365" priority="311" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="361" priority="311" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C288)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="364" priority="312" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="360" priority="312" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C288)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C113">
-    <cfRule type="containsText" dxfId="363" priority="306" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="359" priority="306" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C113)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="362" priority="307" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="358" priority="307" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C113)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="361" priority="308" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="357" priority="308" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C113)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C113">
-    <cfRule type="containsText" dxfId="360" priority="305" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="356" priority="305" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C113)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C150">
-    <cfRule type="containsText" dxfId="359" priority="298" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="355" priority="298" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C150)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="358" priority="299" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="354" priority="299" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C150)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="357" priority="300" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="353" priority="300" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C150)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C150">
-    <cfRule type="containsText" dxfId="356" priority="297" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="352" priority="297" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C150)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C151">
-    <cfRule type="containsText" dxfId="355" priority="294" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="351" priority="294" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C151)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="354" priority="295" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="350" priority="295" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C151)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="353" priority="296" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="349" priority="296" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C151)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C151">
-    <cfRule type="containsText" dxfId="352" priority="293" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="348" priority="293" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C151)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C152">
-    <cfRule type="containsText" dxfId="351" priority="290" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="347" priority="290" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C152)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="350" priority="291" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="346" priority="291" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C152)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="349" priority="292" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="345" priority="292" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C152)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C152">
-    <cfRule type="containsText" dxfId="348" priority="289" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="344" priority="289" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C152)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C153">
-    <cfRule type="containsText" dxfId="347" priority="286" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="343" priority="286" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C153)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="346" priority="287" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="342" priority="287" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C153)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="345" priority="288" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="341" priority="288" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C153)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C153">
-    <cfRule type="containsText" dxfId="344" priority="285" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="340" priority="285" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C153)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C154">
-    <cfRule type="containsText" dxfId="343" priority="282" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="339" priority="282" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C154)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="342" priority="283" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="338" priority="283" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C154)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="341" priority="284" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="337" priority="284" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C154)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C154">
-    <cfRule type="containsText" dxfId="340" priority="281" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="336" priority="281" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C154)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C155">
-    <cfRule type="containsText" dxfId="339" priority="278" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="335" priority="278" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C155)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="338" priority="279" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="334" priority="279" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C155)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="337" priority="280" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="333" priority="280" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C155)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C155">
-    <cfRule type="containsText" dxfId="336" priority="277" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="332" priority="277" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C155)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C156">
-    <cfRule type="containsText" dxfId="335" priority="274" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="331" priority="274" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C156)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="334" priority="275" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="330" priority="275" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C156)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="333" priority="276" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="329" priority="276" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C156)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C156">
-    <cfRule type="containsText" dxfId="332" priority="273" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="328" priority="273" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C156)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C157">
-    <cfRule type="containsText" dxfId="331" priority="270" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="327" priority="270" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C157)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="330" priority="271" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="326" priority="271" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C157)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="329" priority="272" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="325" priority="272" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C157)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C157">
-    <cfRule type="containsText" dxfId="328" priority="269" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="324" priority="269" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C157)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C158">
-    <cfRule type="containsText" dxfId="327" priority="266" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="323" priority="266" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C158)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="326" priority="267" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="322" priority="267" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C158)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="325" priority="268" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="321" priority="268" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C158)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C158">
-    <cfRule type="containsText" dxfId="324" priority="265" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="320" priority="265" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C158)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C159">
-    <cfRule type="containsText" dxfId="323" priority="262" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="319" priority="262" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C159)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="322" priority="263" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="318" priority="263" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C159)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="321" priority="264" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="317" priority="264" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C159)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C159">
-    <cfRule type="containsText" dxfId="320" priority="261" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="316" priority="261" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C159)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C160">
-    <cfRule type="containsText" dxfId="319" priority="258" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="315" priority="258" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C160)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="318" priority="259" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="314" priority="259" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C160)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="317" priority="260" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="313" priority="260" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C160)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C160">
-    <cfRule type="containsText" dxfId="316" priority="257" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="312" priority="257" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C160)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C161">
-    <cfRule type="containsText" dxfId="315" priority="254" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="311" priority="254" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C161)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="314" priority="255" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="310" priority="255" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C161)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="313" priority="256" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="309" priority="256" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C161)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C161">
-    <cfRule type="containsText" dxfId="312" priority="253" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="308" priority="253" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C161)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C162">
-    <cfRule type="containsText" dxfId="311" priority="250" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="307" priority="250" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C162)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="310" priority="251" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="306" priority="251" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C162)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="309" priority="252" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="305" priority="252" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C162)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C162">
-    <cfRule type="containsText" dxfId="308" priority="249" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="304" priority="249" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C162)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C163">
-    <cfRule type="containsText" dxfId="307" priority="246" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="303" priority="246" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C163)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="306" priority="247" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="302" priority="247" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C163)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="305" priority="248" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="301" priority="248" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C163)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C163">
-    <cfRule type="containsText" dxfId="304" priority="245" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="300" priority="245" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C163)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C164">
-    <cfRule type="containsText" dxfId="303" priority="242" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="299" priority="242" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C164)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="302" priority="243" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="298" priority="243" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C164)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="301" priority="244" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="297" priority="244" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C164)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C164">
-    <cfRule type="containsText" dxfId="300" priority="241" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="296" priority="241" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C164)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C165">
-    <cfRule type="containsText" dxfId="299" priority="238" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="295" priority="238" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C165)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="298" priority="239" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="294" priority="239" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C165)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="297" priority="240" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="293" priority="240" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C165)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C165">
-    <cfRule type="containsText" dxfId="296" priority="237" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="292" priority="237" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C165)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C166">
-    <cfRule type="containsText" dxfId="295" priority="234" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="291" priority="234" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C166)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="294" priority="235" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="290" priority="235" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C166)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="293" priority="236" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="289" priority="236" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C166)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C166">
-    <cfRule type="containsText" dxfId="292" priority="233" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="288" priority="233" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C166)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C167">
-    <cfRule type="containsText" dxfId="291" priority="230" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="287" priority="230" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C167)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="290" priority="231" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="286" priority="231" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C167)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="289" priority="232" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="285" priority="232" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C167)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C167">
-    <cfRule type="containsText" dxfId="288" priority="229" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="284" priority="229" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C167)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C168:C170">
-    <cfRule type="containsText" dxfId="287" priority="226" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="283" priority="226" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C168)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="286" priority="227" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="282" priority="227" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C168)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="285" priority="228" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="281" priority="228" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C168)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C168:C170">
-    <cfRule type="containsText" dxfId="284" priority="225" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="280" priority="225" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C168)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C299">
-    <cfRule type="containsText" dxfId="283" priority="218" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="279" priority="218" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C299)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="282" priority="219" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="278" priority="219" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C299)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="281" priority="220" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="277" priority="220" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C299)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C299">
-    <cfRule type="containsText" dxfId="280" priority="217" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="276" priority="217" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C299)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C86">
-    <cfRule type="containsText" dxfId="279" priority="206" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="275" priority="206" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="278" priority="207" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="274" priority="207" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="277" priority="208" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="273" priority="208" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C86)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C86">
-    <cfRule type="containsText" dxfId="276" priority="205" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="272" priority="205" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C86)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="275" priority="194" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="271" priority="194" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="274" priority="195" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="270" priority="195" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="273" priority="196" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="269" priority="196" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="272" priority="193" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="268" priority="193" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C75">
-    <cfRule type="containsText" dxfId="271" priority="182" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="267" priority="182" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="270" priority="183" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="266" priority="183" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="269" priority="184" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="265" priority="184" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C75">
-    <cfRule type="containsText" dxfId="268" priority="181" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="264" priority="181" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74">
-    <cfRule type="containsText" dxfId="267" priority="186" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="263" priority="186" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C74)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="266" priority="187" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="262" priority="187" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C74)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="265" priority="188" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="261" priority="188" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74">
-    <cfRule type="containsText" dxfId="264" priority="185" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="260" priority="185" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51:C52">
-    <cfRule type="containsText" dxfId="263" priority="190" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="259" priority="190" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="262" priority="191" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="258" priority="191" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="261" priority="192" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="257" priority="192" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51:C52">
-    <cfRule type="containsText" dxfId="260" priority="189" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="256" priority="189" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C97">
-    <cfRule type="containsText" dxfId="259" priority="174" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="255" priority="174" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C97)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="258" priority="175" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="254" priority="175" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C97)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="257" priority="176" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="253" priority="176" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C97)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C97">
-    <cfRule type="containsText" dxfId="256" priority="173" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="252" priority="173" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C97)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="255" priority="170" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="251" priority="170" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="254" priority="171" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="250" priority="171" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="253" priority="172" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="249" priority="172" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="252" priority="169" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="248" priority="169" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="containsText" dxfId="251" priority="166" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="247" priority="166" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="250" priority="167" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="246" priority="167" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="249" priority="168" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="245" priority="168" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="containsText" dxfId="248" priority="165" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="244" priority="165" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C49">
-    <cfRule type="containsText" dxfId="247" priority="162" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="243" priority="162" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="246" priority="163" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="242" priority="163" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="245" priority="164" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="241" priority="164" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C49">
-    <cfRule type="containsText" dxfId="244" priority="161" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="240" priority="161" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="243" priority="158" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="239" priority="158" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="242" priority="159" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="238" priority="159" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="241" priority="160" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="237" priority="160" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="240" priority="157" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="236" priority="157" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="239" priority="154" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="235" priority="154" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="238" priority="155" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="234" priority="155" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="237" priority="156" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="233" priority="156" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="236" priority="153" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="232" priority="153" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="containsText" dxfId="235" priority="150" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="231" priority="150" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="234" priority="151" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="230" priority="151" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="233" priority="152" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="229" priority="152" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="containsText" dxfId="232" priority="149" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="228" priority="149" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C230">
-    <cfRule type="containsText" dxfId="231" priority="146" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="227" priority="146" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C230)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="230" priority="147" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="226" priority="147" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C230)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="229" priority="148" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="225" priority="148" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C230)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C230">
-    <cfRule type="containsText" dxfId="228" priority="145" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="224" priority="145" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C230)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C231">
-    <cfRule type="containsText" dxfId="227" priority="142" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="223" priority="142" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C231)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="226" priority="143" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="222" priority="143" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C231)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="225" priority="144" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="221" priority="144" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C231)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C231">
-    <cfRule type="containsText" dxfId="224" priority="141" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="220" priority="141" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C231)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C232">
-    <cfRule type="containsText" dxfId="223" priority="138" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="219" priority="138" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C232)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="222" priority="139" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="218" priority="139" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C232)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="221" priority="140" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="217" priority="140" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C232)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C232">
-    <cfRule type="containsText" dxfId="220" priority="137" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="216" priority="137" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C232)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C145:C146">
-    <cfRule type="containsText" dxfId="219" priority="134" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="215" priority="134" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C145)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="218" priority="135" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="214" priority="135" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C145)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="217" priority="136" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="213" priority="136" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C145)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C145:C146">
-    <cfRule type="containsText" dxfId="216" priority="133" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="212" priority="133" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C145)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C143">
-    <cfRule type="containsText" dxfId="215" priority="122" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="211" priority="122" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C143)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="214" priority="123" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="210" priority="123" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C143)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="213" priority="124" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="209" priority="124" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C143)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C143">
-    <cfRule type="containsText" dxfId="212" priority="121" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="208" priority="121" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C143)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C138">
-    <cfRule type="containsText" dxfId="211" priority="118" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="207" priority="118" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C138)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="210" priority="119" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="206" priority="119" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C138)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="209" priority="120" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="205" priority="120" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C138)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C138">
-    <cfRule type="containsText" dxfId="208" priority="117" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="204" priority="117" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C138)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C239">
-    <cfRule type="containsText" dxfId="207" priority="110" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="203" priority="110" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C239)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="206" priority="111" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="202" priority="111" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C239)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="205" priority="112" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="201" priority="112" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C239)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C239">
-    <cfRule type="containsText" dxfId="204" priority="109" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="200" priority="109" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C239)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C241:C243">
-    <cfRule type="containsText" dxfId="203" priority="106" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="199" priority="106" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C241)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="202" priority="107" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="198" priority="107" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C241)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="201" priority="108" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="197" priority="108" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C241)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C241:C243">
-    <cfRule type="containsText" dxfId="200" priority="105" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="196" priority="105" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C241)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C238">
-    <cfRule type="containsText" dxfId="199" priority="102" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="195" priority="102" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C238)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="198" priority="103" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="194" priority="103" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C238)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="197" priority="104" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="193" priority="104" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C238)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C238">
-    <cfRule type="containsText" dxfId="196" priority="101" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="192" priority="101" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C238)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C255">
-    <cfRule type="containsText" dxfId="195" priority="98" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="191" priority="98" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C255)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="194" priority="99" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="190" priority="99" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C255)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="193" priority="100" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="189" priority="100" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C255)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C255">
-    <cfRule type="containsText" dxfId="192" priority="97" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="188" priority="97" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C255)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C256:C260">
-    <cfRule type="containsText" dxfId="191" priority="94" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="187" priority="94" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C256)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="190" priority="95" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="186" priority="95" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C256)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="189" priority="96" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="185" priority="96" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C256)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C256:C260">
-    <cfRule type="containsText" dxfId="188" priority="93" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="184" priority="93" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C256)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A254:E258">
-    <cfRule type="containsText" dxfId="187" priority="90" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="183" priority="90" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",A254)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="186" priority="91" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="182" priority="91" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",A254)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="185" priority="92" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="181" priority="92" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",A254)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A254:E258">
-    <cfRule type="containsText" dxfId="184" priority="89" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="180" priority="89" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",A254)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C248">
-    <cfRule type="containsText" dxfId="183" priority="86" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="179" priority="86" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C248)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="182" priority="87" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="178" priority="87" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C248)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="181" priority="88" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="177" priority="88" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C248)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C248">
-    <cfRule type="containsText" dxfId="180" priority="85" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="176" priority="85" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C248)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C247">
-    <cfRule type="containsText" dxfId="179" priority="78" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="175" priority="78" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C247)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="178" priority="79" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="174" priority="79" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C247)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="177" priority="80" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="173" priority="80" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C247)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C247">
-    <cfRule type="containsText" dxfId="176" priority="77" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="172" priority="77" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C247)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C205">
-    <cfRule type="containsText" dxfId="175" priority="74" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="171" priority="74" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C205)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="174" priority="75" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="170" priority="75" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C205)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="173" priority="76" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="169" priority="76" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C205)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C205">
-    <cfRule type="containsText" dxfId="172" priority="73" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="168" priority="73" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C205)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C301">
-    <cfRule type="containsText" dxfId="171" priority="62" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="167" priority="62" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C301)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="170" priority="63" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="166" priority="63" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C301)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="169" priority="64" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="165" priority="64" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C301)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C301">
-    <cfRule type="containsText" dxfId="168" priority="61" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="164" priority="61" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C301)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C305">
-    <cfRule type="containsText" dxfId="167" priority="54" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="163" priority="54" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C305)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="166" priority="55" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="162" priority="55" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C305)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="165" priority="56" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="161" priority="56" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C305)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C305">
-    <cfRule type="containsText" dxfId="164" priority="53" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="160" priority="53" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C305)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C302:C304">
-    <cfRule type="containsText" dxfId="163" priority="58" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="159" priority="58" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C302)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="162" priority="59" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="158" priority="59" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C302)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="161" priority="60" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="157" priority="60" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C302:C304">
-    <cfRule type="containsText" dxfId="160" priority="57" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="156" priority="57" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C267:C268">
-    <cfRule type="containsText" dxfId="159" priority="50" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="155" priority="50" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C267)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="158" priority="51" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="154" priority="51" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C267)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="157" priority="52" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="153" priority="52" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C267)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C267:C268">
-    <cfRule type="containsText" dxfId="156" priority="49" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="152" priority="49" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C267)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A264:E266">
-    <cfRule type="containsText" dxfId="155" priority="34" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="151" priority="34" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",A264)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="154" priority="35" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="150" priority="35" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",A264)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="153" priority="36" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="149" priority="36" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",A264)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A264:E266">
-    <cfRule type="containsText" dxfId="152" priority="33" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="148" priority="33" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",A264)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A272:E277">
-    <cfRule type="containsText" dxfId="151" priority="30" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="147" priority="30" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",A272)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="150" priority="31" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="146" priority="31" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",A272)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="149" priority="32" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="145" priority="32" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",A272)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A272:E277">
-    <cfRule type="containsText" dxfId="148" priority="29" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="144" priority="29" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",A272)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C95">
-    <cfRule type="containsText" dxfId="147" priority="26" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="143" priority="26" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C95)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="146" priority="27" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="142" priority="27" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C95)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="145" priority="28" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="141" priority="28" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C95)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C95">
-    <cfRule type="containsText" dxfId="144" priority="25" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="140" priority="25" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C95)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C240">
-    <cfRule type="containsText" dxfId="143" priority="22" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="139" priority="22" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C240)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="142" priority="23" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="138" priority="23" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C240)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="141" priority="24" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="137" priority="24" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C240)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C240">
-    <cfRule type="containsText" dxfId="140" priority="21" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="136" priority="21" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C240)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C282">
-    <cfRule type="containsText" dxfId="139" priority="18" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="135" priority="18" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C282)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="138" priority="19" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="134" priority="19" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C282)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="137" priority="20" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="133" priority="20" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C282)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C282">
-    <cfRule type="containsText" dxfId="136" priority="17" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="132" priority="17" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C282)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="containsText" dxfId="135" priority="14" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="131" priority="14" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="134" priority="15" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="130" priority="15" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="133" priority="16" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="129" priority="16" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="containsText" dxfId="132" priority="13" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="128" priority="13" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C293">
-    <cfRule type="containsText" dxfId="131" priority="10" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="127" priority="10" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C293)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="11" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="126" priority="11" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C293)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="12" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="125" priority="12" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C293)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C293">
-    <cfRule type="containsText" dxfId="128" priority="9" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="124" priority="9" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C293)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="containsText" dxfId="127" priority="2" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="123" priority="2" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C53)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="3" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="122" priority="3" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C53)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="125" priority="4" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="121" priority="4" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="containsText" dxfId="124" priority="1" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="120" priority="1" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C53)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12550,8 +12525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="A122" sqref="A122"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="52.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13223,8 +13198,12 @@
       <c r="B59" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C59" s="69"/>
-      <c r="D59" s="69"/>
+      <c r="C59" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D59" s="69" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="35" t="s">
@@ -15111,482 +15090,482 @@
     <mergeCell ref="A1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="B96">
-    <cfRule type="containsText" dxfId="123" priority="302" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="119" priority="302" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="122" priority="303" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="118" priority="303" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="304" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="117" priority="304" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B96)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B96">
-    <cfRule type="containsText" dxfId="120" priority="301" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="116" priority="301" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B96)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B40 B43:B45 B77:B91 B63:B74 B6:B14 B55:B61">
-    <cfRule type="containsText" dxfId="119" priority="318" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="115" priority="318" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="319" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="114" priority="319" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="320" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="113" priority="320" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B40 B43:B45 B77:B91 B63:B74 B6:B14 B55:B61">
-    <cfRule type="containsText" dxfId="116" priority="317" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="112" priority="317" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B93">
-    <cfRule type="containsText" dxfId="115" priority="314" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="111" priority="314" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="315" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="110" priority="315" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="113" priority="316" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="109" priority="316" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B93)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B93">
-    <cfRule type="containsText" dxfId="112" priority="313" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="108" priority="313" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B93)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B95">
-    <cfRule type="containsText" dxfId="111" priority="305" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="107" priority="305" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B95)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B94">
-    <cfRule type="containsText" dxfId="110" priority="310" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="106" priority="310" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B94)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="311" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="105" priority="311" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B94)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="312" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="104" priority="312" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B94)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B94">
-    <cfRule type="containsText" dxfId="107" priority="309" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="103" priority="309" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B94)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B95">
-    <cfRule type="containsText" dxfId="106" priority="306" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="102" priority="306" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B95)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="307" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="101" priority="307" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B95)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="308" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="100" priority="308" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B95)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B209">
-    <cfRule type="containsText" dxfId="103" priority="289" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="99" priority="289" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B209)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B209">
-    <cfRule type="containsText" dxfId="102" priority="290" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="98" priority="290" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B209)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="101" priority="291" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="97" priority="291" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B209)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="292" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="96" priority="292" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B209)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B210">
-    <cfRule type="containsText" dxfId="99" priority="286" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="95" priority="286" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B210)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="287" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="94" priority="287" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B210)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="288" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="93" priority="288" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B210)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B210">
-    <cfRule type="containsText" dxfId="96" priority="285" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="92" priority="285" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B210)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B211">
-    <cfRule type="containsText" dxfId="95" priority="282" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="91" priority="282" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B211)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="283" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="90" priority="283" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B211)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="284" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="89" priority="284" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B211)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B211">
-    <cfRule type="containsText" dxfId="92" priority="281" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="88" priority="281" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B211)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B212">
-    <cfRule type="containsText" dxfId="91" priority="278" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="87" priority="278" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B212)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="279" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="86" priority="279" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B212)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="280" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="85" priority="280" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B212)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B212">
-    <cfRule type="containsText" dxfId="88" priority="277" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="84" priority="277" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B212)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B213">
-    <cfRule type="containsText" dxfId="87" priority="274" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="83" priority="274" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B213)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="275" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="82" priority="275" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B213)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="276" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="81" priority="276" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B213)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B213">
-    <cfRule type="containsText" dxfId="84" priority="273" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="80" priority="273" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B213)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B215">
-    <cfRule type="containsText" dxfId="83" priority="186" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="79" priority="186" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B215)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="187" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="78" priority="187" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B215)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="188" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="77" priority="188" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B215)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B215">
-    <cfRule type="containsText" dxfId="80" priority="185" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="76" priority="185" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B215)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46:B47">
-    <cfRule type="containsText" dxfId="79" priority="178" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="75" priority="178" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="179" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="74" priority="179" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="180" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="73" priority="180" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46:B47">
-    <cfRule type="containsText" dxfId="76" priority="177" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="72" priority="177" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76">
-    <cfRule type="containsText" dxfId="75" priority="166" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="71" priority="166" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B76)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="167" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="70" priority="167" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B76)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="168" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="69" priority="168" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76">
-    <cfRule type="containsText" dxfId="72" priority="165" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="68" priority="165" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75">
-    <cfRule type="containsText" dxfId="71" priority="170" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="67" priority="170" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="171" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="66" priority="171" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="172" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="65" priority="172" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75">
-    <cfRule type="containsText" dxfId="68" priority="169" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="64" priority="169" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52:B54">
-    <cfRule type="containsText" dxfId="67" priority="174" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="63" priority="174" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="175" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="62" priority="175" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="176" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="61" priority="176" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52:B54">
-    <cfRule type="containsText" dxfId="64" priority="173" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="60" priority="173" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="containsText" dxfId="63" priority="158" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="59" priority="158" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="159" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="58" priority="159" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="160" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="57" priority="160" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="containsText" dxfId="60" priority="157" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="56" priority="157" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="containsText" dxfId="59" priority="154" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="55" priority="154" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="155" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="54" priority="155" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="156" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="53" priority="156" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="containsText" dxfId="56" priority="153" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="52" priority="153" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49:B50">
-    <cfRule type="containsText" dxfId="55" priority="150" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="51" priority="150" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="151" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="50" priority="151" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="152" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="49" priority="152" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49:B50">
-    <cfRule type="containsText" dxfId="52" priority="149" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="48" priority="149" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41">
-    <cfRule type="containsText" dxfId="51" priority="146" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="47" priority="146" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="147" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="46" priority="147" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="148" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="45" priority="148" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41">
-    <cfRule type="containsText" dxfId="48" priority="145" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="44" priority="145" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="containsText" dxfId="47" priority="142" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="43" priority="142" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B42)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="143" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="42" priority="143" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B42)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="144" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="41" priority="144" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="containsText" dxfId="44" priority="141" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="40" priority="141" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51">
-    <cfRule type="containsText" dxfId="43" priority="138" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="39" priority="138" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="139" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="38" priority="139" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="140" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="37" priority="140" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51">
-    <cfRule type="containsText" dxfId="40" priority="137" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="36" priority="137" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B217">
-    <cfRule type="containsText" dxfId="39" priority="74" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="35" priority="74" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B217)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="75" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="34" priority="75" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B217)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="76" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="33" priority="76" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B217)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B217">
-    <cfRule type="containsText" dxfId="36" priority="73" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="32" priority="73" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B217)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B223">
-    <cfRule type="containsText" dxfId="35" priority="66" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="31" priority="66" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B223)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="67" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="30" priority="67" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B223)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="68" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="29" priority="68" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B223)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B223">
-    <cfRule type="containsText" dxfId="32" priority="65" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="28" priority="65" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B223)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B218:B219 B222">
-    <cfRule type="containsText" dxfId="31" priority="70" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="27" priority="70" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B218)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="71" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="26" priority="71" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B218)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="72" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="25" priority="72" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B218)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B218:B219 B222">
-    <cfRule type="containsText" dxfId="28" priority="69" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="24" priority="69" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B218)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B92">
-    <cfRule type="containsText" dxfId="27" priority="50" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="23" priority="50" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B92)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="51" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="22" priority="51" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B92)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="52" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="21" priority="52" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B92)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B92">
-    <cfRule type="containsText" dxfId="24" priority="49" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="20" priority="49" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B92)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B97:B111 B145:B208 B113:B143">
-    <cfRule type="containsText" dxfId="23" priority="18" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="19" priority="18" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B97)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="19" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B97)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="20" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="17" priority="20" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B97)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B97:B111 B145:B208 B113:B143">
-    <cfRule type="containsText" dxfId="20" priority="17" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B97)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B144">
-    <cfRule type="containsText" dxfId="19" priority="14" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="15" priority="14" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B144)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="15" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B144)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="13" priority="16" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B144)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B144">
-    <cfRule type="containsText" dxfId="16" priority="13" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B144)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62">
-    <cfRule type="containsText" dxfId="15" priority="10" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="11" priority="10" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B62)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="11" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B62)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="12" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62">
-    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B220:B221">
-    <cfRule type="containsText" dxfId="11" priority="6" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="7" priority="6" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B220)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B220)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="5" priority="8" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B220)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B220:B221">
-    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B220)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B112">
-    <cfRule type="containsText" dxfId="7" priority="2" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="3" priority="2" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B112)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B112)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B112">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B112)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Creation of Dump tables & expanding games config for dump
</commit_message>
<xml_diff>
--- a/Technical documentation/AL table analysis.xlsx
+++ b/Technical documentation/AL table analysis.xlsx
@@ -22,7 +22,7 @@
     <sheet name="Menu Structure" sheetId="7" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Checklist!$A$5:$C$226</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Checklist!$A$5:$C$228</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Table overview'!$A$81:$E$81</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -1143,7 +1143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1921" uniqueCount="632">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1937" uniqueCount="640">
   <si>
     <t>Table name</t>
   </si>
@@ -3042,6 +3042,30 @@
   </si>
   <si>
     <t>Deleted using script nr 247</t>
+  </si>
+  <si>
+    <t>media_type</t>
+  </si>
+  <si>
+    <t>Created using DB script nr 251</t>
+  </si>
+  <si>
+    <t>Created using DB script nr 250</t>
+  </si>
+  <si>
+    <t>Created using DB script nr 253</t>
+  </si>
+  <si>
+    <t>media_scan_type</t>
+  </si>
+  <si>
+    <t>Created using DB script nr 255</t>
+  </si>
+  <si>
+    <t>Created using DB script 256</t>
+  </si>
+  <si>
+    <t>Created using DB script 257</t>
   </si>
 </sst>
 </file>
@@ -3656,7 +3680,35 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="408">
+  <dxfs count="412">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC2E49C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFDB69"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5757"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -11367,1154 +11419,1154 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C82:C85 C281 C289:C291 C98:C99 C76:C78 C54:C73 C4:C11 C87:C94 C42:C44 C181 C114:C115 C249:C250 C118:C119 C96 C283:C287 C27:C39 C13:C25">
-    <cfRule type="containsText" dxfId="407" priority="358" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="411" priority="358" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="406" priority="359" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="410" priority="359" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="405" priority="360" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="409" priority="360" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C85 C281 C289:C291 C98:C99 C76:C78 C54:C73 C4:C11 C87:C94 C42:C44 C181 C114:C115 C249:C250 C118:C119 C96 C283:C287 C27:C39 C13:C25">
-    <cfRule type="containsText" dxfId="404" priority="357" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="408" priority="357" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C103">
-    <cfRule type="containsText" dxfId="403" priority="354" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="407" priority="354" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C103)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="402" priority="355" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="406" priority="355" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C103)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="401" priority="356" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="405" priority="356" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C103)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C103">
-    <cfRule type="containsText" dxfId="400" priority="353" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="404" priority="353" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C103)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C105">
-    <cfRule type="containsText" dxfId="399" priority="345" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="403" priority="345" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C105)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C104">
-    <cfRule type="containsText" dxfId="398" priority="350" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="402" priority="350" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C104)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="397" priority="351" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="401" priority="351" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C104)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="396" priority="352" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="400" priority="352" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C104)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C104">
-    <cfRule type="containsText" dxfId="395" priority="349" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="399" priority="349" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C104)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C105">
-    <cfRule type="containsText" dxfId="394" priority="346" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="398" priority="346" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C105)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="393" priority="347" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="397" priority="347" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C105)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="392" priority="348" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="396" priority="348" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C105)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C107:C109">
-    <cfRule type="containsText" dxfId="391" priority="337" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="395" priority="337" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C107)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C106">
-    <cfRule type="containsText" dxfId="390" priority="341" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="394" priority="341" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C106)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C106">
-    <cfRule type="containsText" dxfId="389" priority="342" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="393" priority="342" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C106)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="388" priority="343" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="392" priority="343" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C106)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="387" priority="344" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="391" priority="344" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C106)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C288">
-    <cfRule type="containsText" dxfId="386" priority="309" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="390" priority="309" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C288)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C107:C109">
-    <cfRule type="containsText" dxfId="385" priority="338" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="389" priority="338" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="384" priority="339" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="388" priority="339" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="383" priority="340" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="387" priority="340" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C107)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C292">
-    <cfRule type="containsText" dxfId="382" priority="334" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="386" priority="334" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C292)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="381" priority="335" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="385" priority="335" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C292)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="380" priority="336" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="384" priority="336" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C292)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C292">
-    <cfRule type="containsText" dxfId="379" priority="333" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="383" priority="333" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C292)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C294">
-    <cfRule type="containsText" dxfId="378" priority="326" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="382" priority="326" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C294)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="377" priority="327" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="381" priority="327" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C294)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="376" priority="328" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="380" priority="328" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C294)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C294">
-    <cfRule type="containsText" dxfId="375" priority="325" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="379" priority="325" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C294)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C295">
-    <cfRule type="containsText" dxfId="374" priority="322" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="378" priority="322" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C295)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="373" priority="323" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="377" priority="323" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C295)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="372" priority="324" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="376" priority="324" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C295)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C295">
-    <cfRule type="containsText" dxfId="371" priority="321" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="375" priority="321" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C295)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C296">
-    <cfRule type="containsText" dxfId="370" priority="318" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="374" priority="318" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C296)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="369" priority="319" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="373" priority="319" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C296)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="368" priority="320" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="372" priority="320" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C296)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C296">
-    <cfRule type="containsText" dxfId="367" priority="317" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="371" priority="317" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C296)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C297">
-    <cfRule type="containsText" dxfId="366" priority="314" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="370" priority="314" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C297)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="365" priority="315" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="369" priority="315" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C297)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="364" priority="316" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="368" priority="316" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C297)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C297">
-    <cfRule type="containsText" dxfId="363" priority="313" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="367" priority="313" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C297)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C288">
-    <cfRule type="containsText" dxfId="362" priority="310" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="366" priority="310" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C288)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="361" priority="311" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="365" priority="311" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C288)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="360" priority="312" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="364" priority="312" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C288)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C113">
-    <cfRule type="containsText" dxfId="359" priority="306" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="363" priority="306" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C113)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="358" priority="307" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="362" priority="307" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C113)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="357" priority="308" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="361" priority="308" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C113)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C113">
-    <cfRule type="containsText" dxfId="356" priority="305" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="360" priority="305" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C113)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C150">
-    <cfRule type="containsText" dxfId="355" priority="298" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="359" priority="298" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C150)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="354" priority="299" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="358" priority="299" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C150)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="353" priority="300" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="357" priority="300" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C150)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C150">
-    <cfRule type="containsText" dxfId="352" priority="297" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="356" priority="297" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C150)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C151">
-    <cfRule type="containsText" dxfId="351" priority="294" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="355" priority="294" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C151)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="350" priority="295" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="354" priority="295" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C151)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="349" priority="296" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="353" priority="296" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C151)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C151">
-    <cfRule type="containsText" dxfId="348" priority="293" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="352" priority="293" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C151)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C152">
-    <cfRule type="containsText" dxfId="347" priority="290" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="351" priority="290" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C152)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="346" priority="291" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="350" priority="291" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C152)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="345" priority="292" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="349" priority="292" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C152)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C152">
-    <cfRule type="containsText" dxfId="344" priority="289" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="348" priority="289" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C152)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C153">
-    <cfRule type="containsText" dxfId="343" priority="286" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="347" priority="286" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C153)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="342" priority="287" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="346" priority="287" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C153)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="341" priority="288" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="345" priority="288" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C153)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C153">
-    <cfRule type="containsText" dxfId="340" priority="285" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="344" priority="285" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C153)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C154">
-    <cfRule type="containsText" dxfId="339" priority="282" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="343" priority="282" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C154)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="338" priority="283" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="342" priority="283" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C154)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="337" priority="284" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="341" priority="284" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C154)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C154">
-    <cfRule type="containsText" dxfId="336" priority="281" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="340" priority="281" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C154)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C155">
-    <cfRule type="containsText" dxfId="335" priority="278" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="339" priority="278" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C155)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="334" priority="279" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="338" priority="279" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C155)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="333" priority="280" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="337" priority="280" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C155)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C155">
-    <cfRule type="containsText" dxfId="332" priority="277" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="336" priority="277" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C155)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C156">
-    <cfRule type="containsText" dxfId="331" priority="274" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="335" priority="274" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C156)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="330" priority="275" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="334" priority="275" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C156)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="329" priority="276" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="333" priority="276" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C156)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C156">
-    <cfRule type="containsText" dxfId="328" priority="273" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="332" priority="273" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C156)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C157">
-    <cfRule type="containsText" dxfId="327" priority="270" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="331" priority="270" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C157)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="326" priority="271" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="330" priority="271" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C157)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="325" priority="272" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="329" priority="272" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C157)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C157">
-    <cfRule type="containsText" dxfId="324" priority="269" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="328" priority="269" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C157)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C158">
-    <cfRule type="containsText" dxfId="323" priority="266" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="327" priority="266" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C158)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="322" priority="267" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="326" priority="267" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C158)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="321" priority="268" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="325" priority="268" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C158)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C158">
-    <cfRule type="containsText" dxfId="320" priority="265" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="324" priority="265" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C158)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C159">
-    <cfRule type="containsText" dxfId="319" priority="262" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="323" priority="262" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C159)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="318" priority="263" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="322" priority="263" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C159)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="317" priority="264" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="321" priority="264" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C159)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C159">
-    <cfRule type="containsText" dxfId="316" priority="261" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="320" priority="261" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C159)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C160">
-    <cfRule type="containsText" dxfId="315" priority="258" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="319" priority="258" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C160)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="314" priority="259" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="318" priority="259" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C160)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="313" priority="260" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="317" priority="260" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C160)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C160">
-    <cfRule type="containsText" dxfId="312" priority="257" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="316" priority="257" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C160)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C161">
-    <cfRule type="containsText" dxfId="311" priority="254" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="315" priority="254" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C161)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="310" priority="255" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="314" priority="255" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C161)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="309" priority="256" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="313" priority="256" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C161)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C161">
-    <cfRule type="containsText" dxfId="308" priority="253" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="312" priority="253" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C161)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C162">
-    <cfRule type="containsText" dxfId="307" priority="250" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="311" priority="250" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C162)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="306" priority="251" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="310" priority="251" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C162)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="305" priority="252" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="309" priority="252" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C162)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C162">
-    <cfRule type="containsText" dxfId="304" priority="249" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="308" priority="249" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C162)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C163">
-    <cfRule type="containsText" dxfId="303" priority="246" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="307" priority="246" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C163)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="302" priority="247" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="306" priority="247" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C163)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="301" priority="248" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="305" priority="248" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C163)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C163">
-    <cfRule type="containsText" dxfId="300" priority="245" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="304" priority="245" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C163)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C164">
-    <cfRule type="containsText" dxfId="299" priority="242" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="303" priority="242" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C164)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="298" priority="243" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="302" priority="243" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C164)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="297" priority="244" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="301" priority="244" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C164)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C164">
-    <cfRule type="containsText" dxfId="296" priority="241" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="300" priority="241" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C164)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C165">
-    <cfRule type="containsText" dxfId="295" priority="238" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="299" priority="238" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C165)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="294" priority="239" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="298" priority="239" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C165)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="293" priority="240" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="297" priority="240" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C165)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C165">
-    <cfRule type="containsText" dxfId="292" priority="237" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="296" priority="237" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C165)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C166">
-    <cfRule type="containsText" dxfId="291" priority="234" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="295" priority="234" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C166)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="290" priority="235" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="294" priority="235" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C166)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="289" priority="236" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="293" priority="236" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C166)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C166">
-    <cfRule type="containsText" dxfId="288" priority="233" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="292" priority="233" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C166)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C167">
-    <cfRule type="containsText" dxfId="287" priority="230" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="291" priority="230" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C167)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="286" priority="231" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="290" priority="231" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C167)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="285" priority="232" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="289" priority="232" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C167)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C167">
-    <cfRule type="containsText" dxfId="284" priority="229" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="288" priority="229" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C167)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C168:C170">
-    <cfRule type="containsText" dxfId="283" priority="226" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="287" priority="226" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C168)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="282" priority="227" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="286" priority="227" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C168)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="281" priority="228" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="285" priority="228" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C168)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C168:C170">
-    <cfRule type="containsText" dxfId="280" priority="225" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="284" priority="225" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C168)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C299">
-    <cfRule type="containsText" dxfId="279" priority="218" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="283" priority="218" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C299)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="278" priority="219" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="282" priority="219" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C299)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="277" priority="220" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="281" priority="220" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C299)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C299">
-    <cfRule type="containsText" dxfId="276" priority="217" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="280" priority="217" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C299)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C86">
-    <cfRule type="containsText" dxfId="275" priority="206" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="279" priority="206" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="274" priority="207" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="278" priority="207" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="273" priority="208" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="277" priority="208" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C86)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C86">
-    <cfRule type="containsText" dxfId="272" priority="205" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="276" priority="205" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C86)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="271" priority="194" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="275" priority="194" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="270" priority="195" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="274" priority="195" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="269" priority="196" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="273" priority="196" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="268" priority="193" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="272" priority="193" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C75">
-    <cfRule type="containsText" dxfId="267" priority="182" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="271" priority="182" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="266" priority="183" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="270" priority="183" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="265" priority="184" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="269" priority="184" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C75">
-    <cfRule type="containsText" dxfId="264" priority="181" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="268" priority="181" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74">
-    <cfRule type="containsText" dxfId="263" priority="186" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="267" priority="186" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C74)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="262" priority="187" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="266" priority="187" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C74)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="261" priority="188" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="265" priority="188" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74">
-    <cfRule type="containsText" dxfId="260" priority="185" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="264" priority="185" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51:C52">
-    <cfRule type="containsText" dxfId="259" priority="190" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="263" priority="190" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="258" priority="191" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="262" priority="191" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="257" priority="192" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="261" priority="192" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51:C52">
-    <cfRule type="containsText" dxfId="256" priority="189" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="260" priority="189" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C97">
-    <cfRule type="containsText" dxfId="255" priority="174" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="259" priority="174" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C97)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="254" priority="175" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="258" priority="175" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C97)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="253" priority="176" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="257" priority="176" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C97)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C97">
-    <cfRule type="containsText" dxfId="252" priority="173" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="256" priority="173" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C97)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="251" priority="170" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="255" priority="170" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="250" priority="171" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="254" priority="171" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="249" priority="172" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="253" priority="172" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="248" priority="169" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="252" priority="169" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="containsText" dxfId="247" priority="166" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="251" priority="166" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="246" priority="167" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="250" priority="167" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="245" priority="168" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="249" priority="168" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="containsText" dxfId="244" priority="165" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="248" priority="165" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C49">
-    <cfRule type="containsText" dxfId="243" priority="162" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="247" priority="162" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="242" priority="163" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="246" priority="163" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="241" priority="164" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="245" priority="164" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C49">
-    <cfRule type="containsText" dxfId="240" priority="161" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="244" priority="161" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="239" priority="158" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="243" priority="158" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="238" priority="159" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="242" priority="159" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="237" priority="160" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="241" priority="160" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="236" priority="157" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="240" priority="157" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="235" priority="154" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="239" priority="154" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="234" priority="155" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="238" priority="155" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="233" priority="156" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="237" priority="156" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="232" priority="153" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="236" priority="153" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="containsText" dxfId="231" priority="150" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="235" priority="150" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="230" priority="151" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="234" priority="151" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="229" priority="152" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="233" priority="152" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="containsText" dxfId="228" priority="149" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="232" priority="149" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C230">
-    <cfRule type="containsText" dxfId="227" priority="146" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="231" priority="146" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C230)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="226" priority="147" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="230" priority="147" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C230)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="225" priority="148" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="229" priority="148" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C230)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C230">
-    <cfRule type="containsText" dxfId="224" priority="145" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="228" priority="145" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C230)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C231">
-    <cfRule type="containsText" dxfId="223" priority="142" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="227" priority="142" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C231)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="222" priority="143" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="226" priority="143" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C231)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="221" priority="144" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="225" priority="144" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C231)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C231">
-    <cfRule type="containsText" dxfId="220" priority="141" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="224" priority="141" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C231)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C232">
-    <cfRule type="containsText" dxfId="219" priority="138" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="223" priority="138" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C232)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="218" priority="139" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="222" priority="139" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C232)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="217" priority="140" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="221" priority="140" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C232)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C232">
-    <cfRule type="containsText" dxfId="216" priority="137" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="220" priority="137" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C232)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C145:C146">
-    <cfRule type="containsText" dxfId="215" priority="134" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="219" priority="134" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C145)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="214" priority="135" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="218" priority="135" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C145)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="213" priority="136" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="217" priority="136" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C145)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C145:C146">
-    <cfRule type="containsText" dxfId="212" priority="133" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="216" priority="133" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C145)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C143">
-    <cfRule type="containsText" dxfId="211" priority="122" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="215" priority="122" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C143)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="210" priority="123" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="214" priority="123" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C143)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="209" priority="124" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="213" priority="124" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C143)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C143">
-    <cfRule type="containsText" dxfId="208" priority="121" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="212" priority="121" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C143)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C138">
-    <cfRule type="containsText" dxfId="207" priority="118" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="211" priority="118" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C138)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="206" priority="119" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="210" priority="119" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C138)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="205" priority="120" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="209" priority="120" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C138)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C138">
-    <cfRule type="containsText" dxfId="204" priority="117" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="208" priority="117" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C138)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C239">
-    <cfRule type="containsText" dxfId="203" priority="110" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="207" priority="110" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C239)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="202" priority="111" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="206" priority="111" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C239)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="201" priority="112" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="205" priority="112" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C239)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C239">
-    <cfRule type="containsText" dxfId="200" priority="109" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="204" priority="109" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C239)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C241:C243">
-    <cfRule type="containsText" dxfId="199" priority="106" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="203" priority="106" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C241)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="198" priority="107" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="202" priority="107" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C241)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="197" priority="108" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="201" priority="108" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C241)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C241:C243">
-    <cfRule type="containsText" dxfId="196" priority="105" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="200" priority="105" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C241)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C238">
-    <cfRule type="containsText" dxfId="195" priority="102" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="199" priority="102" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C238)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="194" priority="103" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="198" priority="103" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C238)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="193" priority="104" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="197" priority="104" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C238)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C238">
-    <cfRule type="containsText" dxfId="192" priority="101" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="196" priority="101" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C238)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C255">
-    <cfRule type="containsText" dxfId="191" priority="98" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="195" priority="98" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C255)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="190" priority="99" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="194" priority="99" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C255)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="189" priority="100" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="193" priority="100" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C255)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C255">
-    <cfRule type="containsText" dxfId="188" priority="97" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="192" priority="97" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C255)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C256:C260">
-    <cfRule type="containsText" dxfId="187" priority="94" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="191" priority="94" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C256)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="186" priority="95" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="190" priority="95" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C256)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="185" priority="96" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="189" priority="96" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C256)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C256:C260">
-    <cfRule type="containsText" dxfId="184" priority="93" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="188" priority="93" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C256)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A254:E258">
-    <cfRule type="containsText" dxfId="183" priority="90" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="187" priority="90" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",A254)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="182" priority="91" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="186" priority="91" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",A254)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="181" priority="92" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="185" priority="92" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",A254)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A254:E258">
-    <cfRule type="containsText" dxfId="180" priority="89" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="184" priority="89" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",A254)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C248">
-    <cfRule type="containsText" dxfId="179" priority="86" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="183" priority="86" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C248)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="178" priority="87" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="182" priority="87" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C248)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="177" priority="88" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="181" priority="88" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C248)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C248">
-    <cfRule type="containsText" dxfId="176" priority="85" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="180" priority="85" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C248)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C247">
-    <cfRule type="containsText" dxfId="175" priority="78" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="179" priority="78" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C247)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="174" priority="79" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="178" priority="79" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C247)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="173" priority="80" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="177" priority="80" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C247)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C247">
-    <cfRule type="containsText" dxfId="172" priority="77" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="176" priority="77" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C247)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C205">
-    <cfRule type="containsText" dxfId="171" priority="74" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="175" priority="74" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C205)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="170" priority="75" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="174" priority="75" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C205)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="169" priority="76" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="173" priority="76" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C205)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C205">
-    <cfRule type="containsText" dxfId="168" priority="73" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="172" priority="73" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C205)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C301">
-    <cfRule type="containsText" dxfId="167" priority="62" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="171" priority="62" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C301)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="166" priority="63" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="170" priority="63" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C301)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="165" priority="64" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="169" priority="64" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C301)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C301">
-    <cfRule type="containsText" dxfId="164" priority="61" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="168" priority="61" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C301)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C305">
-    <cfRule type="containsText" dxfId="163" priority="54" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="167" priority="54" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C305)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="162" priority="55" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="166" priority="55" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C305)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="161" priority="56" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="165" priority="56" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C305)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C305">
-    <cfRule type="containsText" dxfId="160" priority="53" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="164" priority="53" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C305)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C302:C304">
-    <cfRule type="containsText" dxfId="159" priority="58" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="163" priority="58" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C302)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="158" priority="59" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="162" priority="59" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C302)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="157" priority="60" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="161" priority="60" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C302:C304">
-    <cfRule type="containsText" dxfId="156" priority="57" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="160" priority="57" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C267:C268">
-    <cfRule type="containsText" dxfId="155" priority="50" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="159" priority="50" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C267)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="154" priority="51" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="158" priority="51" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C267)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="153" priority="52" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="157" priority="52" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C267)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C267:C268">
-    <cfRule type="containsText" dxfId="152" priority="49" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="156" priority="49" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C267)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A264:E266">
-    <cfRule type="containsText" dxfId="151" priority="34" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="155" priority="34" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",A264)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="150" priority="35" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="154" priority="35" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",A264)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="149" priority="36" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="153" priority="36" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",A264)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A264:E266">
-    <cfRule type="containsText" dxfId="148" priority="33" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="152" priority="33" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",A264)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A272:E277">
-    <cfRule type="containsText" dxfId="147" priority="30" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="151" priority="30" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",A272)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="146" priority="31" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="150" priority="31" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",A272)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="145" priority="32" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="149" priority="32" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",A272)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A272:E277">
-    <cfRule type="containsText" dxfId="144" priority="29" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="148" priority="29" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",A272)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C95">
-    <cfRule type="containsText" dxfId="143" priority="26" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="147" priority="26" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C95)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="142" priority="27" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="146" priority="27" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C95)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="141" priority="28" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="145" priority="28" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C95)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C95">
-    <cfRule type="containsText" dxfId="140" priority="25" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="144" priority="25" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C95)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C240">
-    <cfRule type="containsText" dxfId="139" priority="22" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="143" priority="22" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C240)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="138" priority="23" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="142" priority="23" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C240)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="137" priority="24" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="141" priority="24" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C240)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C240">
-    <cfRule type="containsText" dxfId="136" priority="21" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="140" priority="21" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C240)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C282">
-    <cfRule type="containsText" dxfId="135" priority="18" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="139" priority="18" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C282)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="134" priority="19" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="138" priority="19" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C282)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="133" priority="20" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="137" priority="20" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C282)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C282">
-    <cfRule type="containsText" dxfId="132" priority="17" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="136" priority="17" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C282)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="containsText" dxfId="131" priority="14" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="135" priority="14" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="15" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="134" priority="15" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="16" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="133" priority="16" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="containsText" dxfId="128" priority="13" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="132" priority="13" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C293">
-    <cfRule type="containsText" dxfId="127" priority="10" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="131" priority="10" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C293)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="11" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="130" priority="11" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C293)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="125" priority="12" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="129" priority="12" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C293)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C293">
-    <cfRule type="containsText" dxfId="124" priority="9" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="128" priority="9" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C293)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="containsText" dxfId="123" priority="2" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="127" priority="2" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C53)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="122" priority="3" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="126" priority="3" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C53)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="4" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="125" priority="4" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="containsText" dxfId="120" priority="1" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="124" priority="1" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C53)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12534,10 +12586,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P226"/>
+  <dimension ref="A1:P228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="D132" sqref="D132"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="52.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13161,8 +13213,12 @@
       <c r="B55" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C55" s="69"/>
-      <c r="D55" s="69"/>
+      <c r="C55" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D55" s="69" t="s">
+        <v>638</v>
+      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="26" t="s">
@@ -13171,8 +13227,12 @@
       <c r="B56" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C56" s="69"/>
-      <c r="D56" s="69"/>
+      <c r="C56" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D56" s="69" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="57" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="35" t="s">
@@ -14343,22 +14403,30 @@
       <c r="B152" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C152" s="69"/>
-      <c r="D152" s="69"/>
+      <c r="C152" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D152" s="69" t="s">
+        <v>633</v>
+      </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="35" t="s">
-        <v>115</v>
+        <v>632</v>
       </c>
       <c r="B153" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C153" s="69"/>
-      <c r="D153" s="69"/>
+      <c r="C153" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D153" s="69" t="s">
+        <v>634</v>
+      </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="35" t="s">
-        <v>65</v>
+        <v>115</v>
       </c>
       <c r="B154" s="42" t="s">
         <v>16</v>
@@ -14367,12 +14435,12 @@
         <v>550</v>
       </c>
       <c r="D154" s="69" t="s">
-        <v>617</v>
+        <v>637</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="35" t="s">
-        <v>629</v>
+        <v>636</v>
       </c>
       <c r="B155" s="42" t="s">
         <v>16</v>
@@ -14381,42 +14449,50 @@
         <v>550</v>
       </c>
       <c r="D155" s="69" t="s">
-        <v>630</v>
+        <v>635</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="35" t="s">
-        <v>386</v>
+        <v>65</v>
       </c>
       <c r="B156" s="42" t="s">
-        <v>204</v>
-      </c>
-      <c r="C156" s="69"/>
-      <c r="D156" s="69"/>
+        <v>16</v>
+      </c>
+      <c r="C156" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D156" s="69" t="s">
+        <v>617</v>
+      </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="35" t="s">
-        <v>402</v>
+        <v>629</v>
       </c>
       <c r="B157" s="42" t="s">
-        <v>204</v>
-      </c>
-      <c r="C157" s="69"/>
-      <c r="D157" s="69"/>
+        <v>16</v>
+      </c>
+      <c r="C157" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D157" s="69" t="s">
+        <v>630</v>
+      </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="35" t="s">
-        <v>398</v>
+        <v>386</v>
       </c>
       <c r="B158" s="42" t="s">
-        <v>3</v>
+        <v>204</v>
       </c>
       <c r="C158" s="69"/>
       <c r="D158" s="69"/>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="35" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="B159" s="42" t="s">
         <v>204</v>
@@ -14426,17 +14502,17 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="35" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B160" s="42" t="s">
-        <v>204</v>
+        <v>3</v>
       </c>
       <c r="C160" s="69"/>
       <c r="D160" s="69"/>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="35" t="s">
-        <v>387</v>
+        <v>400</v>
       </c>
       <c r="B161" s="42" t="s">
         <v>204</v>
@@ -14446,7 +14522,7 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="35" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="B162" s="42" t="s">
         <v>204</v>
@@ -14456,7 +14532,7 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="35" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="B163" s="42" t="s">
         <v>204</v>
@@ -14466,7 +14542,7 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="35" t="s">
-        <v>392</v>
+        <v>404</v>
       </c>
       <c r="B164" s="42" t="s">
         <v>204</v>
@@ -14476,7 +14552,7 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="35" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B165" s="42" t="s">
         <v>204</v>
@@ -14486,7 +14562,7 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="35" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="B166" s="42" t="s">
         <v>204</v>
@@ -14496,7 +14572,7 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="35" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B167" s="42" t="s">
         <v>204</v>
@@ -14506,7 +14582,7 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="35" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="B168" s="42" t="s">
         <v>204</v>
@@ -14516,7 +14592,7 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="35" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="B169" s="42" t="s">
         <v>204</v>
@@ -14526,7 +14602,7 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="35" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B170" s="42" t="s">
         <v>204</v>
@@ -14536,7 +14612,7 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="35" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
       <c r="B171" s="42" t="s">
         <v>204</v>
@@ -14546,7 +14622,7 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="35" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="B172" s="42" t="s">
         <v>204</v>
@@ -14556,7 +14632,7 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="35" t="s">
-        <v>385</v>
+        <v>403</v>
       </c>
       <c r="B173" s="42" t="s">
         <v>204</v>
@@ -14566,17 +14642,17 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="35" t="s">
-        <v>430</v>
+        <v>384</v>
       </c>
       <c r="B174" s="42" t="s">
-        <v>3</v>
+        <v>204</v>
       </c>
       <c r="C174" s="69"/>
       <c r="D174" s="69"/>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="35" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="B175" s="42" t="s">
         <v>204</v>
@@ -14586,17 +14662,17 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="35" t="s">
-        <v>383</v>
+        <v>430</v>
       </c>
       <c r="B176" s="42" t="s">
-        <v>204</v>
+        <v>3</v>
       </c>
       <c r="C176" s="69"/>
       <c r="D176" s="69"/>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="35" t="s">
-        <v>397</v>
+        <v>382</v>
       </c>
       <c r="B177" s="42" t="s">
         <v>204</v>
@@ -14606,7 +14682,7 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="35" t="s">
-        <v>433</v>
+        <v>383</v>
       </c>
       <c r="B178" s="42" t="s">
         <v>204</v>
@@ -14616,7 +14692,7 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="35" t="s">
-        <v>436</v>
+        <v>397</v>
       </c>
       <c r="B179" s="42" t="s">
         <v>204</v>
@@ -14626,7 +14702,7 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="35" t="s">
-        <v>524</v>
+        <v>433</v>
       </c>
       <c r="B180" s="42" t="s">
         <v>204</v>
@@ -14636,7 +14712,7 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="35" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B181" s="42" t="s">
         <v>204</v>
@@ -14646,7 +14722,7 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="35" t="s">
-        <v>442</v>
+        <v>524</v>
       </c>
       <c r="B182" s="42" t="s">
         <v>204</v>
@@ -14656,7 +14732,7 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="35" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B183" s="42" t="s">
         <v>204</v>
@@ -14666,7 +14742,7 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="35" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B184" s="42" t="s">
         <v>204</v>
@@ -14676,7 +14752,7 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="35" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B185" s="42" t="s">
         <v>204</v>
@@ -14686,7 +14762,7 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="35" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B186" s="42" t="s">
         <v>204</v>
@@ -14696,69 +14772,65 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="35" t="s">
-        <v>112</v>
+        <v>445</v>
       </c>
       <c r="B187" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="C187" s="69" t="s">
-        <v>589</v>
-      </c>
-      <c r="D187" s="69" t="s">
-        <v>590</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="C187" s="69"/>
+      <c r="D187" s="69"/>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="35" t="s">
-        <v>12</v>
+        <v>446</v>
       </c>
       <c r="B188" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="C188" s="69" t="s">
-        <v>550</v>
-      </c>
-      <c r="D188" s="69" t="s">
-        <v>584</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="C188" s="69"/>
+      <c r="D188" s="69"/>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="35" t="s">
-        <v>453</v>
+        <v>112</v>
       </c>
       <c r="B189" s="42" t="s">
-        <v>204</v>
-      </c>
-      <c r="C189" s="69"/>
-      <c r="D189" s="69"/>
+        <v>16</v>
+      </c>
+      <c r="C189" s="69" t="s">
+        <v>589</v>
+      </c>
+      <c r="D189" s="69" t="s">
+        <v>590</v>
+      </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="35" t="s">
-        <v>455</v>
+        <v>12</v>
       </c>
       <c r="B190" s="42" t="s">
-        <v>204</v>
-      </c>
-      <c r="C190" s="69"/>
-      <c r="D190" s="69"/>
+        <v>16</v>
+      </c>
+      <c r="C190" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D190" s="69" t="s">
+        <v>584</v>
+      </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="35" t="s">
-        <v>55</v>
+        <v>453</v>
       </c>
       <c r="B191" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="C191" s="69" t="s">
-        <v>550</v>
-      </c>
-      <c r="D191" s="69" t="s">
-        <v>556</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="C191" s="69"/>
+      <c r="D191" s="69"/>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="35" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B192" s="42" t="s">
         <v>204</v>
@@ -14768,17 +14840,21 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="35" t="s">
-        <v>460</v>
+        <v>55</v>
       </c>
       <c r="B193" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="C193" s="69"/>
-      <c r="D193" s="69"/>
+        <v>16</v>
+      </c>
+      <c r="C193" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D193" s="69" t="s">
+        <v>556</v>
+      </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="35" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="B194" s="42" t="s">
         <v>204</v>
@@ -14788,17 +14864,17 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="35" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="B195" s="42" t="s">
-        <v>204</v>
+        <v>3</v>
       </c>
       <c r="C195" s="69"/>
       <c r="D195" s="69"/>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="35" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="B196" s="42" t="s">
         <v>204</v>
@@ -14808,7 +14884,7 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="35" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="B197" s="42" t="s">
         <v>204</v>
@@ -14818,7 +14894,7 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="35" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="B198" s="42" t="s">
         <v>204</v>
@@ -14828,7 +14904,7 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="35" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="B199" s="42" t="s">
         <v>204</v>
@@ -14838,7 +14914,7 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="35" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="B200" s="42" t="s">
         <v>204</v>
@@ -14848,7 +14924,7 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="35" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="B201" s="42" t="s">
         <v>204</v>
@@ -14858,7 +14934,7 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="35" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="B202" s="42" t="s">
         <v>204</v>
@@ -14868,7 +14944,7 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="35" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="B203" s="42" t="s">
         <v>204</v>
@@ -14878,7 +14954,7 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="35" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="B204" s="42" t="s">
         <v>204</v>
@@ -14888,7 +14964,7 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="35" t="s">
-        <v>474</v>
+        <v>485</v>
       </c>
       <c r="B205" s="42" t="s">
         <v>204</v>
@@ -14898,7 +14974,7 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="35" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B206" s="42" t="s">
         <v>204</v>
@@ -14908,7 +14984,7 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="35" t="s">
-        <v>490</v>
+        <v>474</v>
       </c>
       <c r="B207" s="42" t="s">
         <v>204</v>
@@ -14918,7 +14994,7 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="35" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="B208" s="42" t="s">
         <v>204</v>
@@ -14928,17 +15004,17 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="35" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="B209" s="42" t="s">
-        <v>3</v>
+        <v>204</v>
       </c>
       <c r="C209" s="69"/>
       <c r="D209" s="69"/>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="35" t="s">
-        <v>250</v>
+        <v>492</v>
       </c>
       <c r="B210" s="42" t="s">
         <v>204</v>
@@ -14948,41 +15024,41 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="35" t="s">
-        <v>50</v>
+        <v>494</v>
       </c>
       <c r="B211" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="C211" s="69" t="s">
-        <v>550</v>
-      </c>
-      <c r="D211" s="69" t="s">
-        <v>551</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C211" s="69"/>
+      <c r="D211" s="69"/>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="35" t="s">
-        <v>497</v>
+        <v>250</v>
       </c>
       <c r="B212" s="42" t="s">
-        <v>3</v>
+        <v>204</v>
       </c>
       <c r="C212" s="69"/>
       <c r="D212" s="69"/>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="35" t="s">
-        <v>499</v>
+        <v>50</v>
       </c>
       <c r="B213" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="C213" s="69"/>
-      <c r="D213" s="69"/>
+        <v>16</v>
+      </c>
+      <c r="C213" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="D213" s="69" t="s">
+        <v>551</v>
+      </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" s="35" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="B214" s="42" t="s">
         <v>3</v>
@@ -14992,7 +15068,7 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="35" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B215" s="42" t="s">
         <v>3</v>
@@ -15002,29 +15078,29 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="35" t="s">
-        <v>68</v>
+        <v>500</v>
       </c>
       <c r="B216" s="42" t="s">
-        <v>204</v>
+        <v>3</v>
       </c>
       <c r="C216" s="69"/>
       <c r="D216" s="69"/>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="35" t="s">
-        <v>123</v>
+        <v>501</v>
       </c>
       <c r="B217" s="42" t="s">
-        <v>204</v>
+        <v>3</v>
       </c>
       <c r="C217" s="69"/>
       <c r="D217" s="69"/>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="35" t="s">
-        <v>503</v>
-      </c>
-      <c r="B218" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="B218" s="42" t="s">
         <v>204</v>
       </c>
       <c r="C218" s="69"/>
@@ -15032,9 +15108,9 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="35" t="s">
-        <v>504</v>
-      </c>
-      <c r="B219" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="B219" s="42" t="s">
         <v>204</v>
       </c>
       <c r="C219" s="69"/>
@@ -15042,9 +15118,9 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="35" t="s">
-        <v>507</v>
-      </c>
-      <c r="B220" s="42" t="s">
+        <v>503</v>
+      </c>
+      <c r="B220" s="38" t="s">
         <v>204</v>
       </c>
       <c r="C220" s="69"/>
@@ -15052,17 +15128,17 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" s="35" t="s">
-        <v>509</v>
-      </c>
-      <c r="B221" s="42" t="s">
-        <v>3</v>
+        <v>504</v>
+      </c>
+      <c r="B221" s="38" t="s">
+        <v>204</v>
       </c>
       <c r="C221" s="69"/>
       <c r="D221" s="69"/>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" s="35" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="B222" s="42" t="s">
         <v>204</v>
@@ -15072,17 +15148,17 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" s="35" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="B223" s="42" t="s">
-        <v>204</v>
+        <v>3</v>
       </c>
       <c r="C223" s="69"/>
       <c r="D223" s="69"/>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" s="35" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="B224" s="42" t="s">
         <v>204</v>
@@ -15092,7 +15168,7 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" s="35" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="B225" s="42" t="s">
         <v>204</v>
@@ -15101,17 +15177,37 @@
       <c r="D225" s="69"/>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A226" s="46" t="s">
+      <c r="A226" s="35" t="s">
+        <v>516</v>
+      </c>
+      <c r="B226" s="42" t="s">
+        <v>204</v>
+      </c>
+      <c r="C226" s="69"/>
+      <c r="D226" s="69"/>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A227" s="35" t="s">
+        <v>519</v>
+      </c>
+      <c r="B227" s="42" t="s">
+        <v>204</v>
+      </c>
+      <c r="C227" s="69"/>
+      <c r="D227" s="69"/>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A228" s="46" t="s">
         <v>520</v>
       </c>
-      <c r="B226" s="48" t="s">
-        <v>204</v>
-      </c>
-      <c r="C226" s="70"/>
-      <c r="D226" s="70"/>
+      <c r="B228" s="48" t="s">
+        <v>204</v>
+      </c>
+      <c r="C228" s="70"/>
+      <c r="D228" s="70"/>
     </row>
   </sheetData>
-  <autoFilter ref="A5:C226"/>
+  <autoFilter ref="A5:C228"/>
   <sortState ref="A6:E224">
     <sortCondition ref="A6"/>
   </sortState>
@@ -15119,487 +15215,503 @@
     <mergeCell ref="A1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="B96">
-    <cfRule type="containsText" dxfId="119" priority="302" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="123" priority="306" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="303" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="122" priority="307" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="304" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="121" priority="308" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B96)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B96">
-    <cfRule type="containsText" dxfId="116" priority="301" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="120" priority="305" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B96)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B40 B43:B45 B77:B91 B63:B74 B6:B14 B55:B61">
+    <cfRule type="containsText" dxfId="119" priority="322" stopIfTrue="1" operator="containsText" text="Delete">
+      <formula>NOT(ISERROR(SEARCH("Delete",B6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="118" priority="323" operator="containsText" text="Change">
+      <formula>NOT(ISERROR(SEARCH("Change",B6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="117" priority="324" operator="containsText" text="Create">
+      <formula>NOT(ISERROR(SEARCH("Create",B6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16:B40 B43:B45 B77:B91 B63:B74 B6:B14 B55:B61">
+    <cfRule type="containsText" dxfId="116" priority="321" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",B6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B93">
     <cfRule type="containsText" dxfId="115" priority="318" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B6)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Delete",B93)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="114" priority="319" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B6)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Change",B93)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="113" priority="320" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B16:B40 B43:B45 B77:B91 B63:B74 B6:B14 B55:B61">
+      <formula>NOT(ISERROR(SEARCH("Create",B93)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B93">
     <cfRule type="containsText" dxfId="112" priority="317" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B93">
-    <cfRule type="containsText" dxfId="111" priority="314" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B93)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="110" priority="315" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B93)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="316" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B93)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B93">
-    <cfRule type="containsText" dxfId="108" priority="313" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B93)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B95">
-    <cfRule type="containsText" dxfId="107" priority="305" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="111" priority="309" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B95)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B94">
+    <cfRule type="containsText" dxfId="110" priority="314" stopIfTrue="1" operator="containsText" text="Delete">
+      <formula>NOT(ISERROR(SEARCH("Delete",B94)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="109" priority="315" operator="containsText" text="Change">
+      <formula>NOT(ISERROR(SEARCH("Change",B94)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="108" priority="316" operator="containsText" text="Create">
+      <formula>NOT(ISERROR(SEARCH("Create",B94)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B94">
+    <cfRule type="containsText" dxfId="107" priority="313" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",B94)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B95">
     <cfRule type="containsText" dxfId="106" priority="310" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B94)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Delete",B95)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="105" priority="311" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B94)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Change",B95)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="104" priority="312" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B94)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B94">
-    <cfRule type="containsText" dxfId="103" priority="309" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B94)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B95">
-    <cfRule type="containsText" dxfId="102" priority="306" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B95)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="101" priority="307" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B95)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="308" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B95)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B210">
-    <cfRule type="containsText" dxfId="99" priority="289" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B210)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B210">
-    <cfRule type="containsText" dxfId="98" priority="290" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B210)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="291" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B210)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="292" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B210)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B211">
+  <conditionalFormatting sqref="B212">
+    <cfRule type="containsText" dxfId="103" priority="293" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",B212)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B212">
+    <cfRule type="containsText" dxfId="102" priority="294" stopIfTrue="1" operator="containsText" text="Delete">
+      <formula>NOT(ISERROR(SEARCH("Delete",B212)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="101" priority="295" operator="containsText" text="Change">
+      <formula>NOT(ISERROR(SEARCH("Change",B212)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="100" priority="296" operator="containsText" text="Create">
+      <formula>NOT(ISERROR(SEARCH("Create",B212)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B213">
+    <cfRule type="containsText" dxfId="99" priority="290" stopIfTrue="1" operator="containsText" text="Delete">
+      <formula>NOT(ISERROR(SEARCH("Delete",B213)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="98" priority="291" operator="containsText" text="Change">
+      <formula>NOT(ISERROR(SEARCH("Change",B213)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="97" priority="292" operator="containsText" text="Create">
+      <formula>NOT(ISERROR(SEARCH("Create",B213)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B213">
+    <cfRule type="containsText" dxfId="96" priority="289" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",B213)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B214">
     <cfRule type="containsText" dxfId="95" priority="286" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B211)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Delete",B214)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="94" priority="287" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B211)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Change",B214)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="93" priority="288" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B211)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B211">
+      <formula>NOT(ISERROR(SEARCH("Create",B214)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B214">
     <cfRule type="containsText" dxfId="92" priority="285" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B211)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B212">
+      <formula>NOT(ISERROR(SEARCH("None",B214)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B215">
     <cfRule type="containsText" dxfId="91" priority="282" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B212)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Delete",B215)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="90" priority="283" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B212)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Change",B215)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="89" priority="284" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B212)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B212">
+      <formula>NOT(ISERROR(SEARCH("Create",B215)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B215">
     <cfRule type="containsText" dxfId="88" priority="281" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B212)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B213">
+      <formula>NOT(ISERROR(SEARCH("None",B215)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B216">
     <cfRule type="containsText" dxfId="87" priority="278" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B213)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Delete",B216)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="86" priority="279" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B213)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Change",B216)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="85" priority="280" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B213)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B213">
+      <formula>NOT(ISERROR(SEARCH("Create",B216)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B216">
     <cfRule type="containsText" dxfId="84" priority="277" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B213)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B214">
-    <cfRule type="containsText" dxfId="83" priority="274" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B214)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="275" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B214)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="276" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B214)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B214">
-    <cfRule type="containsText" dxfId="80" priority="273" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B214)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B216">
-    <cfRule type="containsText" dxfId="79" priority="186" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B216)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="187" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B216)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="188" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B216)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B216">
-    <cfRule type="containsText" dxfId="76" priority="185" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B216)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B218">
+    <cfRule type="containsText" dxfId="83" priority="190" stopIfTrue="1" operator="containsText" text="Delete">
+      <formula>NOT(ISERROR(SEARCH("Delete",B218)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="82" priority="191" operator="containsText" text="Change">
+      <formula>NOT(ISERROR(SEARCH("Change",B218)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="81" priority="192" operator="containsText" text="Create">
+      <formula>NOT(ISERROR(SEARCH("Create",B218)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B218">
+    <cfRule type="containsText" dxfId="80" priority="189" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",B218)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B46:B47">
-    <cfRule type="containsText" dxfId="75" priority="178" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="79" priority="182" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="179" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="78" priority="183" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="180" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="77" priority="184" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46:B47">
-    <cfRule type="containsText" dxfId="72" priority="177" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="76" priority="181" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76">
-    <cfRule type="containsText" dxfId="71" priority="166" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="75" priority="170" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B76)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="167" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="74" priority="171" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B76)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="168" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="73" priority="172" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76">
-    <cfRule type="containsText" dxfId="68" priority="165" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="72" priority="169" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75">
-    <cfRule type="containsText" dxfId="67" priority="170" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="71" priority="174" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="171" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="70" priority="175" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="172" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="69" priority="176" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75">
-    <cfRule type="containsText" dxfId="64" priority="169" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="68" priority="173" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52:B54">
-    <cfRule type="containsText" dxfId="63" priority="174" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="67" priority="178" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="175" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="66" priority="179" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="176" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="65" priority="180" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52:B54">
-    <cfRule type="containsText" dxfId="60" priority="173" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="64" priority="177" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
+    <cfRule type="containsText" dxfId="63" priority="162" stopIfTrue="1" operator="containsText" text="Delete">
+      <formula>NOT(ISERROR(SEARCH("Delete",B48)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="62" priority="163" operator="containsText" text="Change">
+      <formula>NOT(ISERROR(SEARCH("Change",B48)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="61" priority="164" operator="containsText" text="Create">
+      <formula>NOT(ISERROR(SEARCH("Create",B48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B48">
+    <cfRule type="containsText" dxfId="60" priority="161" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",B48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15">
     <cfRule type="containsText" dxfId="59" priority="158" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B48)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Delete",B15)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="58" priority="159" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B48)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Change",B15)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="57" priority="160" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B48">
+      <formula>NOT(ISERROR(SEARCH("Create",B15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15">
     <cfRule type="containsText" dxfId="56" priority="157" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15">
+      <formula>NOT(ISERROR(SEARCH("None",B15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B49:B50">
     <cfRule type="containsText" dxfId="55" priority="154" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B15)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Delete",B49)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="54" priority="155" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B15)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Change",B49)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="53" priority="156" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15">
+      <formula>NOT(ISERROR(SEARCH("Create",B49)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B49:B50">
     <cfRule type="containsText" dxfId="52" priority="153" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B49:B50">
+      <formula>NOT(ISERROR(SEARCH("None",B49)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B41">
     <cfRule type="containsText" dxfId="51" priority="150" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B49)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Delete",B41)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="50" priority="151" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B49)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Change",B41)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="49" priority="152" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B49)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B49:B50">
+      <formula>NOT(ISERROR(SEARCH("Create",B41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B41">
     <cfRule type="containsText" dxfId="48" priority="149" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B49)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B41">
+      <formula>NOT(ISERROR(SEARCH("None",B41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B42">
     <cfRule type="containsText" dxfId="47" priority="146" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B41)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Delete",B42)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="46" priority="147" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B41)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Change",B42)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="45" priority="148" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B41)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B41">
+      <formula>NOT(ISERROR(SEARCH("Create",B42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B42">
     <cfRule type="containsText" dxfId="44" priority="145" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B41)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B42">
+      <formula>NOT(ISERROR(SEARCH("None",B42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B51">
     <cfRule type="containsText" dxfId="43" priority="142" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B42)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Delete",B51)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="42" priority="143" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B42)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Change",B51)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="41" priority="144" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B42)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B42">
+      <formula>NOT(ISERROR(SEARCH("Create",B51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B51">
     <cfRule type="containsText" dxfId="40" priority="141" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B42)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B51">
-    <cfRule type="containsText" dxfId="39" priority="138" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B51)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="139" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B51)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="140" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B51">
-    <cfRule type="containsText" dxfId="36" priority="137" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B51)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B218">
-    <cfRule type="containsText" dxfId="35" priority="74" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B218)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="75" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B218)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="76" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B218)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B218">
-    <cfRule type="containsText" dxfId="32" priority="73" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B218)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B224">
-    <cfRule type="containsText" dxfId="31" priority="66" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B224)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="67" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B224)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="68" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B224)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B224">
-    <cfRule type="containsText" dxfId="28" priority="65" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B224)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B219:B220 B223">
-    <cfRule type="containsText" dxfId="27" priority="70" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B219)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="71" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B219)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="72" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B219)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B219:B220 B223">
-    <cfRule type="containsText" dxfId="24" priority="69" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B219)))</formula>
+  <conditionalFormatting sqref="B220">
+    <cfRule type="containsText" dxfId="39" priority="78" stopIfTrue="1" operator="containsText" text="Delete">
+      <formula>NOT(ISERROR(SEARCH("Delete",B220)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="79" operator="containsText" text="Change">
+      <formula>NOT(ISERROR(SEARCH("Change",B220)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="80" operator="containsText" text="Create">
+      <formula>NOT(ISERROR(SEARCH("Create",B220)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B220">
+    <cfRule type="containsText" dxfId="36" priority="77" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",B220)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B226">
+    <cfRule type="containsText" dxfId="35" priority="70" stopIfTrue="1" operator="containsText" text="Delete">
+      <formula>NOT(ISERROR(SEARCH("Delete",B226)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="71" operator="containsText" text="Change">
+      <formula>NOT(ISERROR(SEARCH("Change",B226)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="72" operator="containsText" text="Create">
+      <formula>NOT(ISERROR(SEARCH("Create",B226)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B226">
+    <cfRule type="containsText" dxfId="32" priority="69" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",B226)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B221:B222 B225">
+    <cfRule type="containsText" dxfId="31" priority="74" stopIfTrue="1" operator="containsText" text="Delete">
+      <formula>NOT(ISERROR(SEARCH("Delete",B221)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="75" operator="containsText" text="Change">
+      <formula>NOT(ISERROR(SEARCH("Change",B221)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="29" priority="76" operator="containsText" text="Create">
+      <formula>NOT(ISERROR(SEARCH("Create",B221)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B221:B222 B225">
+    <cfRule type="containsText" dxfId="28" priority="73" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",B221)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B92">
-    <cfRule type="containsText" dxfId="23" priority="50" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="27" priority="54" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B92)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="51" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="26" priority="55" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B92)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="52" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="25" priority="56" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B92)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B92">
-    <cfRule type="containsText" dxfId="20" priority="49" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="24" priority="53" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B92)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B97:B111 B113:B143 B145:B209">
+  <conditionalFormatting sqref="B97:B111 B113:B143 B145:B154 B156:B211">
+    <cfRule type="containsText" dxfId="23" priority="22" stopIfTrue="1" operator="containsText" text="Delete">
+      <formula>NOT(ISERROR(SEARCH("Delete",B97)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="Change">
+      <formula>NOT(ISERROR(SEARCH("Change",B97)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="Create">
+      <formula>NOT(ISERROR(SEARCH("Create",B97)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B97:B111 B113:B143 B145:B154 B156:B211">
+    <cfRule type="containsText" dxfId="20" priority="21" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",B97)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B144">
     <cfRule type="containsText" dxfId="19" priority="18" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B97)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Delete",B144)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B97)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Change",B144)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="17" priority="20" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B97)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B97:B111 B113:B143 B145:B209">
+      <formula>NOT(ISERROR(SEARCH("Create",B144)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B144">
     <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B97)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B144">
+      <formula>NOT(ISERROR(SEARCH("None",B144)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B62">
     <cfRule type="containsText" dxfId="15" priority="14" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B144)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Delete",B62)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B144)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Change",B62)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="13" priority="16" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B144)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B144">
+      <formula>NOT(ISERROR(SEARCH("Create",B62)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B62">
     <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B144)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B62">
+      <formula>NOT(ISERROR(SEARCH("None",B62)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B223:B224">
     <cfRule type="containsText" dxfId="11" priority="10" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B62)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Delete",B223)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B62)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Change",B223)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B62)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B62">
+      <formula>NOT(ISERROR(SEARCH("Create",B223)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B223:B224">
     <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B62)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B221:B222">
+      <formula>NOT(ISERROR(SEARCH("None",B223)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B112">
     <cfRule type="containsText" dxfId="7" priority="6" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B221)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Delete",B112)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B221)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Change",B112)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="5" priority="8" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B221)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B221:B222">
+      <formula>NOT(ISERROR(SEARCH("Create",B112)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B112">
     <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B221)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B112">
+      <formula>NOT(ISERROR(SEARCH("None",B112)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B155">
     <cfRule type="containsText" dxfId="3" priority="2" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B112)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Delete",B155)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B112)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Change",B155)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B112)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B112">
+      <formula>NOT(ISERROR(SEARCH("Create",B155)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B155">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B112)))</formula>
+      <formula>NOT(ISERROR(SEARCH("None",B155)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B216 B218:B224 B6:B214">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B218 B220:B226 B6:B216">
       <formula1>$G$6:$G$9</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Link Crew to Release
-Add link crew to release
-remove bug in crew section
</commit_message>
<xml_diff>
--- a/Technical documentation/AL table analysis.xlsx
+++ b/Technical documentation/AL table analysis.xlsx
@@ -22,7 +22,7 @@
     <sheet name="Menu Structure" sheetId="7" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Checklist!$A$5:$C$232</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Checklist!$A$5:$C$233</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Table overview'!$A$81:$E$81</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -1143,7 +1143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1993" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1999" uniqueCount="652">
   <si>
     <t>Table name</t>
   </si>
@@ -3093,6 +3093,15 @@
   </si>
   <si>
     <t>This table is replaced by the game_release_scan table</t>
+  </si>
+  <si>
+    <t>game_release_crew</t>
+  </si>
+  <si>
+    <t>The cross table between a release and the crew in case we are dealing with a crack or hack release</t>
+  </si>
+  <si>
+    <t>Created using DB script nr 270</t>
   </si>
 </sst>
 </file>
@@ -3727,7 +3736,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="468">
+  <dxfs count="440">
     <dxf>
       <fill>
         <patternFill>
@@ -3738,6 +3747,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFC2E49C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFDB69"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5757"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="0"/>
         </patternFill>
       </fill>
@@ -3822,6 +3852,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFC2E49C"/>
         </patternFill>
       </fill>
@@ -3906,6 +3943,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFC2E49C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFDB69"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5757"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="0"/>
         </patternFill>
       </fill>
@@ -3934,6 +3992,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFC2E49C"/>
         </patternFill>
       </fill>
@@ -4543,6 +4608,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFC2E49C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFDB69"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5757"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="0"/>
         </patternFill>
       </fill>
@@ -4606,6 +4692,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFC2E49C"/>
         </patternFill>
       </fill>
@@ -4795,6 +4888,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFC2E49C"/>
         </patternFill>
       </fill>
@@ -4879,6 +4979,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFC2E49C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFDB69"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5757"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="0"/>
         </patternFill>
       </fill>
@@ -6363,6 +6484,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFC2E49C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFDB69"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5757"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="0"/>
         </patternFill>
       </fill>
@@ -6503,6 +6645,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFC2E49C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFDB69"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5757"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="0"/>
         </patternFill>
       </fill>
@@ -6538,6 +6701,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFC2E49C"/>
         </patternFill>
       </fill>
@@ -6588,363 +6758,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC2E49C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDB69"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5757"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC2E49C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDB69"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5757"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC2E49C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDB69"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5757"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC2E49C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDB69"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5757"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC2E49C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDB69"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5757"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC2E49C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDB69"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5757"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC2E49C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDB69"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5757"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC2E49C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDB69"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5757"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC2E49C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDB69"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5757"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC2E49C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDB69"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5757"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC2E49C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDB69"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5757"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC2E49C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDB69"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5757"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC2E49C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDB69"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5757"/>
         </patternFill>
       </fill>
     </dxf>
@@ -11858,1170 +11671,1170 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C82:C85 C281 C289:C291 C98:C99 C76:C78 C54:C73 C4:C11 C87:C94 C42:C44 C181 C114:C115 C249:C250 C118:C119 C96 C283:C287 C27:C39 C13:C25">
-    <cfRule type="containsText" dxfId="463" priority="366" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="439" priority="366" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="462" priority="367" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="438" priority="367" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="461" priority="368" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="437" priority="368" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C85 C281 C289:C291 C98:C99 C76:C78 C54:C73 C4:C11 C87:C94 C42:C44 C181 C114:C115 C249:C250 C118:C119 C96 C283:C287 C27:C39 C13:C25">
-    <cfRule type="containsText" dxfId="460" priority="365" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="436" priority="365" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C103">
-    <cfRule type="containsText" dxfId="459" priority="362" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="435" priority="362" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C103)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="458" priority="363" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="434" priority="363" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C103)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="457" priority="364" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="433" priority="364" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C103)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C103">
-    <cfRule type="containsText" dxfId="456" priority="361" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="432" priority="361" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C103)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C105">
-    <cfRule type="containsText" dxfId="455" priority="353" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="431" priority="353" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C105)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C104">
-    <cfRule type="containsText" dxfId="454" priority="358" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="430" priority="358" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C104)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="453" priority="359" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="429" priority="359" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C104)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="452" priority="360" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="428" priority="360" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C104)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C104">
-    <cfRule type="containsText" dxfId="451" priority="357" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="427" priority="357" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C104)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C105">
-    <cfRule type="containsText" dxfId="450" priority="354" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="426" priority="354" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C105)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="449" priority="355" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="425" priority="355" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C105)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="448" priority="356" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="424" priority="356" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C105)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C107:C109">
-    <cfRule type="containsText" dxfId="447" priority="345" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="423" priority="345" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C107)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C106">
-    <cfRule type="containsText" dxfId="446" priority="349" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="422" priority="349" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C106)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C106">
-    <cfRule type="containsText" dxfId="445" priority="350" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="421" priority="350" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C106)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="444" priority="351" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="420" priority="351" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C106)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="443" priority="352" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="419" priority="352" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C106)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C288">
-    <cfRule type="containsText" dxfId="442" priority="317" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="418" priority="317" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C288)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C107:C109">
-    <cfRule type="containsText" dxfId="441" priority="346" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="417" priority="346" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="440" priority="347" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="416" priority="347" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="439" priority="348" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="415" priority="348" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C107)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C292">
-    <cfRule type="containsText" dxfId="438" priority="342" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="414" priority="342" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C292)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="437" priority="343" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="413" priority="343" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C292)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="436" priority="344" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="412" priority="344" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C292)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C292">
-    <cfRule type="containsText" dxfId="435" priority="341" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="411" priority="341" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C292)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C294">
-    <cfRule type="containsText" dxfId="434" priority="334" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="410" priority="334" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C294)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="433" priority="335" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="409" priority="335" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C294)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="432" priority="336" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="408" priority="336" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C294)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C294">
-    <cfRule type="containsText" dxfId="431" priority="333" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="407" priority="333" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C294)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C295">
-    <cfRule type="containsText" dxfId="430" priority="330" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="406" priority="330" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C295)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="429" priority="331" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="405" priority="331" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C295)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="428" priority="332" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="404" priority="332" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C295)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C295">
-    <cfRule type="containsText" dxfId="427" priority="329" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="403" priority="329" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C295)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C296">
-    <cfRule type="containsText" dxfId="426" priority="326" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="402" priority="326" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C296)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="425" priority="327" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="401" priority="327" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C296)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="424" priority="328" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="400" priority="328" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C296)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C296">
-    <cfRule type="containsText" dxfId="423" priority="325" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="399" priority="325" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C296)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C297">
-    <cfRule type="containsText" dxfId="422" priority="322" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="398" priority="322" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C297)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="421" priority="323" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="397" priority="323" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C297)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="420" priority="324" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="396" priority="324" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C297)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C297">
-    <cfRule type="containsText" dxfId="419" priority="321" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="395" priority="321" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C297)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C288">
-    <cfRule type="containsText" dxfId="418" priority="318" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="394" priority="318" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C288)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="417" priority="319" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="393" priority="319" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C288)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="416" priority="320" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="392" priority="320" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C288)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C113">
-    <cfRule type="containsText" dxfId="415" priority="314" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="391" priority="314" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C113)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="414" priority="315" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="390" priority="315" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C113)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="413" priority="316" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="389" priority="316" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C113)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C113">
-    <cfRule type="containsText" dxfId="412" priority="313" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="388" priority="313" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C113)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C150">
-    <cfRule type="containsText" dxfId="411" priority="306" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="387" priority="306" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C150)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="410" priority="307" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="386" priority="307" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C150)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="409" priority="308" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="385" priority="308" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C150)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C150">
-    <cfRule type="containsText" dxfId="408" priority="305" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="384" priority="305" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C150)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C151">
-    <cfRule type="containsText" dxfId="407" priority="302" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="383" priority="302" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C151)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="406" priority="303" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="382" priority="303" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C151)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="405" priority="304" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="381" priority="304" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C151)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C151">
-    <cfRule type="containsText" dxfId="404" priority="301" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="380" priority="301" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C151)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C152">
-    <cfRule type="containsText" dxfId="403" priority="298" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="379" priority="298" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C152)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="402" priority="299" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="378" priority="299" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C152)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="401" priority="300" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="377" priority="300" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C152)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C152">
-    <cfRule type="containsText" dxfId="400" priority="297" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="376" priority="297" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C152)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C153">
-    <cfRule type="containsText" dxfId="399" priority="294" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="375" priority="294" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C153)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="398" priority="295" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="374" priority="295" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C153)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="397" priority="296" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="373" priority="296" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C153)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C153">
-    <cfRule type="containsText" dxfId="396" priority="293" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="372" priority="293" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C153)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C154">
-    <cfRule type="containsText" dxfId="395" priority="290" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="371" priority="290" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C154)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="394" priority="291" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="370" priority="291" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C154)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="393" priority="292" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="369" priority="292" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C154)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C154">
-    <cfRule type="containsText" dxfId="392" priority="289" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="368" priority="289" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C154)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C155">
-    <cfRule type="containsText" dxfId="391" priority="286" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="367" priority="286" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C155)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="390" priority="287" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="366" priority="287" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C155)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="389" priority="288" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="365" priority="288" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C155)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C155">
-    <cfRule type="containsText" dxfId="388" priority="285" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="364" priority="285" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C155)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C156">
-    <cfRule type="containsText" dxfId="387" priority="282" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="363" priority="282" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C156)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="386" priority="283" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="362" priority="283" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C156)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="385" priority="284" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="361" priority="284" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C156)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C156">
-    <cfRule type="containsText" dxfId="384" priority="281" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="360" priority="281" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C156)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C157">
-    <cfRule type="containsText" dxfId="383" priority="278" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="359" priority="278" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C157)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="382" priority="279" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="358" priority="279" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C157)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="381" priority="280" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="357" priority="280" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C157)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C157">
-    <cfRule type="containsText" dxfId="380" priority="277" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="356" priority="277" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C157)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C158">
-    <cfRule type="containsText" dxfId="379" priority="274" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="355" priority="274" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C158)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="378" priority="275" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="354" priority="275" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C158)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="377" priority="276" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="353" priority="276" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C158)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C158">
-    <cfRule type="containsText" dxfId="376" priority="273" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="352" priority="273" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C158)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C159">
-    <cfRule type="containsText" dxfId="375" priority="270" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="351" priority="270" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C159)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="374" priority="271" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="350" priority="271" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C159)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="373" priority="272" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="349" priority="272" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C159)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C159">
-    <cfRule type="containsText" dxfId="372" priority="269" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="348" priority="269" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C159)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C160">
-    <cfRule type="containsText" dxfId="371" priority="266" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="347" priority="266" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C160)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="370" priority="267" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="346" priority="267" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C160)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="369" priority="268" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="345" priority="268" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C160)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C160">
-    <cfRule type="containsText" dxfId="368" priority="265" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="344" priority="265" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C160)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C161">
-    <cfRule type="containsText" dxfId="367" priority="262" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="343" priority="262" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C161)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="366" priority="263" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="342" priority="263" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C161)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="365" priority="264" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="341" priority="264" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C161)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C161">
-    <cfRule type="containsText" dxfId="364" priority="261" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="340" priority="261" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C161)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C162">
-    <cfRule type="containsText" dxfId="363" priority="258" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="339" priority="258" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C162)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="362" priority="259" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="338" priority="259" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C162)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="361" priority="260" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="337" priority="260" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C162)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C162">
-    <cfRule type="containsText" dxfId="360" priority="257" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="336" priority="257" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C162)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C163">
-    <cfRule type="containsText" dxfId="359" priority="254" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="335" priority="254" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C163)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="358" priority="255" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="334" priority="255" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C163)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="357" priority="256" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="333" priority="256" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C163)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C163">
-    <cfRule type="containsText" dxfId="356" priority="253" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="332" priority="253" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C163)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C164">
-    <cfRule type="containsText" dxfId="355" priority="250" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="331" priority="250" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C164)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="354" priority="251" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="330" priority="251" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C164)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="353" priority="252" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="329" priority="252" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C164)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C164">
-    <cfRule type="containsText" dxfId="352" priority="249" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="328" priority="249" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C164)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C165">
-    <cfRule type="containsText" dxfId="351" priority="246" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="327" priority="246" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C165)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="350" priority="247" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="326" priority="247" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C165)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="349" priority="248" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="325" priority="248" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C165)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C165">
-    <cfRule type="containsText" dxfId="348" priority="245" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="324" priority="245" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C165)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C166">
-    <cfRule type="containsText" dxfId="347" priority="242" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="323" priority="242" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C166)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="346" priority="243" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="322" priority="243" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C166)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="345" priority="244" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="321" priority="244" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C166)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C166">
-    <cfRule type="containsText" dxfId="344" priority="241" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="320" priority="241" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C166)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C167">
-    <cfRule type="containsText" dxfId="343" priority="238" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="319" priority="238" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C167)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="342" priority="239" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="318" priority="239" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C167)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="341" priority="240" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="317" priority="240" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C167)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C167">
-    <cfRule type="containsText" dxfId="340" priority="237" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="316" priority="237" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C167)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C168:C170">
-    <cfRule type="containsText" dxfId="339" priority="234" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="315" priority="234" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C168)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="338" priority="235" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="314" priority="235" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C168)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="337" priority="236" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="313" priority="236" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C168)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C168:C170">
-    <cfRule type="containsText" dxfId="336" priority="233" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="312" priority="233" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C168)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C299">
-    <cfRule type="containsText" dxfId="335" priority="226" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="311" priority="226" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C299)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="334" priority="227" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="310" priority="227" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C299)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="333" priority="228" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="309" priority="228" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C299)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C299">
-    <cfRule type="containsText" dxfId="332" priority="225" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="308" priority="225" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C299)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C86">
-    <cfRule type="containsText" dxfId="331" priority="214" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="307" priority="214" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="330" priority="215" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="306" priority="215" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="329" priority="216" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="305" priority="216" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C86)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C86">
-    <cfRule type="containsText" dxfId="328" priority="213" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="304" priority="213" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C86)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="327" priority="202" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="303" priority="202" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="326" priority="203" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="302" priority="203" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="325" priority="204" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="301" priority="204" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="324" priority="201" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="300" priority="201" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C75">
-    <cfRule type="containsText" dxfId="323" priority="190" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="299" priority="190" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="322" priority="191" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="298" priority="191" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="321" priority="192" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="297" priority="192" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C75">
-    <cfRule type="containsText" dxfId="320" priority="189" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="296" priority="189" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74">
-    <cfRule type="containsText" dxfId="319" priority="194" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="295" priority="194" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C74)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="318" priority="195" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="294" priority="195" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C74)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="317" priority="196" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="293" priority="196" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74">
-    <cfRule type="containsText" dxfId="316" priority="193" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="292" priority="193" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C97">
-    <cfRule type="containsText" dxfId="311" priority="182" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="291" priority="182" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C97)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="310" priority="183" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="290" priority="183" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C97)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="309" priority="184" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="289" priority="184" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C97)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C97">
-    <cfRule type="containsText" dxfId="308" priority="181" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="288" priority="181" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C97)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="307" priority="178" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="287" priority="178" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="306" priority="179" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="286" priority="179" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="305" priority="180" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="285" priority="180" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="304" priority="177" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="284" priority="177" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="containsText" dxfId="303" priority="174" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="283" priority="174" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="302" priority="175" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="282" priority="175" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="301" priority="176" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="281" priority="176" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="containsText" dxfId="300" priority="173" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="280" priority="173" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C49">
-    <cfRule type="containsText" dxfId="299" priority="170" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="279" priority="170" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="298" priority="171" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="278" priority="171" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="297" priority="172" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="277" priority="172" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C49">
-    <cfRule type="containsText" dxfId="296" priority="169" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="276" priority="169" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="295" priority="166" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="275" priority="166" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="294" priority="167" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="274" priority="167" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="293" priority="168" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="273" priority="168" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="292" priority="165" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="272" priority="165" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="291" priority="162" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="271" priority="162" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="290" priority="163" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="270" priority="163" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="289" priority="164" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="269" priority="164" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="288" priority="161" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="268" priority="161" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="containsText" dxfId="287" priority="158" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="267" priority="158" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="286" priority="159" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="266" priority="159" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="285" priority="160" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="265" priority="160" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="containsText" dxfId="284" priority="157" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="264" priority="157" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C230">
-    <cfRule type="containsText" dxfId="283" priority="154" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="263" priority="154" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C230)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="282" priority="155" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="262" priority="155" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C230)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="281" priority="156" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="261" priority="156" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C230)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C230">
-    <cfRule type="containsText" dxfId="280" priority="153" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="260" priority="153" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C230)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C231">
-    <cfRule type="containsText" dxfId="279" priority="150" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="259" priority="150" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C231)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="278" priority="151" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="258" priority="151" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C231)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="277" priority="152" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="257" priority="152" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C231)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C231">
-    <cfRule type="containsText" dxfId="276" priority="149" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="256" priority="149" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C231)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C232">
-    <cfRule type="containsText" dxfId="275" priority="146" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="255" priority="146" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C232)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="274" priority="147" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="254" priority="147" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C232)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="273" priority="148" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="253" priority="148" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C232)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C232">
-    <cfRule type="containsText" dxfId="272" priority="145" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="252" priority="145" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C232)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C145:C146">
-    <cfRule type="containsText" dxfId="271" priority="142" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="251" priority="142" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C145)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="270" priority="143" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="250" priority="143" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C145)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="269" priority="144" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="249" priority="144" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C145)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C145:C146">
-    <cfRule type="containsText" dxfId="268" priority="141" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="248" priority="141" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C145)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C143">
-    <cfRule type="containsText" dxfId="267" priority="130" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="247" priority="130" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C143)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="266" priority="131" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="246" priority="131" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C143)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="265" priority="132" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="245" priority="132" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C143)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C143">
-    <cfRule type="containsText" dxfId="264" priority="129" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="244" priority="129" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C143)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C138">
-    <cfRule type="containsText" dxfId="263" priority="126" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="243" priority="126" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C138)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="262" priority="127" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="242" priority="127" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C138)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="261" priority="128" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="241" priority="128" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C138)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C138">
-    <cfRule type="containsText" dxfId="260" priority="125" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="240" priority="125" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C138)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C239">
-    <cfRule type="containsText" dxfId="259" priority="118" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="239" priority="118" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C239)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="258" priority="119" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="238" priority="119" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C239)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="257" priority="120" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="237" priority="120" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C239)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C239">
-    <cfRule type="containsText" dxfId="256" priority="117" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="236" priority="117" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C239)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C241:C243">
-    <cfRule type="containsText" dxfId="255" priority="114" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="235" priority="114" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C241)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="254" priority="115" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="234" priority="115" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C241)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="253" priority="116" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="233" priority="116" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C241)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C241:C243">
-    <cfRule type="containsText" dxfId="252" priority="113" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="232" priority="113" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C241)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C238">
-    <cfRule type="containsText" dxfId="251" priority="110" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="231" priority="110" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C238)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="250" priority="111" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="230" priority="111" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C238)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="249" priority="112" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="229" priority="112" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C238)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C238">
-    <cfRule type="containsText" dxfId="248" priority="109" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="228" priority="109" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C238)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C255">
-    <cfRule type="containsText" dxfId="247" priority="106" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="227" priority="106" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C255)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="246" priority="107" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="226" priority="107" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C255)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="245" priority="108" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="225" priority="108" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C255)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C255">
-    <cfRule type="containsText" dxfId="244" priority="105" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="224" priority="105" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C255)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C256:C260">
-    <cfRule type="containsText" dxfId="243" priority="102" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="223" priority="102" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C256)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="242" priority="103" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="222" priority="103" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C256)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="241" priority="104" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="221" priority="104" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C256)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C256:C260">
-    <cfRule type="containsText" dxfId="240" priority="101" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="220" priority="101" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C256)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A254:E258">
-    <cfRule type="containsText" dxfId="239" priority="98" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="219" priority="98" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",A254)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="238" priority="99" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="218" priority="99" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",A254)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="237" priority="100" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="217" priority="100" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",A254)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A254:E258">
-    <cfRule type="containsText" dxfId="236" priority="97" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="216" priority="97" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",A254)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C248">
-    <cfRule type="containsText" dxfId="235" priority="94" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="215" priority="94" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C248)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="234" priority="95" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="214" priority="95" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C248)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="233" priority="96" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="213" priority="96" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C248)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C248">
-    <cfRule type="containsText" dxfId="232" priority="93" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="212" priority="93" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C248)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C247">
-    <cfRule type="containsText" dxfId="231" priority="86" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="211" priority="86" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C247)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="230" priority="87" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="210" priority="87" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C247)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="229" priority="88" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="209" priority="88" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C247)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C247">
-    <cfRule type="containsText" dxfId="228" priority="85" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="208" priority="85" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C247)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C205">
-    <cfRule type="containsText" dxfId="227" priority="82" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="207" priority="82" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C205)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="226" priority="83" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="206" priority="83" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C205)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="225" priority="84" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="205" priority="84" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C205)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C205">
-    <cfRule type="containsText" dxfId="224" priority="81" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="204" priority="81" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C205)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C301">
-    <cfRule type="containsText" dxfId="223" priority="70" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="203" priority="70" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C301)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="222" priority="71" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="202" priority="71" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C301)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="221" priority="72" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="201" priority="72" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C301)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C301">
-    <cfRule type="containsText" dxfId="220" priority="69" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="200" priority="69" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C301)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C305">
-    <cfRule type="containsText" dxfId="219" priority="62" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="199" priority="62" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C305)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="218" priority="63" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="198" priority="63" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C305)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="217" priority="64" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="197" priority="64" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C305)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C305">
-    <cfRule type="containsText" dxfId="216" priority="61" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="196" priority="61" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C305)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C302:C304">
-    <cfRule type="containsText" dxfId="215" priority="66" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="195" priority="66" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C302)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="214" priority="67" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="194" priority="67" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C302)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="213" priority="68" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="193" priority="68" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C302:C304">
-    <cfRule type="containsText" dxfId="212" priority="65" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="192" priority="65" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C302)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C267:C268">
-    <cfRule type="containsText" dxfId="211" priority="58" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="191" priority="58" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C267)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="210" priority="59" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="190" priority="59" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C267)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="209" priority="60" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="189" priority="60" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C267)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C267:C268">
-    <cfRule type="containsText" dxfId="208" priority="57" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="188" priority="57" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C267)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A264:E266">
-    <cfRule type="containsText" dxfId="207" priority="42" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="187" priority="42" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",A264)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="206" priority="43" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="186" priority="43" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",A264)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="205" priority="44" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="185" priority="44" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",A264)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A264:E266">
-    <cfRule type="containsText" dxfId="204" priority="41" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="184" priority="41" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",A264)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A272:E277">
-    <cfRule type="containsText" dxfId="203" priority="38" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="183" priority="38" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",A272)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="202" priority="39" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="182" priority="39" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",A272)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="201" priority="40" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="181" priority="40" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",A272)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A272:E277">
-    <cfRule type="containsText" dxfId="200" priority="37" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="180" priority="37" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",A272)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C95">
-    <cfRule type="containsText" dxfId="199" priority="34" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="179" priority="34" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C95)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="198" priority="35" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="178" priority="35" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C95)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="197" priority="36" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="177" priority="36" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C95)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C95">
-    <cfRule type="containsText" dxfId="196" priority="33" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="176" priority="33" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C95)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C240">
-    <cfRule type="containsText" dxfId="195" priority="30" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="175" priority="30" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C240)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="194" priority="31" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="174" priority="31" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C240)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="193" priority="32" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="173" priority="32" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C240)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C240">
-    <cfRule type="containsText" dxfId="192" priority="29" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="172" priority="29" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C240)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C282">
-    <cfRule type="containsText" dxfId="191" priority="26" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="171" priority="26" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C282)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="190" priority="27" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="170" priority="27" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C282)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="189" priority="28" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="169" priority="28" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C282)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C282">
-    <cfRule type="containsText" dxfId="188" priority="25" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="168" priority="25" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C282)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="containsText" dxfId="187" priority="22" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="167" priority="22" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="186" priority="23" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="166" priority="23" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="185" priority="24" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="165" priority="24" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="containsText" dxfId="184" priority="21" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="164" priority="21" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C293">
-    <cfRule type="containsText" dxfId="183" priority="18" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="163" priority="18" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C293)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="182" priority="19" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="162" priority="19" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C293)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="181" priority="20" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="161" priority="20" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C293)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C293">
-    <cfRule type="containsText" dxfId="180" priority="17" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="160" priority="17" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C293)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="containsText" dxfId="179" priority="10" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="159" priority="10" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C53)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="178" priority="11" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="158" priority="11" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C53)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="177" priority="12" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="157" priority="12" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="containsText" dxfId="176" priority="9" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="156" priority="9" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51">
-    <cfRule type="containsText" dxfId="15" priority="6" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="155" priority="6" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="7" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="154" priority="7" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="153" priority="8" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51">
-    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="152" priority="5" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52">
-    <cfRule type="containsText" dxfId="7" priority="2" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="151" priority="2" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",C52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="150" priority="3" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",C52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="149" priority="4" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",C52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="148" priority="1" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",C52)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13041,10 +12854,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P232"/>
+  <dimension ref="A1:P233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="52.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14365,7 +14178,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="35" t="s">
-        <v>104</v>
+        <v>649</v>
       </c>
       <c r="B106" s="42" t="s">
         <v>16</v>
@@ -14374,12 +14187,12 @@
         <v>548</v>
       </c>
       <c r="D106" s="69" t="s">
-        <v>623</v>
+        <v>651</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="35" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="B107" s="42" t="s">
         <v>16</v>
@@ -14388,12 +14201,12 @@
         <v>548</v>
       </c>
       <c r="D107" s="69" t="s">
-        <v>612</v>
+        <v>623</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="35" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B108" s="42" t="s">
         <v>16</v>
@@ -14402,36 +14215,36 @@
         <v>548</v>
       </c>
       <c r="D108" s="69" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="B109" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C109" s="69" t="s">
+        <v>548</v>
+      </c>
+      <c r="D109" s="69" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="97" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="97" t="s">
         <v>89</v>
       </c>
-      <c r="B109" s="98" t="s">
+      <c r="B110" s="98" t="s">
         <v>16</v>
       </c>
-      <c r="C109" s="69"/>
-      <c r="D109" s="69"/>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="35" t="s">
-        <v>172</v>
-      </c>
-      <c r="B110" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="C110" s="69" t="s">
-        <v>548</v>
-      </c>
-      <c r="D110" s="69" t="s">
-        <v>619</v>
-      </c>
+      <c r="C110" s="69"/>
+      <c r="D110" s="69"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="35" t="s">
-        <v>94</v>
+        <v>172</v>
       </c>
       <c r="B111" s="42" t="s">
         <v>16</v>
@@ -14440,12 +14253,12 @@
         <v>548</v>
       </c>
       <c r="D111" s="69" t="s">
-        <v>575</v>
+        <v>619</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B112" s="42" t="s">
         <v>16</v>
@@ -14454,12 +14267,12 @@
         <v>548</v>
       </c>
       <c r="D112" s="69" t="s">
-        <v>614</v>
+        <v>575</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="35" t="s">
-        <v>624</v>
+        <v>95</v>
       </c>
       <c r="B113" s="42" t="s">
         <v>16</v>
@@ -14468,36 +14281,36 @@
         <v>548</v>
       </c>
       <c r="D113" s="69" t="s">
-        <v>625</v>
+        <v>614</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="35" t="s">
-        <v>96</v>
+        <v>624</v>
       </c>
       <c r="B114" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C114" s="69"/>
-      <c r="D114" s="69"/>
+      <c r="C114" s="69" t="s">
+        <v>548</v>
+      </c>
+      <c r="D114" s="69" t="s">
+        <v>625</v>
+      </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="35" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B115" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C115" s="69" t="s">
-        <v>548</v>
-      </c>
-      <c r="D115" s="69" t="s">
-        <v>553</v>
-      </c>
+      <c r="C115" s="69"/>
+      <c r="D115" s="69"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="35" t="s">
-        <v>646</v>
+        <v>93</v>
       </c>
       <c r="B116" s="42" t="s">
         <v>16</v>
@@ -14506,12 +14319,12 @@
         <v>548</v>
       </c>
       <c r="D116" s="69" t="s">
-        <v>647</v>
+        <v>553</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="35" t="s">
-        <v>92</v>
+        <v>646</v>
       </c>
       <c r="B117" s="42" t="s">
         <v>16</v>
@@ -14520,12 +14333,12 @@
         <v>548</v>
       </c>
       <c r="D117" s="69" t="s">
-        <v>551</v>
+        <v>647</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="35" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B118" s="42" t="s">
         <v>16</v>
@@ -14534,12 +14347,12 @@
         <v>548</v>
       </c>
       <c r="D118" s="69" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="35" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B119" s="42" t="s">
         <v>16</v>
@@ -14548,12 +14361,12 @@
         <v>548</v>
       </c>
       <c r="D119" s="69" t="s">
-        <v>616</v>
+        <v>552</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="35" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="B120" s="42" t="s">
         <v>16</v>
@@ -14562,36 +14375,36 @@
         <v>548</v>
       </c>
       <c r="D120" s="69" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="B121" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C121" s="69" t="s">
+        <v>548</v>
+      </c>
+      <c r="D121" s="69" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="41" t="s">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B121" s="42" t="s">
-        <v>204</v>
-      </c>
-      <c r="C121" s="69"/>
-      <c r="D121" s="69"/>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="44" t="s">
+      <c r="B122" s="42" t="s">
+        <v>204</v>
+      </c>
+      <c r="C122" s="69"/>
+      <c r="D122" s="69"/>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="44" t="s">
         <v>25</v>
-      </c>
-      <c r="B122" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="C122" s="69" t="s">
-        <v>548</v>
-      </c>
-      <c r="D122" s="69" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="35" t="s">
-        <v>347</v>
       </c>
       <c r="B123" s="42" t="s">
         <v>3</v>
@@ -14600,50 +14413,50 @@
         <v>548</v>
       </c>
       <c r="D123" s="69" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="35" t="s">
-        <v>22</v>
+        <v>347</v>
       </c>
       <c r="B124" s="42" t="s">
-        <v>204</v>
-      </c>
-      <c r="C124" s="69"/>
-      <c r="D124" s="69"/>
+        <v>3</v>
+      </c>
+      <c r="C124" s="69" t="s">
+        <v>548</v>
+      </c>
+      <c r="D124" s="69" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="35" t="s">
-        <v>640</v>
+        <v>22</v>
       </c>
       <c r="B125" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="C125" s="69" t="s">
-        <v>548</v>
-      </c>
-      <c r="D125" s="69" t="s">
-        <v>641</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="C125" s="69"/>
+      <c r="D125" s="69"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="35" t="s">
-        <v>85</v>
+        <v>640</v>
       </c>
       <c r="B126" s="42" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C126" s="69" t="s">
         <v>548</v>
       </c>
       <c r="D126" s="69" t="s">
-        <v>594</v>
+        <v>641</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="35" t="s">
-        <v>556</v>
+        <v>85</v>
       </c>
       <c r="B127" s="42" t="s">
         <v>3</v>
@@ -14652,12 +14465,12 @@
         <v>548</v>
       </c>
       <c r="D127" s="69" t="s">
-        <v>557</v>
+        <v>594</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="35" t="s">
-        <v>83</v>
+        <v>556</v>
       </c>
       <c r="B128" s="42" t="s">
         <v>3</v>
@@ -14666,12 +14479,12 @@
         <v>548</v>
       </c>
       <c r="D128" s="69" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="35" t="s">
-        <v>348</v>
+        <v>83</v>
       </c>
       <c r="B129" s="42" t="s">
         <v>3</v>
@@ -14680,36 +14493,36 @@
         <v>548</v>
       </c>
       <c r="D129" s="69" t="s">
-        <v>580</v>
+        <v>555</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="35" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B130" s="42" t="s">
-        <v>204</v>
-      </c>
-      <c r="C130" s="69"/>
-      <c r="D130" s="69"/>
+        <v>3</v>
+      </c>
+      <c r="C130" s="69" t="s">
+        <v>548</v>
+      </c>
+      <c r="D130" s="69" t="s">
+        <v>580</v>
+      </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="35" t="s">
-        <v>84</v>
+        <v>349</v>
       </c>
       <c r="B131" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="C131" s="69" t="s">
-        <v>548</v>
-      </c>
-      <c r="D131" s="69" t="s">
-        <v>621</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="C131" s="69"/>
+      <c r="D131" s="69"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="35" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B132" s="42" t="s">
         <v>3</v>
@@ -14723,17 +14536,21 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="35" t="s">
-        <v>351</v>
+        <v>86</v>
       </c>
       <c r="B133" s="42" t="s">
-        <v>204</v>
-      </c>
-      <c r="C133" s="69"/>
-      <c r="D133" s="69"/>
+        <v>3</v>
+      </c>
+      <c r="C133" s="69" t="s">
+        <v>548</v>
+      </c>
+      <c r="D133" s="69" t="s">
+        <v>621</v>
+      </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="35" t="s">
-        <v>28</v>
+        <v>351</v>
       </c>
       <c r="B134" s="42" t="s">
         <v>204</v>
@@ -14743,21 +14560,17 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="35" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="B135" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="C135" s="69" t="s">
-        <v>548</v>
-      </c>
-      <c r="D135" s="69" t="s">
-        <v>629</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="C135" s="69"/>
+      <c r="D135" s="69"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="35" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B136" s="42" t="s">
         <v>3</v>
@@ -14766,42 +14579,46 @@
         <v>548</v>
       </c>
       <c r="D136" s="69" t="s">
-        <v>565</v>
+        <v>629</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="35" t="s">
-        <v>311</v>
+        <v>71</v>
       </c>
       <c r="B137" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C137" s="69"/>
-      <c r="D137" s="69"/>
+      <c r="C137" s="69" t="s">
+        <v>548</v>
+      </c>
+      <c r="D137" s="69" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="35" t="s">
-        <v>46</v>
+        <v>311</v>
       </c>
       <c r="B138" s="42" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C138" s="69"/>
       <c r="D138" s="69"/>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="35" t="s">
-        <v>256</v>
+        <v>46</v>
       </c>
       <c r="B139" s="42" t="s">
-        <v>204</v>
+        <v>16</v>
       </c>
       <c r="C139" s="69"/>
       <c r="D139" s="69"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="35" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B140" s="42" t="s">
         <v>204</v>
@@ -14811,7 +14628,7 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="35" t="s">
-        <v>355</v>
+        <v>257</v>
       </c>
       <c r="B141" s="42" t="s">
         <v>204</v>
@@ -14821,7 +14638,7 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="35" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B142" s="42" t="s">
         <v>204</v>
@@ -14831,7 +14648,7 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="35" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="B143" s="42" t="s">
         <v>204</v>
@@ -14841,7 +14658,7 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="35" t="s">
-        <v>364</v>
+        <v>353</v>
       </c>
       <c r="B144" s="42" t="s">
         <v>204</v>
@@ -14851,7 +14668,7 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="35" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B145" s="42" t="s">
         <v>204</v>
@@ -14861,7 +14678,7 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="35" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B146" s="42" t="s">
         <v>204</v>
@@ -14871,7 +14688,7 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="35" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B147" s="42" t="s">
         <v>204</v>
@@ -14881,73 +14698,73 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="35" t="s">
-        <v>40</v>
+        <v>370</v>
       </c>
       <c r="B148" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="C148" s="94" t="s">
-        <v>548</v>
-      </c>
-      <c r="D148" s="66" t="s">
-        <v>576</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="C148" s="69"/>
+      <c r="D148" s="69"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="35" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B149" s="42" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C149" s="94" t="s">
         <v>548</v>
       </c>
       <c r="D149" s="66" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="35" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B150" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="C150" s="69" t="s">
+        <v>2</v>
+      </c>
+      <c r="C150" s="94" t="s">
         <v>548</v>
       </c>
-      <c r="D150" s="69" t="s">
-        <v>579</v>
+      <c r="D150" s="66" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="35" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="B151" s="42" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C151" s="69" t="s">
         <v>548</v>
       </c>
       <c r="D151" s="69" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="35" t="s">
-        <v>432</v>
+        <v>62</v>
       </c>
       <c r="B152" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="C152" s="69"/>
-      <c r="D152" s="69"/>
+        <v>16</v>
+      </c>
+      <c r="C152" s="69" t="s">
+        <v>548</v>
+      </c>
+      <c r="D152" s="69" t="s">
+        <v>578</v>
+      </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="35" t="s">
-        <v>376</v>
+        <v>432</v>
       </c>
       <c r="B153" s="42" t="s">
         <v>3</v>
@@ -14957,7 +14774,7 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="35" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B154" s="42" t="s">
         <v>3</v>
@@ -14967,21 +14784,17 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="35" t="s">
-        <v>114</v>
+        <v>378</v>
       </c>
       <c r="B155" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="C155" s="69" t="s">
-        <v>548</v>
-      </c>
-      <c r="D155" s="69" t="s">
-        <v>631</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C155" s="69"/>
+      <c r="D155" s="69"/>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="35" t="s">
-        <v>630</v>
+        <v>114</v>
       </c>
       <c r="B156" s="42" t="s">
         <v>16</v>
@@ -14990,12 +14803,12 @@
         <v>548</v>
       </c>
       <c r="D156" s="69" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="35" t="s">
-        <v>115</v>
+        <v>630</v>
       </c>
       <c r="B157" s="42" t="s">
         <v>16</v>
@@ -15004,12 +14817,12 @@
         <v>548</v>
       </c>
       <c r="D157" s="69" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="35" t="s">
-        <v>634</v>
+        <v>115</v>
       </c>
       <c r="B158" s="42" t="s">
         <v>16</v>
@@ -15018,12 +14831,12 @@
         <v>548</v>
       </c>
       <c r="D158" s="69" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="35" t="s">
-        <v>65</v>
+        <v>634</v>
       </c>
       <c r="B159" s="42" t="s">
         <v>16</v>
@@ -15032,12 +14845,12 @@
         <v>548</v>
       </c>
       <c r="D159" s="69" t="s">
-        <v>615</v>
+        <v>633</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="35" t="s">
-        <v>627</v>
+        <v>65</v>
       </c>
       <c r="B160" s="42" t="s">
         <v>16</v>
@@ -15046,22 +14859,26 @@
         <v>548</v>
       </c>
       <c r="D160" s="69" t="s">
-        <v>628</v>
+        <v>615</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="35" t="s">
-        <v>384</v>
+        <v>627</v>
       </c>
       <c r="B161" s="42" t="s">
-        <v>204</v>
-      </c>
-      <c r="C161" s="69"/>
-      <c r="D161" s="69"/>
+        <v>16</v>
+      </c>
+      <c r="C161" s="69" t="s">
+        <v>548</v>
+      </c>
+      <c r="D161" s="69" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="35" t="s">
-        <v>400</v>
+        <v>384</v>
       </c>
       <c r="B162" s="42" t="s">
         <v>204</v>
@@ -15071,27 +14888,27 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="35" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="B163" s="42" t="s">
-        <v>3</v>
+        <v>204</v>
       </c>
       <c r="C163" s="69"/>
       <c r="D163" s="69"/>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="35" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B164" s="42" t="s">
-        <v>204</v>
+        <v>3</v>
       </c>
       <c r="C164" s="69"/>
       <c r="D164" s="69"/>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="35" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B165" s="42" t="s">
         <v>204</v>
@@ -15101,7 +14918,7 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="35" t="s">
-        <v>385</v>
+        <v>397</v>
       </c>
       <c r="B166" s="42" t="s">
         <v>204</v>
@@ -15111,7 +14928,7 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="35" t="s">
-        <v>402</v>
+        <v>385</v>
       </c>
       <c r="B167" s="42" t="s">
         <v>204</v>
@@ -15121,7 +14938,7 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="35" t="s">
-        <v>388</v>
+        <v>402</v>
       </c>
       <c r="B168" s="42" t="s">
         <v>204</v>
@@ -15131,7 +14948,7 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="35" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B169" s="42" t="s">
         <v>204</v>
@@ -15141,7 +14958,7 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="35" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B170" s="42" t="s">
         <v>204</v>
@@ -15151,7 +14968,7 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="35" t="s">
-        <v>386</v>
+        <v>391</v>
       </c>
       <c r="B171" s="42" t="s">
         <v>204</v>
@@ -15161,7 +14978,7 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="35" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="B172" s="42" t="s">
         <v>204</v>
@@ -15171,7 +14988,7 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="35" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="B173" s="42" t="s">
         <v>204</v>
@@ -15181,7 +14998,7 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="35" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="B174" s="42" t="s">
         <v>204</v>
@@ -15191,7 +15008,7 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="35" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="B175" s="42" t="s">
         <v>204</v>
@@ -15201,7 +15018,7 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="35" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="B176" s="42" t="s">
         <v>204</v>
@@ -15211,7 +15028,7 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="35" t="s">
-        <v>382</v>
+        <v>401</v>
       </c>
       <c r="B177" s="42" t="s">
         <v>204</v>
@@ -15221,7 +15038,7 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="35" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B178" s="42" t="s">
         <v>204</v>
@@ -15231,27 +15048,27 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="35" t="s">
-        <v>428</v>
+        <v>383</v>
       </c>
       <c r="B179" s="42" t="s">
-        <v>3</v>
+        <v>204</v>
       </c>
       <c r="C179" s="69"/>
       <c r="D179" s="69"/>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="35" t="s">
-        <v>380</v>
+        <v>428</v>
       </c>
       <c r="B180" s="42" t="s">
-        <v>204</v>
+        <v>3</v>
       </c>
       <c r="C180" s="69"/>
       <c r="D180" s="69"/>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="35" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B181" s="42" t="s">
         <v>204</v>
@@ -15261,7 +15078,7 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="35" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="B182" s="42" t="s">
         <v>204</v>
@@ -15271,7 +15088,7 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="35" t="s">
-        <v>431</v>
+        <v>395</v>
       </c>
       <c r="B183" s="42" t="s">
         <v>204</v>
@@ -15281,7 +15098,7 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="35" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B184" s="42" t="s">
         <v>204</v>
@@ -15291,7 +15108,7 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="35" t="s">
-        <v>522</v>
+        <v>434</v>
       </c>
       <c r="B185" s="42" t="s">
         <v>204</v>
@@ -15301,7 +15118,7 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="35" t="s">
-        <v>437</v>
+        <v>522</v>
       </c>
       <c r="B186" s="42" t="s">
         <v>204</v>
@@ -15311,7 +15128,7 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="35" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B187" s="42" t="s">
         <v>204</v>
@@ -15321,7 +15138,7 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="35" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B188" s="42" t="s">
         <v>204</v>
@@ -15331,7 +15148,7 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="35" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B189" s="42" t="s">
         <v>204</v>
@@ -15341,7 +15158,7 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="35" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B190" s="42" t="s">
         <v>204</v>
@@ -15351,7 +15168,7 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="35" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B191" s="42" t="s">
         <v>204</v>
@@ -15361,45 +15178,45 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="35" t="s">
-        <v>112</v>
+        <v>444</v>
       </c>
       <c r="B192" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="C192" s="69" t="s">
-        <v>587</v>
-      </c>
-      <c r="D192" s="69" t="s">
-        <v>588</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="C192" s="69"/>
+      <c r="D192" s="69"/>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="35" t="s">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="B193" s="42" t="s">
         <v>16</v>
       </c>
       <c r="C193" s="69" t="s">
-        <v>548</v>
+        <v>587</v>
       </c>
       <c r="D193" s="69" t="s">
-        <v>582</v>
+        <v>588</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="35" t="s">
-        <v>451</v>
+        <v>12</v>
       </c>
       <c r="B194" s="42" t="s">
-        <v>204</v>
-      </c>
-      <c r="C194" s="69"/>
-      <c r="D194" s="69"/>
+        <v>16</v>
+      </c>
+      <c r="C194" s="69" t="s">
+        <v>548</v>
+      </c>
+      <c r="D194" s="69" t="s">
+        <v>582</v>
+      </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="35" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B195" s="42" t="s">
         <v>204</v>
@@ -15409,55 +15226,55 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="35" t="s">
-        <v>55</v>
+        <v>453</v>
       </c>
       <c r="B196" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="C196" s="69" t="s">
-        <v>548</v>
-      </c>
-      <c r="D196" s="69" t="s">
-        <v>554</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="C196" s="69"/>
+      <c r="D196" s="69"/>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="35" t="s">
-        <v>456</v>
+        <v>55</v>
       </c>
       <c r="B197" s="42" t="s">
-        <v>204</v>
-      </c>
-      <c r="C197" s="69"/>
-      <c r="D197" s="69"/>
+        <v>16</v>
+      </c>
+      <c r="C197" s="69" t="s">
+        <v>548</v>
+      </c>
+      <c r="D197" s="69" t="s">
+        <v>554</v>
+      </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="35" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B198" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="C198" s="69" t="s">
-        <v>548</v>
-      </c>
-      <c r="D198" s="69" t="s">
-        <v>642</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="C198" s="69"/>
+      <c r="D198" s="69"/>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="35" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B199" s="42" t="s">
-        <v>204</v>
-      </c>
-      <c r="C199" s="69"/>
-      <c r="D199" s="69"/>
+        <v>3</v>
+      </c>
+      <c r="C199" s="69" t="s">
+        <v>548</v>
+      </c>
+      <c r="D199" s="69" t="s">
+        <v>642</v>
+      </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="35" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B200" s="42" t="s">
         <v>204</v>
@@ -15467,7 +15284,7 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="35" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B201" s="42" t="s">
         <v>204</v>
@@ -15477,7 +15294,7 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="35" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B202" s="42" t="s">
         <v>204</v>
@@ -15487,7 +15304,7 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="35" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B203" s="42" t="s">
         <v>204</v>
@@ -15497,7 +15314,7 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="35" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="B204" s="42" t="s">
         <v>204</v>
@@ -15507,7 +15324,7 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="35" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B205" s="42" t="s">
         <v>204</v>
@@ -15517,7 +15334,7 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="35" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B206" s="42" t="s">
         <v>204</v>
@@ -15527,7 +15344,7 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="35" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B207" s="42" t="s">
         <v>204</v>
@@ -15537,7 +15354,7 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="35" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="B208" s="42" t="s">
         <v>204</v>
@@ -15547,7 +15364,7 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="35" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B209" s="42" t="s">
         <v>204</v>
@@ -15557,7 +15374,7 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="35" t="s">
-        <v>472</v>
+        <v>485</v>
       </c>
       <c r="B210" s="42" t="s">
         <v>204</v>
@@ -15567,7 +15384,7 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="35" t="s">
-        <v>486</v>
+        <v>472</v>
       </c>
       <c r="B211" s="42" t="s">
         <v>204</v>
@@ -15577,7 +15394,7 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="35" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B212" s="42" t="s">
         <v>204</v>
@@ -15587,79 +15404,79 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="35" t="s">
+        <v>488</v>
+      </c>
+      <c r="B213" s="42" t="s">
+        <v>204</v>
+      </c>
+      <c r="C213" s="69"/>
+      <c r="D213" s="69"/>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" s="35" t="s">
         <v>638</v>
       </c>
-      <c r="B213" s="42" t="s">
+      <c r="B214" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C213" s="69" t="s">
+      <c r="C214" s="69" t="s">
         <v>548</v>
       </c>
-      <c r="D213" s="69" t="s">
+      <c r="D214" s="69" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="214" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A214" s="35" t="s">
+    <row r="215" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A215" s="35" t="s">
         <v>490</v>
       </c>
-      <c r="B214" s="42" t="s">
-        <v>204</v>
-      </c>
-      <c r="C214" s="69"/>
-      <c r="D214" s="69"/>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A215" s="35" t="s">
-        <v>492</v>
-      </c>
       <c r="B215" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="C215" s="69" t="s">
-        <v>548</v>
-      </c>
-      <c r="D215" s="69" t="s">
-        <v>642</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="C215" s="69"/>
+      <c r="D215" s="69"/>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="35" t="s">
-        <v>250</v>
+        <v>492</v>
       </c>
       <c r="B216" s="42" t="s">
-        <v>204</v>
-      </c>
-      <c r="C216" s="69"/>
-      <c r="D216" s="69"/>
+        <v>3</v>
+      </c>
+      <c r="C216" s="69" t="s">
+        <v>548</v>
+      </c>
+      <c r="D216" s="69" t="s">
+        <v>642</v>
+      </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="35" t="s">
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="B217" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="C217" s="69" t="s">
-        <v>548</v>
-      </c>
-      <c r="D217" s="69" t="s">
-        <v>549</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="C217" s="69"/>
+      <c r="D217" s="69"/>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="35" t="s">
-        <v>495</v>
+        <v>50</v>
       </c>
       <c r="B218" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="C218" s="69"/>
-      <c r="D218" s="69"/>
+        <v>16</v>
+      </c>
+      <c r="C218" s="69" t="s">
+        <v>548</v>
+      </c>
+      <c r="D218" s="69" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="35" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B219" s="42" t="s">
         <v>3</v>
@@ -15669,7 +15486,7 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="35" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B220" s="42" t="s">
         <v>3</v>
@@ -15679,7 +15496,7 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" s="35" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B221" s="42" t="s">
         <v>3</v>
@@ -15689,17 +15506,17 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" s="35" t="s">
-        <v>68</v>
+        <v>499</v>
       </c>
       <c r="B222" s="42" t="s">
-        <v>204</v>
+        <v>3</v>
       </c>
       <c r="C222" s="69"/>
       <c r="D222" s="69"/>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" s="35" t="s">
-        <v>123</v>
+        <v>68</v>
       </c>
       <c r="B223" s="42" t="s">
         <v>204</v>
@@ -15709,9 +15526,9 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" s="35" t="s">
-        <v>501</v>
-      </c>
-      <c r="B224" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="B224" s="42" t="s">
         <v>204</v>
       </c>
       <c r="C224" s="69"/>
@@ -15719,7 +15536,7 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" s="35" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B225" s="38" t="s">
         <v>204</v>
@@ -15729,9 +15546,9 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" s="35" t="s">
-        <v>505</v>
-      </c>
-      <c r="B226" s="42" t="s">
+        <v>502</v>
+      </c>
+      <c r="B226" s="38" t="s">
         <v>204</v>
       </c>
       <c r="C226" s="69"/>
@@ -15739,7 +15556,7 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" s="35" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B227" s="42" t="s">
         <v>204</v>
@@ -15749,7 +15566,7 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" s="35" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B228" s="42" t="s">
         <v>204</v>
@@ -15759,7 +15576,7 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" s="35" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="B229" s="42" t="s">
         <v>204</v>
@@ -15769,7 +15586,7 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" s="35" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B230" s="42" t="s">
         <v>204</v>
@@ -15779,7 +15596,7 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" s="35" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="B231" s="42" t="s">
         <v>204</v>
@@ -15788,17 +15605,27 @@
       <c r="D231" s="69"/>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232" s="46" t="s">
+      <c r="A232" s="35" t="s">
+        <v>517</v>
+      </c>
+      <c r="B232" s="42" t="s">
+        <v>204</v>
+      </c>
+      <c r="C232" s="69"/>
+      <c r="D232" s="69"/>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A233" s="46" t="s">
         <v>518</v>
       </c>
-      <c r="B232" s="48" t="s">
-        <v>204</v>
-      </c>
-      <c r="C232" s="70"/>
-      <c r="D232" s="70"/>
+      <c r="B233" s="48" t="s">
+        <v>204</v>
+      </c>
+      <c r="C233" s="70"/>
+      <c r="D233" s="70"/>
     </row>
   </sheetData>
-  <autoFilter ref="A5:C232"/>
+  <autoFilter ref="A5:C233"/>
   <sortState ref="A6:E224">
     <sortCondition ref="A6"/>
   </sortState>
@@ -15806,583 +15633,583 @@
     <mergeCell ref="A1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="B96">
-    <cfRule type="containsText" dxfId="175" priority="326" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="147" priority="326" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="174" priority="327" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="146" priority="327" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="173" priority="328" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="145" priority="328" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B96)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B96">
-    <cfRule type="containsText" dxfId="172" priority="325" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="144" priority="325" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B96)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B40 B43:B45 B77:B91 B6:B14 B55:B61 B63:B74">
-    <cfRule type="containsText" dxfId="171" priority="342" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="143" priority="342" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="170" priority="343" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="142" priority="343" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="169" priority="344" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="141" priority="344" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B40 B43:B45 B77:B91 B6:B14 B55:B61 B63:B74">
-    <cfRule type="containsText" dxfId="168" priority="341" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="140" priority="341" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B93">
-    <cfRule type="containsText" dxfId="167" priority="338" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="139" priority="338" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="166" priority="339" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="138" priority="339" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="165" priority="340" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="137" priority="340" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B93)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B93">
-    <cfRule type="containsText" dxfId="164" priority="337" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="136" priority="337" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B93)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B95">
-    <cfRule type="containsText" dxfId="163" priority="329" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="135" priority="329" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B95)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B94">
-    <cfRule type="containsText" dxfId="162" priority="334" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="134" priority="334" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B94)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="161" priority="335" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="133" priority="335" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B94)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="160" priority="336" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="132" priority="336" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B94)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B94">
-    <cfRule type="containsText" dxfId="159" priority="333" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="131" priority="333" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B94)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B95">
-    <cfRule type="containsText" dxfId="158" priority="330" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="130" priority="330" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B95)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="157" priority="331" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="129" priority="331" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B95)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="156" priority="332" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="128" priority="332" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B95)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B216">
-    <cfRule type="containsText" dxfId="155" priority="313" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B216)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B216">
-    <cfRule type="containsText" dxfId="154" priority="314" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B216)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="153" priority="315" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B216)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="152" priority="316" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B216)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B217">
-    <cfRule type="containsText" dxfId="151" priority="310" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="127" priority="313" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",B217)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B217">
+    <cfRule type="containsText" dxfId="126" priority="314" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B217)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="150" priority="311" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="125" priority="315" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B217)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="149" priority="312" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="124" priority="316" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B217)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B217">
-    <cfRule type="containsText" dxfId="148" priority="309" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B217)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B218">
-    <cfRule type="containsText" dxfId="147" priority="306" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="123" priority="310" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B218)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="146" priority="307" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="122" priority="311" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B218)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="145" priority="308" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="121" priority="312" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B218)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B218">
-    <cfRule type="containsText" dxfId="144" priority="305" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="120" priority="309" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B218)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B219">
-    <cfRule type="containsText" dxfId="143" priority="302" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="119" priority="306" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B219)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="142" priority="303" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="118" priority="307" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B219)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="141" priority="304" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="117" priority="308" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B219)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B219">
-    <cfRule type="containsText" dxfId="140" priority="301" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="116" priority="305" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B219)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B220">
-    <cfRule type="containsText" dxfId="139" priority="298" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="115" priority="302" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B220)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="138" priority="299" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="114" priority="303" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B220)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="137" priority="300" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="113" priority="304" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B220)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B220">
-    <cfRule type="containsText" dxfId="136" priority="297" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="112" priority="301" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B220)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B222">
-    <cfRule type="containsText" dxfId="135" priority="210" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B222)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="134" priority="211" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B222)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="133" priority="212" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B222)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B222">
-    <cfRule type="containsText" dxfId="132" priority="209" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B222)))</formula>
+  <conditionalFormatting sqref="B221">
+    <cfRule type="containsText" dxfId="111" priority="298" stopIfTrue="1" operator="containsText" text="Delete">
+      <formula>NOT(ISERROR(SEARCH("Delete",B221)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="110" priority="299" operator="containsText" text="Change">
+      <formula>NOT(ISERROR(SEARCH("Change",B221)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="109" priority="300" operator="containsText" text="Create">
+      <formula>NOT(ISERROR(SEARCH("Create",B221)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B221">
+    <cfRule type="containsText" dxfId="108" priority="297" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",B221)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B223">
+    <cfRule type="containsText" dxfId="107" priority="210" stopIfTrue="1" operator="containsText" text="Delete">
+      <formula>NOT(ISERROR(SEARCH("Delete",B223)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="106" priority="211" operator="containsText" text="Change">
+      <formula>NOT(ISERROR(SEARCH("Change",B223)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="105" priority="212" operator="containsText" text="Create">
+      <formula>NOT(ISERROR(SEARCH("Create",B223)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B223">
+    <cfRule type="containsText" dxfId="104" priority="209" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",B223)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46:B47">
-    <cfRule type="containsText" dxfId="131" priority="202" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="103" priority="202" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="203" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="102" priority="203" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="204" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="101" priority="204" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46:B47">
-    <cfRule type="containsText" dxfId="128" priority="201" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="100" priority="201" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76">
-    <cfRule type="containsText" dxfId="127" priority="190" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="99" priority="190" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B76)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="191" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="98" priority="191" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B76)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="125" priority="192" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="97" priority="192" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76">
-    <cfRule type="containsText" dxfId="124" priority="189" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="96" priority="189" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75">
-    <cfRule type="containsText" dxfId="123" priority="194" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="95" priority="194" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="122" priority="195" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="94" priority="195" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="196" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="93" priority="196" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75">
-    <cfRule type="containsText" dxfId="120" priority="193" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="92" priority="193" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52:B54">
-    <cfRule type="containsText" dxfId="119" priority="198" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="91" priority="198" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="199" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="90" priority="199" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="200" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="89" priority="200" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52:B54">
-    <cfRule type="containsText" dxfId="116" priority="197" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="88" priority="197" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="containsText" dxfId="115" priority="182" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="87" priority="182" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="183" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="86" priority="183" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="113" priority="184" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="85" priority="184" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="containsText" dxfId="112" priority="181" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="84" priority="181" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="containsText" dxfId="111" priority="178" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="83" priority="178" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="110" priority="179" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="82" priority="179" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="180" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="81" priority="180" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="containsText" dxfId="108" priority="177" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="80" priority="177" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49:B50">
-    <cfRule type="containsText" dxfId="107" priority="174" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="79" priority="174" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="175" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="78" priority="175" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="176" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="77" priority="176" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49:B50">
-    <cfRule type="containsText" dxfId="104" priority="173" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="76" priority="173" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41">
-    <cfRule type="containsText" dxfId="103" priority="170" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="75" priority="170" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="171" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="74" priority="171" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="101" priority="172" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="73" priority="172" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41">
-    <cfRule type="containsText" dxfId="100" priority="169" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="72" priority="169" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="containsText" dxfId="99" priority="166" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="71" priority="166" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B42)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="167" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="70" priority="167" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B42)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="168" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="69" priority="168" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="containsText" dxfId="96" priority="165" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="68" priority="165" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51">
-    <cfRule type="containsText" dxfId="95" priority="162" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="67" priority="162" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="163" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="66" priority="163" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="164" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="65" priority="164" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51">
-    <cfRule type="containsText" dxfId="92" priority="161" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="64" priority="161" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B51)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B224">
-    <cfRule type="containsText" dxfId="91" priority="98" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B224)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="99" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B224)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="100" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B224)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B224">
-    <cfRule type="containsText" dxfId="88" priority="97" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B224)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B230">
-    <cfRule type="containsText" dxfId="87" priority="90" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B230)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="91" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B230)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="92" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B230)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B230">
-    <cfRule type="containsText" dxfId="84" priority="89" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B230)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B225:B226 B229">
-    <cfRule type="containsText" dxfId="83" priority="94" stopIfTrue="1" operator="containsText" text="Delete">
+  <conditionalFormatting sqref="B225">
+    <cfRule type="containsText" dxfId="63" priority="98" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B225)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="95" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="62" priority="99" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B225)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="96" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="61" priority="100" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B225)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B225:B226 B229">
-    <cfRule type="containsText" dxfId="80" priority="93" operator="containsText" text="None">
+  <conditionalFormatting sqref="B225">
+    <cfRule type="containsText" dxfId="60" priority="97" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B225)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B231">
+    <cfRule type="containsText" dxfId="59" priority="90" stopIfTrue="1" operator="containsText" text="Delete">
+      <formula>NOT(ISERROR(SEARCH("Delete",B231)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="58" priority="91" operator="containsText" text="Change">
+      <formula>NOT(ISERROR(SEARCH("Change",B231)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="57" priority="92" operator="containsText" text="Create">
+      <formula>NOT(ISERROR(SEARCH("Create",B231)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B231">
+    <cfRule type="containsText" dxfId="56" priority="89" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",B231)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B226:B227 B230">
+    <cfRule type="containsText" dxfId="55" priority="94" stopIfTrue="1" operator="containsText" text="Delete">
+      <formula>NOT(ISERROR(SEARCH("Delete",B226)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="54" priority="95" operator="containsText" text="Change">
+      <formula>NOT(ISERROR(SEARCH("Change",B226)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="53" priority="96" operator="containsText" text="Create">
+      <formula>NOT(ISERROR(SEARCH("Create",B226)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B226:B227 B230">
+    <cfRule type="containsText" dxfId="52" priority="93" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",B226)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B92">
-    <cfRule type="containsText" dxfId="79" priority="74" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="51" priority="74" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B92)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="75" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="50" priority="75" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B92)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="76" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="49" priority="76" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B92)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B92">
-    <cfRule type="containsText" dxfId="76" priority="73" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="48" priority="73" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B92)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B97:B99 B114:B115 B148:B157 B159:B212 B214:B215 B126:B146 B101:B112 B117:B124">
-    <cfRule type="containsText" dxfId="75" priority="42" stopIfTrue="1" operator="containsText" text="Delete">
+  <conditionalFormatting sqref="B97:B99 B115:B116 B149:B158 B160:B213 B215:B216 B127:B147 B118:B125 B101:B113">
+    <cfRule type="containsText" dxfId="47" priority="42" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B97)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="43" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="46" priority="43" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B97)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="44" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="45" priority="44" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B97)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B97:B99 B114:B115 B148:B157 B159:B212 B214:B215 B126:B146 B101:B112 B117:B124">
-    <cfRule type="containsText" dxfId="72" priority="41" operator="containsText" text="None">
+  <conditionalFormatting sqref="B97:B99 B115:B116 B149:B158 B160:B213 B215:B216 B127:B147 B118:B125 B101:B113">
+    <cfRule type="containsText" dxfId="44" priority="41" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B97)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B147">
-    <cfRule type="containsText" dxfId="71" priority="38" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B147)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="39" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B147)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="40" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B147)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B147">
-    <cfRule type="containsText" dxfId="68" priority="37" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B147)))</formula>
+  <conditionalFormatting sqref="B148">
+    <cfRule type="containsText" dxfId="43" priority="38" stopIfTrue="1" operator="containsText" text="Delete">
+      <formula>NOT(ISERROR(SEARCH("Delete",B148)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="42" priority="39" operator="containsText" text="Change">
+      <formula>NOT(ISERROR(SEARCH("Change",B148)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="41" priority="40" operator="containsText" text="Create">
+      <formula>NOT(ISERROR(SEARCH("Create",B148)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B148">
+    <cfRule type="containsText" dxfId="40" priority="37" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",B148)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62">
-    <cfRule type="containsText" dxfId="67" priority="34" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="39" priority="34" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B62)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="35" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="38" priority="35" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B62)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="36" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="37" priority="36" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62">
-    <cfRule type="containsText" dxfId="64" priority="33" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="36" priority="33" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B62)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B229">
+    <cfRule type="containsText" dxfId="35" priority="30" stopIfTrue="1" operator="containsText" text="Delete">
+      <formula>NOT(ISERROR(SEARCH("Delete",B229)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="31" operator="containsText" text="Change">
+      <formula>NOT(ISERROR(SEARCH("Change",B229)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="32" operator="containsText" text="Create">
+      <formula>NOT(ISERROR(SEARCH("Create",B229)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B229">
+    <cfRule type="containsText" dxfId="32" priority="29" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",B229)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B114">
+    <cfRule type="containsText" dxfId="31" priority="26" stopIfTrue="1" operator="containsText" text="Delete">
+      <formula>NOT(ISERROR(SEARCH("Delete",B114)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="27" operator="containsText" text="Change">
+      <formula>NOT(ISERROR(SEARCH("Change",B114)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="29" priority="28" operator="containsText" text="Create">
+      <formula>NOT(ISERROR(SEARCH("Create",B114)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B114">
+    <cfRule type="containsText" dxfId="28" priority="25" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",B114)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B159">
+    <cfRule type="containsText" dxfId="27" priority="22" stopIfTrue="1" operator="containsText" text="Delete">
+      <formula>NOT(ISERROR(SEARCH("Delete",B159)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="23" operator="containsText" text="Change">
+      <formula>NOT(ISERROR(SEARCH("Change",B159)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="24" operator="containsText" text="Create">
+      <formula>NOT(ISERROR(SEARCH("Create",B159)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B159">
+    <cfRule type="containsText" dxfId="24" priority="21" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",B159)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B214">
+    <cfRule type="containsText" dxfId="23" priority="18" stopIfTrue="1" operator="containsText" text="Delete">
+      <formula>NOT(ISERROR(SEARCH("Delete",B214)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="19" operator="containsText" text="Change">
+      <formula>NOT(ISERROR(SEARCH("Change",B214)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="20" operator="containsText" text="Create">
+      <formula>NOT(ISERROR(SEARCH("Create",B214)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B214">
+    <cfRule type="containsText" dxfId="20" priority="17" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",B214)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B126">
+    <cfRule type="containsText" dxfId="19" priority="14" stopIfTrue="1" operator="containsText" text="Delete">
+      <formula>NOT(ISERROR(SEARCH("Delete",B126)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="15" operator="containsText" text="Change">
+      <formula>NOT(ISERROR(SEARCH("Change",B126)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="Create">
+      <formula>NOT(ISERROR(SEARCH("Create",B126)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B126">
+    <cfRule type="containsText" dxfId="16" priority="13" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",B126)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B228">
-    <cfRule type="containsText" dxfId="63" priority="30" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="15" priority="10" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B228)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="31" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="14" priority="11" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B228)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="32" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="13" priority="12" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B228)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B228">
-    <cfRule type="containsText" dxfId="60" priority="29" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B228)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B113">
-    <cfRule type="containsText" dxfId="59" priority="26" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B113)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="27" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B113)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="28" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B113)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B113">
-    <cfRule type="containsText" dxfId="56" priority="25" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B113)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B158">
-    <cfRule type="containsText" dxfId="55" priority="22" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B158)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="23" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B158)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="24" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B158)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B158">
-    <cfRule type="containsText" dxfId="52" priority="21" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B158)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B213">
-    <cfRule type="containsText" dxfId="51" priority="18" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B213)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="19" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B213)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="20" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B213)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B213">
-    <cfRule type="containsText" dxfId="48" priority="17" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B213)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B125">
-    <cfRule type="containsText" dxfId="47" priority="14" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B125)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="15" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B125)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="16" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B125)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B125">
-    <cfRule type="containsText" dxfId="44" priority="13" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B125)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B227">
-    <cfRule type="containsText" dxfId="43" priority="10" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B227)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="11" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B227)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="12" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B227)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B227">
-    <cfRule type="containsText" dxfId="40" priority="9" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B227)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B100">
-    <cfRule type="containsText" dxfId="36" priority="5" operator="containsText" text="None">
+    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B100)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B100">
-    <cfRule type="containsText" dxfId="35" priority="6" stopIfTrue="1" operator="containsText" text="Delete">
+    <cfRule type="containsText" dxfId="10" priority="6" stopIfTrue="1" operator="containsText" text="Delete">
       <formula>NOT(ISERROR(SEARCH("Delete",B100)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="7" operator="containsText" text="Change">
+    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="Change">
       <formula>NOT(ISERROR(SEARCH("Change",B100)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="8" operator="containsText" text="Create">
+    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="Create">
       <formula>NOT(ISERROR(SEARCH("Create",B100)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B116">
-    <cfRule type="containsText" dxfId="31" priority="2" stopIfTrue="1" operator="containsText" text="Delete">
-      <formula>NOT(ISERROR(SEARCH("Delete",B116)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="3" operator="containsText" text="Change">
-      <formula>NOT(ISERROR(SEARCH("Change",B116)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="4" operator="containsText" text="Create">
-      <formula>NOT(ISERROR(SEARCH("Create",B116)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B116">
-    <cfRule type="containsText" dxfId="25" priority="1" operator="containsText" text="None">
-      <formula>NOT(ISERROR(SEARCH("None",B116)))</formula>
+  <conditionalFormatting sqref="B117">
+    <cfRule type="containsText" dxfId="7" priority="2" stopIfTrue="1" operator="containsText" text="Delete">
+      <formula>NOT(ISERROR(SEARCH("Delete",B117)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Change">
+      <formula>NOT(ISERROR(SEARCH("Change",B117)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Create">
+      <formula>NOT(ISERROR(SEARCH("Create",B117)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B117">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="None">
+      <formula>NOT(ISERROR(SEARCH("None",B117)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B222 B224:B230 B6:B220">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B223 B225:B231 B6:B221">
       <formula1>$G$6:$G$9</formula1>
     </dataValidation>
   </dataValidations>
@@ -16393,10 +16220,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A53:E106"/>
+  <dimension ref="A53:E107"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C107" sqref="C107:E107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17034,6 +16861,17 @@
       <c r="C106" s="7"/>
       <c r="D106" s="4"/>
       <c r="E106" s="7"/>
+    </row>
+    <row r="107" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A107" s="15" t="s">
+        <v>649</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="C107" s="7"/>
+      <c r="D107" s="4"/>
+      <c r="E107" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>